<commit_message>
Improvements in weapon configuration
1. Torpedoes have their own warheads, which are loaded from the warhead
file.
2. There are 3 types of torpedoes: heavy long-range, and tracking. Each
can have its own warhead.
3. Additional properties which are loaded from the configuration files:
3.1. The size of the projectile (which now also scales the trail)
3.2. The system hit multiplicity (not yet used in the code)
3.3. For torpedoes: spread size and range
4. Imported a nicer sprite for ship engines.
5. Imported the model the Terran Navarino (Navarin) class
demi-battleship.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="35">
   <si>
     <t>#</t>
   </si>
@@ -51,15 +51,6 @@
     <t>HT</t>
   </si>
   <si>
-    <t>Sx</t>
-  </si>
-  <si>
-    <t>Sy</t>
-  </si>
-  <si>
-    <t>Sz</t>
-  </si>
-  <si>
     <t>Light</t>
   </si>
   <si>
@@ -109,6 +100,30 @@
   </si>
   <si>
     <t>Interval</t>
+  </si>
+  <si>
+    <t>Weapon effect size</t>
+  </si>
+  <si>
+    <t>Projectile Size</t>
+  </si>
+  <si>
+    <t>Tracking</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Systems hit</t>
+  </si>
+  <si>
+    <t>Spread Size</t>
+  </si>
+  <si>
+    <t>Torpedo Type</t>
+  </si>
+  <si>
+    <t>LongRange</t>
   </si>
 </sst>
 </file>
@@ -915,23 +930,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S53"/>
+  <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -942,7 +961,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -966,42 +985,39 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
       </c>
       <c r="D2">
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -1022,46 +1038,43 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="M2">
         <v>0.2</v>
       </c>
-      <c r="N2">
-        <v>0.2</v>
-      </c>
-      <c r="P2">
+      <c r="O2">
         <f>F2/D2</f>
         <v>20</v>
       </c>
-      <c r="Q2">
+      <c r="P2">
         <f>H2/D2</f>
         <v>6</v>
       </c>
-      <c r="R2">
+      <c r="Q2">
         <f>I2/D2</f>
         <v>16</v>
       </c>
-      <c r="S2">
+      <c r="R2">
         <f>J2/D2</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>0.5</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>15</v>
@@ -1082,46 +1095,43 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>0.2</v>
       </c>
-      <c r="N3">
-        <v>0.2</v>
+      <c r="O3">
+        <f>F3/D3</f>
+        <v>30</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P4" si="0">F3/D3</f>
-        <v>30</v>
+        <f>H3/D3</f>
+        <v>10</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q4" si="1">H3/D3</f>
+        <f>I3/D3</f>
+        <v>14</v>
+      </c>
+      <c r="R3">
+        <f>J3/D3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R4" si="2">I3/D3</f>
-        <v>14</v>
-      </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S4" si="3">J3/D3</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>0.5</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>20</v>
@@ -1142,46 +1152,43 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <v>0.3</v>
       </c>
-      <c r="N4">
-        <v>0.3</v>
+      <c r="O4">
+        <f>F4/D4</f>
+        <v>40</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>H4/D4</f>
+        <v>6</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>I4/D4</f>
+        <v>16</v>
       </c>
       <c r="R4">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="S4">
-        <f t="shared" si="3"/>
+        <f>J4/D4</f>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>60</v>
@@ -1202,46 +1209,43 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M6">
         <v>0.3</v>
       </c>
-      <c r="N6">
-        <v>0.3</v>
-      </c>
-      <c r="P6">
+      <c r="O6">
         <f>F6/D6</f>
         <v>30</v>
       </c>
-      <c r="Q6">
+      <c r="P6">
         <f>H6/D6</f>
         <v>4</v>
       </c>
-      <c r="R6">
+      <c r="Q6">
         <f>I6/D6</f>
         <v>20</v>
       </c>
-      <c r="S6">
+      <c r="R6">
         <f>J6/D6</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F7">
         <v>80</v>
@@ -1262,46 +1266,43 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>0.3</v>
       </c>
-      <c r="N7">
-        <v>0.3</v>
+      <c r="O7">
+        <f>F7/D7</f>
+        <v>40</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7:P8" si="4">F7/D7</f>
-        <v>40</v>
+        <f>H7/D7</f>
+        <v>6</v>
       </c>
       <c r="Q7">
-        <f t="shared" ref="Q7:Q8" si="5">H7/D7</f>
-        <v>6</v>
+        <f>I7/D7</f>
+        <v>14</v>
       </c>
       <c r="R7">
-        <f t="shared" ref="R7:R8" si="6">I7/D7</f>
-        <v>14</v>
-      </c>
-      <c r="S7">
-        <f t="shared" ref="S7:S8" si="7">J7/D7</f>
+        <f>J7/D7</f>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F8">
         <v>90</v>
@@ -1322,46 +1323,43 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>0.35</v>
       </c>
-      <c r="N8">
-        <v>0.35</v>
+      <c r="O8">
+        <f>F8/D8</f>
+        <v>45</v>
       </c>
       <c r="P8">
-        <f t="shared" si="4"/>
-        <v>45</v>
+        <f>H8/D8</f>
+        <v>3</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f>I8/D8</f>
+        <v>15</v>
       </c>
       <c r="R8">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <f>J8/D8</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>50</v>
@@ -1382,46 +1380,43 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <v>0.3</v>
       </c>
-      <c r="N10">
-        <v>0.3</v>
-      </c>
-      <c r="P10">
+      <c r="O10">
         <f>F10/D10</f>
         <v>25</v>
       </c>
+      <c r="P10">
+        <f>H10/D10</f>
+        <v>3</v>
+      </c>
       <c r="Q10">
-        <f>H10/D10</f>
-        <v>3</v>
-      </c>
-      <c r="R10">
         <f>I10/D10</f>
         <v>18</v>
       </c>
-      <c r="S10">
+      <c r="R10">
         <f>J10/D10</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F11">
         <v>100</v>
@@ -1442,46 +1437,43 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M11">
         <v>0.35</v>
       </c>
-      <c r="N11">
-        <v>0.35</v>
+      <c r="O11">
+        <f>F11/D11</f>
+        <v>50</v>
       </c>
       <c r="P11">
-        <f t="shared" ref="P11:P12" si="8">F11/D11</f>
-        <v>50</v>
+        <f>H11/D11</f>
+        <v>8</v>
       </c>
       <c r="Q11">
-        <f t="shared" ref="Q11:Q12" si="9">H11/D11</f>
-        <v>8</v>
+        <f>I11/D11</f>
+        <v>17</v>
       </c>
       <c r="R11">
-        <f t="shared" ref="R11:R12" si="10">I11/D11</f>
-        <v>17</v>
-      </c>
-      <c r="S11">
-        <f t="shared" ref="S11:S12" si="11">J11/D11</f>
+        <f>J11/D11</f>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F12">
         <v>120</v>
@@ -1502,32 +1494,29 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M12">
         <v>0.35</v>
       </c>
-      <c r="N12">
-        <v>0.35</v>
+      <c r="O12">
+        <f>F12/D12</f>
+        <v>60</v>
       </c>
       <c r="P12">
-        <f t="shared" si="8"/>
-        <v>60</v>
+        <f>H12/D12</f>
+        <v>3</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="9"/>
-        <v>3</v>
+        <f>I12/D12</f>
+        <v>17.5</v>
       </c>
       <c r="R12">
-        <f t="shared" si="10"/>
-        <v>17.5</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="11"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+        <f>J12/D12</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1556,24 +1545,21 @@
         <v>9</v>
       </c>
       <c r="K14" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="L14" t="s">
-        <v>11</v>
-      </c>
-      <c r="M14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E15">
         <v>45</v>
@@ -1594,24 +1580,21 @@
         <v>8</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -1632,24 +1615,21 @@
         <v>10</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>75</v>
@@ -1670,16 +1650,13 @@
         <v>12</v>
       </c>
       <c r="K17">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="L17">
         <v>0.1</v>
       </c>
-      <c r="M17">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1711,592 +1688,562 @@
         <v>9</v>
       </c>
       <c r="L19" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="M19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
         <v>11</v>
-      </c>
-      <c r="N19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
       </c>
       <c r="D20">
         <v>0.75</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F20">
-        <f>2*P2*D20</f>
+        <f>2*O2*D20</f>
         <v>30</v>
       </c>
       <c r="G20">
         <v>250</v>
       </c>
       <c r="H20">
+        <f>2*P2*D20</f>
+        <v>9</v>
+      </c>
+      <c r="I20">
         <f>2*Q2*D20</f>
-        <v>9</v>
-      </c>
-      <c r="I20">
+        <v>24</v>
+      </c>
+      <c r="J20">
         <f>2*R2*D20</f>
-        <v>24</v>
-      </c>
-      <c r="J20">
-        <f>2*S2*D20</f>
         <v>6</v>
       </c>
       <c r="K20">
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M20">
         <v>0.3</v>
       </c>
-      <c r="N20">
-        <v>0.3</v>
-      </c>
-      <c r="P20">
+      <c r="O20">
         <f>F20/D20</f>
         <v>40</v>
       </c>
-      <c r="Q20">
+      <c r="P20">
         <f>H20/D20</f>
         <v>12</v>
       </c>
-      <c r="R20">
+      <c r="Q20">
         <f>I20/D20</f>
         <v>32</v>
       </c>
-      <c r="S20">
+      <c r="R20">
         <f>J20/D20</f>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D21">
         <v>0.75</v>
       </c>
       <c r="E21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F21">
-        <f t="shared" ref="F21:F22" si="12">2*P3*D21</f>
+        <f>2*O3*D21</f>
         <v>45</v>
       </c>
       <c r="G21">
         <v>170</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:H22" si="13">2*Q3*D21</f>
+        <f>2*P3*D21</f>
         <v>15</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I22" si="14">2*R3*D21</f>
+        <f>2*Q3*D21</f>
         <v>21</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21:J22" si="15">2*S3*D21</f>
+        <f>2*R3*D21</f>
         <v>9</v>
       </c>
       <c r="K21">
         <v>0</v>
       </c>
       <c r="L21">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M21">
         <v>0.3</v>
       </c>
-      <c r="N21">
-        <v>0.3</v>
+      <c r="O21">
+        <f>F21/D21</f>
+        <v>60</v>
       </c>
       <c r="P21">
-        <f t="shared" ref="P21:P22" si="16">F21/D21</f>
-        <v>60</v>
+        <f>H21/D21</f>
+        <v>20</v>
       </c>
       <c r="Q21">
-        <f t="shared" ref="Q21:Q22" si="17">H21/D21</f>
+        <f>I21/D21</f>
+        <v>28</v>
+      </c>
+      <c r="R21">
+        <f>J21/D21</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
         <v>20</v>
       </c>
-      <c r="R21">
-        <f t="shared" ref="R21:R22" si="18">I21/D21</f>
-        <v>28</v>
-      </c>
-      <c r="S21">
-        <f t="shared" ref="S21:S22" si="19">J21/D21</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D22">
         <v>0.75</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F22">
-        <f t="shared" si="12"/>
+        <f>2*O4*D22</f>
         <v>60</v>
       </c>
       <c r="G22">
         <v>120</v>
       </c>
       <c r="H22">
-        <f t="shared" si="13"/>
+        <f>2*P4*D22</f>
         <v>9</v>
       </c>
       <c r="I22">
-        <f t="shared" si="14"/>
+        <f>2*Q4*D22</f>
         <v>24</v>
       </c>
       <c r="J22">
-        <f t="shared" si="15"/>
+        <f>2*R4*D22</f>
         <v>3</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
       <c r="L22">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M22">
         <v>0.35</v>
       </c>
-      <c r="N22">
-        <v>0.35</v>
+      <c r="O22">
+        <f>F22/D22</f>
+        <v>80</v>
       </c>
       <c r="P22">
-        <f t="shared" si="16"/>
-        <v>80</v>
+        <f>H22/D22</f>
+        <v>12</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="17"/>
-        <v>12</v>
+        <f>I22/D22</f>
+        <v>32</v>
       </c>
       <c r="R22">
-        <f t="shared" si="18"/>
-        <v>32</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="19"/>
+        <f>J22/D22</f>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F24">
-        <f>2*P6*D24</f>
+        <f>2*O6*D24</f>
         <v>240</v>
       </c>
       <c r="G24">
         <v>750</v>
       </c>
       <c r="H24">
+        <f>2*P6*D24</f>
+        <v>32</v>
+      </c>
+      <c r="I24">
         <f>2*Q6*D24</f>
+        <v>160</v>
+      </c>
+      <c r="J24">
+        <f>2*R6*D24</f>
         <v>32</v>
       </c>
-      <c r="I24">
-        <f>2*R6*D24</f>
-        <v>160</v>
-      </c>
-      <c r="J24">
-        <f>2*S6*D24</f>
-        <v>32</v>
-      </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M24">
         <v>0.35</v>
       </c>
-      <c r="N24">
-        <v>0.35</v>
-      </c>
-      <c r="P24">
+      <c r="O24">
         <f>F24/D24</f>
         <v>60</v>
       </c>
-      <c r="Q24">
+      <c r="P24">
         <f>H24/D24</f>
         <v>8</v>
       </c>
-      <c r="R24">
+      <c r="Q24">
         <f>I24/D24</f>
         <v>40</v>
       </c>
-      <c r="S24">
+      <c r="R24">
         <f>J24/D24</f>
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25:F26" si="20">2*P7*D25</f>
+        <f>2*O7*D25</f>
         <v>320</v>
       </c>
       <c r="G25">
         <v>500</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25:H26" si="21">2*Q7*D25</f>
+        <f>2*P7*D25</f>
         <v>48</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I26" si="22">2*R7*D25</f>
+        <f>2*Q7*D25</f>
         <v>112</v>
       </c>
       <c r="J25">
-        <f t="shared" ref="J25:J26" si="23">2*S7*D25</f>
+        <f>2*R7*D25</f>
         <v>40</v>
       </c>
       <c r="K25">
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M25">
         <v>0.35</v>
       </c>
-      <c r="N25">
-        <v>0.35</v>
+      <c r="O25">
+        <f>F25/D25</f>
+        <v>80</v>
       </c>
       <c r="P25">
-        <f t="shared" ref="P25:P26" si="24">F25/D25</f>
-        <v>80</v>
+        <f>H25/D25</f>
+        <v>12</v>
       </c>
       <c r="Q25">
-        <f t="shared" ref="Q25:Q26" si="25">H25/D25</f>
-        <v>12</v>
+        <f>I25/D25</f>
+        <v>28</v>
       </c>
       <c r="R25">
-        <f t="shared" ref="R25:R26" si="26">I25/D25</f>
-        <v>28</v>
-      </c>
-      <c r="S25">
-        <f t="shared" ref="S25:S26" si="27">J25/D25</f>
+        <f>J25/D25</f>
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F26">
-        <f t="shared" si="20"/>
+        <f>2*O8*D26</f>
         <v>360</v>
       </c>
       <c r="G26">
         <v>150</v>
       </c>
       <c r="H26">
-        <f t="shared" si="21"/>
+        <f>2*P8*D26</f>
         <v>24</v>
       </c>
       <c r="I26">
-        <f t="shared" si="22"/>
+        <f>2*Q8*D26</f>
         <v>120</v>
       </c>
       <c r="J26">
-        <f t="shared" si="23"/>
+        <f>2*R8*D26</f>
         <v>24</v>
       </c>
       <c r="K26">
         <v>0</v>
       </c>
       <c r="L26">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="M26">
         <v>0.4</v>
       </c>
-      <c r="N26">
-        <v>0.4</v>
+      <c r="O26">
+        <f>F26/D26</f>
+        <v>90</v>
       </c>
       <c r="P26">
-        <f t="shared" si="24"/>
-        <v>90</v>
+        <f>H26/D26</f>
+        <v>6</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="25"/>
+        <f>I26/D26</f>
+        <v>30</v>
+      </c>
+      <c r="R26">
+        <f>J26/D26</f>
         <v>6</v>
       </c>
-      <c r="R26">
-        <f t="shared" si="26"/>
-        <v>30</v>
-      </c>
-      <c r="S26">
-        <f t="shared" si="27"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D28">
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F28">
-        <f>2*P10*D28</f>
+        <f>2*O10*D28</f>
         <v>200</v>
       </c>
       <c r="G28">
         <v>580</v>
       </c>
       <c r="H28">
+        <f>2*P10*D28</f>
+        <v>24</v>
+      </c>
+      <c r="I28">
         <f>2*Q10*D28</f>
+        <v>144</v>
+      </c>
+      <c r="J28">
+        <f>2*R10*D28</f>
         <v>24</v>
       </c>
-      <c r="I28">
-        <f>2*R10*D28</f>
-        <v>144</v>
-      </c>
-      <c r="J28">
-        <f>2*S10*D28</f>
-        <v>24</v>
-      </c>
       <c r="K28">
         <v>0</v>
       </c>
       <c r="L28">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M28">
         <v>0.35</v>
       </c>
-      <c r="N28">
-        <v>0.35</v>
-      </c>
-      <c r="P28">
+      <c r="O28">
         <f>F28/D28</f>
         <v>50</v>
       </c>
-      <c r="Q28">
+      <c r="P28">
         <f>H28/D28</f>
         <v>6</v>
       </c>
-      <c r="R28">
+      <c r="Q28">
         <f>I28/D28</f>
         <v>36</v>
       </c>
-      <c r="S28">
+      <c r="R28">
         <f>J28/D28</f>
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:F30" si="28">2*P11*D29</f>
+        <f>2*O11*D29</f>
         <v>400</v>
       </c>
       <c r="G29">
-        <v>550</v>
+        <v>570</v>
       </c>
       <c r="H29">
-        <f t="shared" ref="H29:H30" si="29">2*Q11*D29</f>
+        <f>2*P11*D29</f>
         <v>64</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="I29:I30" si="30">2*R11*D29</f>
+        <f>2*Q11*D29</f>
         <v>136</v>
       </c>
       <c r="J29">
-        <f t="shared" ref="J29:J30" si="31">2*S11*D29</f>
+        <f>2*R11*D29</f>
         <v>56</v>
       </c>
       <c r="K29">
         <v>0</v>
       </c>
       <c r="L29">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="M29">
         <v>0.45</v>
       </c>
-      <c r="N29">
-        <v>0.45</v>
+      <c r="O29">
+        <f>F29/D29</f>
+        <v>100</v>
       </c>
       <c r="P29">
-        <f t="shared" ref="P29:P30" si="32">F29/D29</f>
-        <v>100</v>
+        <f>H29/D29</f>
+        <v>16</v>
       </c>
       <c r="Q29">
-        <f t="shared" ref="Q29:Q30" si="33">H29/D29</f>
+        <f>I29/D29</f>
+        <v>34</v>
+      </c>
+      <c r="R29">
+        <f>J29/D29</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s">
         <v>16</v>
-      </c>
-      <c r="R29">
-        <f t="shared" ref="R29:R30" si="34">I29/D29</f>
-        <v>34</v>
-      </c>
-      <c r="S29">
-        <f t="shared" ref="S29:S30" si="35">J29/D29</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" t="s">
-        <v>19</v>
       </c>
       <c r="D30">
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F30">
-        <f t="shared" si="28"/>
+        <f>2*O12*D30</f>
         <v>480</v>
       </c>
       <c r="G30">
         <v>160</v>
       </c>
       <c r="H30">
-        <f t="shared" si="29"/>
+        <f>2*P12*D30</f>
         <v>24</v>
       </c>
       <c r="I30">
-        <f t="shared" si="30"/>
+        <f>2*Q12*D30</f>
         <v>140</v>
       </c>
       <c r="J30">
-        <f t="shared" si="31"/>
+        <f>2*R12*D30</f>
         <v>24</v>
       </c>
       <c r="K30">
         <v>0</v>
       </c>
       <c r="L30">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="M30">
         <v>0.45</v>
       </c>
-      <c r="N30">
-        <v>0.45</v>
+      <c r="O30">
+        <f>F30/D30</f>
+        <v>120</v>
       </c>
       <c r="P30">
-        <f t="shared" si="32"/>
-        <v>120</v>
+        <f>H30/D30</f>
+        <v>6</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="33"/>
+        <f>I30/D30</f>
+        <v>35</v>
+      </c>
+      <c r="R30">
+        <f>J30/D30</f>
         <v>6</v>
       </c>
-      <c r="R30">
-        <f t="shared" si="34"/>
-        <v>35</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="35"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2325,24 +2272,21 @@
         <v>9</v>
       </c>
       <c r="K32" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="L32" t="s">
-        <v>11</v>
-      </c>
-      <c r="M32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E33">
         <v>100</v>
@@ -2363,24 +2307,21 @@
         <v>8</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L33">
         <v>0</v>
       </c>
-      <c r="M33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E34">
         <v>250</v>
@@ -2401,24 +2342,21 @@
         <v>10</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L34">
         <v>0</v>
       </c>
-      <c r="M34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E35">
         <v>170</v>
@@ -2439,16 +2377,13 @@
         <v>12</v>
       </c>
       <c r="K35">
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="L35">
         <v>0.125</v>
       </c>
-      <c r="M35">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2480,592 +2415,562 @@
         <v>9</v>
       </c>
       <c r="L37" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="M37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" t="s">
         <v>11</v>
       </c>
-      <c r="N37" t="s">
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>3</v>
-      </c>
-      <c r="B38" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>15</v>
-      </c>
       <c r="F38">
-        <f>2.5*P20*D38</f>
+        <f>2.5*O20*D38</f>
         <v>100</v>
       </c>
       <c r="G38">
         <v>310</v>
       </c>
       <c r="H38">
+        <f>2.5*P20*D38</f>
+        <v>30</v>
+      </c>
+      <c r="I38">
         <f>2.5*Q20*D38</f>
-        <v>30</v>
-      </c>
-      <c r="I38">
+        <v>80</v>
+      </c>
+      <c r="J38">
         <f>2.5*R20*D38</f>
-        <v>80</v>
-      </c>
-      <c r="J38">
-        <f>2.5*S20*D38</f>
         <v>20</v>
       </c>
       <c r="K38">
         <v>0</v>
       </c>
       <c r="L38">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M38">
         <v>0.3</v>
       </c>
-      <c r="N38">
-        <v>0.3</v>
-      </c>
-      <c r="P38">
+      <c r="O38">
         <f>F38/D38</f>
         <v>100</v>
       </c>
-      <c r="Q38">
+      <c r="P38">
         <f>H38/D38</f>
         <v>30</v>
       </c>
-      <c r="R38">
+      <c r="Q38">
         <f>I38/D38</f>
         <v>80</v>
       </c>
-      <c r="S38">
+      <c r="R38">
         <f>J38/D38</f>
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F39">
-        <f t="shared" ref="F39:F40" si="36">2.5*P21*D39</f>
+        <f>2.5*O21*D39</f>
         <v>150</v>
       </c>
       <c r="G39">
         <v>270</v>
       </c>
       <c r="H39">
-        <f t="shared" ref="H39:H40" si="37">2.5*Q21*D39</f>
+        <f>2.5*P21*D39</f>
         <v>50</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:I40" si="38">2.5*R21*D39</f>
+        <f>2.5*Q21*D39</f>
         <v>70</v>
       </c>
       <c r="J39">
-        <f t="shared" ref="J39:J40" si="39">2.5*S21*D39</f>
+        <f>2.5*R21*D39</f>
         <v>30</v>
       </c>
       <c r="K39">
         <v>0</v>
       </c>
       <c r="L39">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="M39">
         <v>0.3</v>
       </c>
-      <c r="N39">
-        <v>0.3</v>
+      <c r="O39">
+        <f>F39/D39</f>
+        <v>150</v>
       </c>
       <c r="P39">
-        <f t="shared" ref="P39:P40" si="40">F39/D39</f>
-        <v>150</v>
+        <f>H39/D39</f>
+        <v>50</v>
       </c>
       <c r="Q39">
-        <f t="shared" ref="Q39:Q40" si="41">H39/D39</f>
-        <v>50</v>
+        <f>I39/D39</f>
+        <v>70</v>
       </c>
       <c r="R39">
-        <f t="shared" ref="R39:R40" si="42">I39/D39</f>
-        <v>70</v>
-      </c>
-      <c r="S39">
-        <f t="shared" ref="S39:S40" si="43">J39/D39</f>
+        <f>J39/D39</f>
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
         <v>14</v>
       </c>
-      <c r="D40">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>17</v>
-      </c>
       <c r="F40">
-        <f t="shared" si="36"/>
+        <f>2.5*O22*D40</f>
         <v>200</v>
       </c>
       <c r="G40">
         <v>180</v>
       </c>
       <c r="H40">
-        <f t="shared" si="37"/>
+        <f>2.5*P22*D40</f>
         <v>30</v>
       </c>
       <c r="I40">
-        <f t="shared" si="38"/>
+        <f>2.5*Q22*D40</f>
         <v>80</v>
       </c>
       <c r="J40">
-        <f t="shared" si="39"/>
+        <f>2.5*R22*D40</f>
         <v>10</v>
       </c>
       <c r="K40">
         <v>0</v>
       </c>
       <c r="L40">
-        <v>0.35</v>
+        <v>1</v>
       </c>
       <c r="M40">
         <v>0.35</v>
       </c>
-      <c r="N40">
-        <v>0.35</v>
+      <c r="O40">
+        <f>F40/D40</f>
+        <v>200</v>
       </c>
       <c r="P40">
-        <f t="shared" si="40"/>
-        <v>200</v>
+        <f>H40/D40</f>
+        <v>30</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="41"/>
-        <v>30</v>
+        <f>I40/D40</f>
+        <v>80</v>
       </c>
       <c r="R40">
-        <f t="shared" si="42"/>
-        <v>80</v>
-      </c>
-      <c r="S40">
-        <f t="shared" si="43"/>
+        <f>J40/D40</f>
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D42">
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F42">
-        <f>2.5*P24*D42</f>
+        <f>2.5*O24*D42</f>
         <v>1200</v>
       </c>
       <c r="G42">
         <v>1000</v>
       </c>
       <c r="H42">
+        <f>2.5*P24*D42</f>
+        <v>160</v>
+      </c>
+      <c r="I42">
         <f>2.5*Q24*D42</f>
+        <v>800</v>
+      </c>
+      <c r="J42">
+        <f>2.5*R24*D42</f>
         <v>160</v>
       </c>
-      <c r="I42">
-        <f>2.5*R24*D42</f>
-        <v>800</v>
-      </c>
-      <c r="J42">
-        <f>2.5*S24*D42</f>
-        <v>160</v>
-      </c>
       <c r="K42">
         <v>0</v>
       </c>
       <c r="L42">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="M42">
         <v>0.4</v>
       </c>
-      <c r="N42">
-        <v>0.4</v>
-      </c>
-      <c r="P42">
+      <c r="O42">
         <f>F42/D42</f>
         <v>150</v>
       </c>
-      <c r="Q42">
+      <c r="P42">
         <f>H42/D42</f>
         <v>20</v>
       </c>
-      <c r="R42">
+      <c r="Q42">
         <f>I42/D42</f>
         <v>100</v>
       </c>
-      <c r="S42">
+      <c r="R42">
         <f>J42/D42</f>
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D43">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F43">
-        <f t="shared" ref="F43:F44" si="44">2.5*P25*D43</f>
+        <f>2.5*O25*D43</f>
         <v>1600</v>
       </c>
       <c r="G43">
         <v>650</v>
       </c>
       <c r="H43">
-        <f t="shared" ref="H43:H44" si="45">2.5*Q25*D43</f>
+        <f>2.5*P25*D43</f>
         <v>240</v>
       </c>
       <c r="I43">
-        <f t="shared" ref="I43:I44" si="46">2.5*R25*D43</f>
+        <f>2.5*Q25*D43</f>
         <v>560</v>
       </c>
       <c r="J43">
-        <f t="shared" ref="J43:J44" si="47">2.5*S25*D43</f>
+        <f>2.5*R25*D43</f>
         <v>200</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>0.45</v>
+        <v>1</v>
       </c>
       <c r="M43">
         <v>0.45</v>
       </c>
-      <c r="N43">
-        <v>0.45</v>
+      <c r="O43">
+        <f>F43/D43</f>
+        <v>200</v>
       </c>
       <c r="P43">
-        <f t="shared" ref="P43:P44" si="48">F43/D43</f>
-        <v>200</v>
+        <f>H43/D43</f>
+        <v>30</v>
       </c>
       <c r="Q43">
-        <f t="shared" ref="Q43:Q44" si="49">H43/D43</f>
-        <v>30</v>
+        <f>I43/D43</f>
+        <v>70</v>
       </c>
       <c r="R43">
-        <f t="shared" ref="R43:R44" si="50">I43/D43</f>
-        <v>70</v>
-      </c>
-      <c r="S43">
-        <f t="shared" ref="S43:S44" si="51">J43/D43</f>
+        <f>J43/D43</f>
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D44">
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F44">
-        <f t="shared" si="44"/>
+        <f>2.5*O26*D44</f>
         <v>1800</v>
       </c>
       <c r="G44">
         <v>180</v>
       </c>
       <c r="H44">
-        <f t="shared" si="45"/>
+        <f>2.5*P26*D44</f>
         <v>120</v>
       </c>
       <c r="I44">
-        <f t="shared" si="46"/>
+        <f>2.5*Q26*D44</f>
         <v>600</v>
       </c>
       <c r="J44">
-        <f t="shared" si="47"/>
+        <f>2.5*R26*D44</f>
         <v>120</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
       <c r="L44">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M44">
         <v>0.5</v>
       </c>
-      <c r="N44">
-        <v>0.5</v>
+      <c r="O44">
+        <f>F44/D44</f>
+        <v>225</v>
       </c>
       <c r="P44">
-        <f t="shared" si="48"/>
-        <v>225</v>
+        <f>H44/D44</f>
+        <v>15</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="49"/>
+        <f>I44/D44</f>
+        <v>75</v>
+      </c>
+      <c r="R44">
+        <f>J44/D44</f>
         <v>15</v>
       </c>
-      <c r="R44">
-        <f t="shared" si="50"/>
-        <v>75</v>
-      </c>
-      <c r="S44">
-        <f t="shared" si="51"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D46">
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F46">
-        <f>2.5*P28*D46</f>
+        <f>2.5*O28*D46</f>
         <v>1000</v>
       </c>
       <c r="G46">
         <v>650</v>
       </c>
       <c r="H46">
+        <f>2.5*P28*D46</f>
+        <v>120</v>
+      </c>
+      <c r="I46">
         <f>2.5*Q28*D46</f>
+        <v>720</v>
+      </c>
+      <c r="J46">
+        <f>2.5*R28*D46</f>
         <v>120</v>
       </c>
-      <c r="I46">
-        <f>2.5*R28*D46</f>
-        <v>720</v>
-      </c>
-      <c r="J46">
-        <f>2.5*S28*D46</f>
-        <v>120</v>
-      </c>
       <c r="K46">
         <v>0</v>
       </c>
       <c r="L46">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="M46">
         <v>0.4</v>
       </c>
-      <c r="N46">
-        <v>0.4</v>
-      </c>
-      <c r="P46">
+      <c r="O46">
         <f>F46/D46</f>
         <v>125</v>
       </c>
-      <c r="Q46">
+      <c r="P46">
         <f>H46/D46</f>
         <v>15</v>
       </c>
-      <c r="R46">
+      <c r="Q46">
         <f>I46/D46</f>
         <v>90</v>
       </c>
-      <c r="S46">
+      <c r="R46">
         <f>J46/D46</f>
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D47">
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F47">
-        <f t="shared" ref="F47:F48" si="52">2.5*P29*D47</f>
+        <f>2.5*O29*D47</f>
         <v>2000</v>
       </c>
       <c r="G47">
-        <v>640</v>
+        <v>680</v>
       </c>
       <c r="H47">
-        <f t="shared" ref="H47:H48" si="53">2.5*Q29*D47</f>
+        <f>2.5*P29*D47</f>
         <v>320</v>
       </c>
       <c r="I47">
-        <f t="shared" ref="I47:I48" si="54">2.5*R29*D47</f>
+        <f>2.5*Q29*D47</f>
         <v>680</v>
       </c>
       <c r="J47">
-        <f t="shared" ref="J47:J48" si="55">2.5*S29*D47</f>
+        <f>2.5*R29*D47</f>
         <v>280</v>
       </c>
       <c r="K47">
         <v>0</v>
       </c>
       <c r="L47">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="M47">
         <v>0.5</v>
       </c>
-      <c r="N47">
-        <v>0.5</v>
+      <c r="O47">
+        <f t="shared" ref="O47:O48" si="0">F47/D47</f>
+        <v>250</v>
       </c>
       <c r="P47">
-        <f t="shared" ref="P47:P48" si="56">F47/D47</f>
-        <v>250</v>
+        <f t="shared" ref="P47:P48" si="1">H47/D47</f>
+        <v>40</v>
       </c>
       <c r="Q47">
-        <f t="shared" ref="Q47:Q48" si="57">H47/D47</f>
-        <v>40</v>
+        <f t="shared" ref="Q47:Q48" si="2">I47/D47</f>
+        <v>85</v>
       </c>
       <c r="R47">
-        <f t="shared" ref="R47:R48" si="58">I47/D47</f>
-        <v>85</v>
-      </c>
-      <c r="S47">
-        <f t="shared" ref="S47:S48" si="59">J47/D47</f>
+        <f t="shared" ref="R47:R48" si="3">J47/D47</f>
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D48">
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F48">
-        <f t="shared" si="52"/>
+        <f>2.5*O30*D48</f>
         <v>2400</v>
       </c>
       <c r="G48">
         <v>160</v>
       </c>
       <c r="H48">
-        <f t="shared" si="53"/>
+        <f>2.5*P30*D48</f>
         <v>120</v>
       </c>
       <c r="I48">
-        <f t="shared" si="54"/>
+        <f>2.5*Q30*D48</f>
         <v>700</v>
       </c>
       <c r="J48">
-        <f t="shared" si="55"/>
+        <f>2.5*R30*D48</f>
         <v>120</v>
       </c>
       <c r="K48">
         <v>0</v>
       </c>
       <c r="L48">
-        <v>0.55000000000000004</v>
+        <v>1</v>
       </c>
       <c r="M48">
         <v>0.55000000000000004</v>
       </c>
-      <c r="N48">
-        <v>0.55000000000000004</v>
+      <c r="O48">
+        <f t="shared" si="0"/>
+        <v>300</v>
       </c>
       <c r="P48">
-        <f t="shared" si="56"/>
-        <v>300</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="57"/>
+        <f t="shared" si="2"/>
+        <v>87.5</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="R48">
-        <f t="shared" si="58"/>
-        <v>87.5</v>
-      </c>
-      <c r="S48">
-        <f t="shared" si="59"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -3094,24 +2999,21 @@
         <v>9</v>
       </c>
       <c r="K50" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="L50" t="s">
-        <v>11</v>
-      </c>
-      <c r="M50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C51" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E51">
         <v>210</v>
@@ -3132,24 +3034,21 @@
         <v>12</v>
       </c>
       <c r="K51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L51">
         <v>0</v>
       </c>
-      <c r="M51">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E52">
         <v>560</v>
@@ -3170,24 +3069,21 @@
         <v>14</v>
       </c>
       <c r="K52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L52">
         <v>0</v>
       </c>
-      <c r="M52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E53">
         <v>370</v>
@@ -3208,13 +3104,198 @@
         <v>16</v>
       </c>
       <c r="K53">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="L53">
         <v>1.5</v>
       </c>
-      <c r="M53">
-        <v>1.5</v>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" t="s">
+        <v>5</v>
+      </c>
+      <c r="H55" t="s">
+        <v>6</v>
+      </c>
+      <c r="I55" t="s">
+        <v>7</v>
+      </c>
+      <c r="J55" t="s">
+        <v>8</v>
+      </c>
+      <c r="K55" t="s">
+        <v>9</v>
+      </c>
+      <c r="L55" t="s">
+        <v>31</v>
+      </c>
+      <c r="M55" t="s">
+        <v>27</v>
+      </c>
+      <c r="N55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>4</v>
+      </c>
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>20</v>
+      </c>
+      <c r="E56">
+        <v>26</v>
+      </c>
+      <c r="F56">
+        <f>O28*D56*0.25</f>
+        <v>250</v>
+      </c>
+      <c r="G56">
+        <f>G29</f>
+        <v>570</v>
+      </c>
+      <c r="H56">
+        <f>P29*D56*0.5</f>
+        <v>160</v>
+      </c>
+      <c r="I56">
+        <f>Q29*D56</f>
+        <v>680</v>
+      </c>
+      <c r="J56">
+        <f>R29*D56*0.75</f>
+        <v>210</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>2</v>
+      </c>
+      <c r="M56">
+        <v>0.45</v>
+      </c>
+      <c r="N56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C57">
+        <v>3</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
+      </c>
+      <c r="E57">
+        <v>15</v>
+      </c>
+      <c r="F57">
+        <f>O38*D57*0.25</f>
+        <v>500</v>
+      </c>
+      <c r="G57">
+        <f>G47</f>
+        <v>680</v>
+      </c>
+      <c r="H57">
+        <f>P47*D57*0.5</f>
+        <v>400</v>
+      </c>
+      <c r="I57">
+        <f>Q47*D57*0.55</f>
+        <v>935.00000000000011</v>
+      </c>
+      <c r="J57">
+        <f>R47*D57*0.5</f>
+        <v>350</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>3</v>
+      </c>
+      <c r="M57">
+        <v>0.5</v>
+      </c>
+      <c r="N57">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>4</v>
+      </c>
+      <c r="B58" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>20</v>
+      </c>
+      <c r="E58">
+        <v>19</v>
+      </c>
+      <c r="F58">
+        <f>O28*D58*0.25</f>
+        <v>250</v>
+      </c>
+      <c r="G58">
+        <f>G25</f>
+        <v>500</v>
+      </c>
+      <c r="H58">
+        <f>P29*D56*0.35</f>
+        <v>112</v>
+      </c>
+      <c r="I58">
+        <f>Q29*D56</f>
+        <v>680</v>
+      </c>
+      <c r="J58">
+        <f>R29*D56*0.65</f>
+        <v>182</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <v>0.45</v>
+      </c>
+      <c r="N58">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented blast radius for flak
Can actually target and hit torpedoes
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="36">
   <si>
     <t>#</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>LongRange</t>
+  </si>
+  <si>
+    <t>Blast Radius</t>
   </si>
 </sst>
 </file>
@@ -930,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="N55" sqref="N55"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,14 +946,15 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -988,22 +992,25 @@
         <v>31</v>
       </c>
       <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1041,26 +1048,29 @@
         <v>1</v>
       </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>0.2</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <f>F2/D2</f>
         <v>20</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <f>H2/D2</f>
         <v>6</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <f>I2/D2</f>
         <v>16</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <f>J2/D2</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1098,26 +1108,29 @@
         <v>1</v>
       </c>
       <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
         <v>0.2</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <f>F3/D3</f>
         <v>30</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <f>H3/D3</f>
         <v>10</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <f>I3/D3</f>
         <v>14</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <f>J3/D3</f>
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1155,26 +1168,30 @@
         <v>1</v>
       </c>
       <c r="M4">
+        <f>N4/0.3*0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="N4">
         <v>0.3</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f>F4/D4</f>
         <v>40</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f>H4/D4</f>
         <v>6</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <f>I4/D4</f>
         <v>16</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <f>J4/D4</f>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1212,26 +1229,29 @@
         <v>1</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>0.3</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f>F6/D6</f>
         <v>30</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f>H6/D6</f>
         <v>4</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f>I6/D6</f>
         <v>20</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f>J6/D6</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1269,26 +1289,29 @@
         <v>1</v>
       </c>
       <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
         <v>0.3</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <f>F7/D7</f>
         <v>40</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <f>H7/D7</f>
         <v>6</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f>I7/D7</f>
         <v>14</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f>J7/D7</f>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1326,26 +1349,30 @@
         <v>1</v>
       </c>
       <c r="M8">
+        <f>N8/0.3*0.25</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="N8">
         <v>0.35</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <f>F8/D8</f>
         <v>45</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f>H8/D8</f>
         <v>3</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <f>I8/D8</f>
         <v>15</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <f>J8/D8</f>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1383,26 +1410,29 @@
         <v>1</v>
       </c>
       <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <v>0.3</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <f>F10/D10</f>
         <v>25</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <f>H10/D10</f>
         <v>3</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <f>I10/D10</f>
         <v>18</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <f>J10/D10</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1440,26 +1470,29 @@
         <v>1</v>
       </c>
       <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <v>0.35</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <f>F11/D11</f>
         <v>50</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <f>H11/D11</f>
         <v>8</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <f>I11/D11</f>
         <v>17</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f>J11/D11</f>
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1497,26 +1530,30 @@
         <v>1</v>
       </c>
       <c r="M12">
+        <f>N12/0.3*0.25</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="N12">
         <v>0.35</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <f>F12/D12</f>
         <v>60</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <f>H12/D12</f>
         <v>3</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <f>I12/D12</f>
         <v>17.5</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f>J12/D12</f>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1551,7 +1588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1586,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1621,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1656,7 +1693,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1691,10 +1728,13 @@
         <v>31</v>
       </c>
       <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1711,22 +1751,22 @@
         <v>12</v>
       </c>
       <c r="F20">
-        <f>2*O2*D20</f>
+        <f>2*P2*D20</f>
         <v>30</v>
       </c>
       <c r="G20">
         <v>250</v>
       </c>
       <c r="H20">
-        <f>2*P2*D20</f>
+        <f>2*Q2*D20</f>
         <v>9</v>
       </c>
       <c r="I20">
-        <f>2*Q2*D20</f>
+        <f>2*R2*D20</f>
         <v>24</v>
       </c>
       <c r="J20">
-        <f>2*R2*D20</f>
+        <f>2*S2*D20</f>
         <v>6</v>
       </c>
       <c r="K20">
@@ -1736,26 +1776,29 @@
         <v>1</v>
       </c>
       <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
         <v>0.3</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <f>F20/D20</f>
         <v>40</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <f>H20/D20</f>
         <v>12</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <f>I20/D20</f>
         <v>32</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <f>J20/D20</f>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1772,22 +1815,22 @@
         <v>13</v>
       </c>
       <c r="F21">
-        <f>2*O3*D21</f>
+        <f>2*P3*D21</f>
         <v>45</v>
       </c>
       <c r="G21">
         <v>170</v>
       </c>
       <c r="H21">
-        <f>2*P3*D21</f>
+        <f>2*Q3*D21</f>
         <v>15</v>
       </c>
       <c r="I21">
-        <f>2*Q3*D21</f>
+        <f>2*R3*D21</f>
         <v>21</v>
       </c>
       <c r="J21">
-        <f>2*R3*D21</f>
+        <f>2*S3*D21</f>
         <v>9</v>
       </c>
       <c r="K21">
@@ -1797,26 +1840,29 @@
         <v>1</v>
       </c>
       <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
         <v>0.3</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <f>F21/D21</f>
         <v>60</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <f>H21/D21</f>
         <v>20</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <f>I21/D21</f>
         <v>28</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <f>J21/D21</f>
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1833,22 +1879,22 @@
         <v>14</v>
       </c>
       <c r="F22">
-        <f>2*O4*D22</f>
+        <f>2*P4*D22</f>
         <v>60</v>
       </c>
       <c r="G22">
         <v>120</v>
       </c>
       <c r="H22">
-        <f>2*P4*D22</f>
+        <f>2*Q4*D22</f>
         <v>9</v>
       </c>
       <c r="I22">
-        <f>2*Q4*D22</f>
+        <f>2*R4*D22</f>
         <v>24</v>
       </c>
       <c r="J22">
-        <f>2*R4*D22</f>
+        <f>2*S4*D22</f>
         <v>3</v>
       </c>
       <c r="K22">
@@ -1858,26 +1904,30 @@
         <v>1</v>
       </c>
       <c r="M22">
+        <f>N22/0.3*0.25</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="N22">
         <v>0.35</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <f>F22/D22</f>
         <v>80</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <f>H22/D22</f>
         <v>12</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <f>I22/D22</f>
         <v>32</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <f>J22/D22</f>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1894,22 +1944,22 @@
         <v>12</v>
       </c>
       <c r="F24">
-        <f>2*O6*D24</f>
+        <f>2*P6*D24</f>
         <v>240</v>
       </c>
       <c r="G24">
         <v>750</v>
       </c>
       <c r="H24">
-        <f>2*P6*D24</f>
+        <f>2*Q6*D24</f>
         <v>32</v>
       </c>
       <c r="I24">
-        <f>2*Q6*D24</f>
+        <f>2*R6*D24</f>
         <v>160</v>
       </c>
       <c r="J24">
-        <f>2*R6*D24</f>
+        <f>2*S6*D24</f>
         <v>32</v>
       </c>
       <c r="K24">
@@ -1919,26 +1969,29 @@
         <v>1</v>
       </c>
       <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
         <v>0.35</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <f>F24/D24</f>
         <v>60</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <f>H24/D24</f>
         <v>8</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <f>I24/D24</f>
         <v>40</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <f>J24/D24</f>
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -1955,22 +2008,22 @@
         <v>13</v>
       </c>
       <c r="F25">
-        <f>2*O7*D25</f>
+        <f>2*P7*D25</f>
         <v>320</v>
       </c>
       <c r="G25">
         <v>500</v>
       </c>
       <c r="H25">
-        <f>2*P7*D25</f>
+        <f>2*Q7*D25</f>
         <v>48</v>
       </c>
       <c r="I25">
-        <f>2*Q7*D25</f>
+        <f>2*R7*D25</f>
         <v>112</v>
       </c>
       <c r="J25">
-        <f>2*R7*D25</f>
+        <f>2*S7*D25</f>
         <v>40</v>
       </c>
       <c r="K25">
@@ -1980,26 +2033,29 @@
         <v>1</v>
       </c>
       <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
         <v>0.35</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <f>F25/D25</f>
         <v>80</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <f>H25/D25</f>
         <v>12</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <f>I25/D25</f>
         <v>28</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <f>J25/D25</f>
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2016,22 +2072,22 @@
         <v>14</v>
       </c>
       <c r="F26">
-        <f>2*O8*D26</f>
+        <f>2*P8*D26</f>
         <v>360</v>
       </c>
       <c r="G26">
         <v>150</v>
       </c>
       <c r="H26">
-        <f>2*P8*D26</f>
+        <f>2*Q8*D26</f>
         <v>24</v>
       </c>
       <c r="I26">
-        <f>2*Q8*D26</f>
+        <f>2*R8*D26</f>
         <v>120</v>
       </c>
       <c r="J26">
-        <f>2*R8*D26</f>
+        <f>2*S8*D26</f>
         <v>24</v>
       </c>
       <c r="K26">
@@ -2041,26 +2097,30 @@
         <v>1</v>
       </c>
       <c r="M26">
+        <f>N26/0.3*0.25</f>
+        <v>0.33333333333333337</v>
+      </c>
+      <c r="N26">
         <v>0.4</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <f>F26/D26</f>
         <v>90</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <f>H26/D26</f>
         <v>6</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <f>I26/D26</f>
         <v>30</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <f>J26/D26</f>
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2077,22 +2137,22 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <f>2*O10*D28</f>
+        <f>2*P10*D28</f>
         <v>200</v>
       </c>
       <c r="G28">
         <v>580</v>
       </c>
       <c r="H28">
-        <f>2*P10*D28</f>
+        <f>2*Q10*D28</f>
         <v>24</v>
       </c>
       <c r="I28">
-        <f>2*Q10*D28</f>
+        <f>2*R10*D28</f>
         <v>144</v>
       </c>
       <c r="J28">
-        <f>2*R10*D28</f>
+        <f>2*S10*D28</f>
         <v>24</v>
       </c>
       <c r="K28">
@@ -2102,26 +2162,29 @@
         <v>1</v>
       </c>
       <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
         <v>0.35</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <f>F28/D28</f>
         <v>50</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <f>H28/D28</f>
         <v>6</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <f>I28/D28</f>
         <v>36</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <f>J28/D28</f>
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2138,22 +2201,22 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <f>2*O11*D29</f>
+        <f>2*P11*D29</f>
         <v>400</v>
       </c>
       <c r="G29">
         <v>570</v>
       </c>
       <c r="H29">
-        <f>2*P11*D29</f>
+        <f>2*Q11*D29</f>
         <v>64</v>
       </c>
       <c r="I29">
-        <f>2*Q11*D29</f>
+        <f>2*R11*D29</f>
         <v>136</v>
       </c>
       <c r="J29">
-        <f>2*R11*D29</f>
+        <f>2*S11*D29</f>
         <v>56</v>
       </c>
       <c r="K29">
@@ -2163,26 +2226,29 @@
         <v>1</v>
       </c>
       <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
         <v>0.45</v>
       </c>
-      <c r="O29">
+      <c r="P29">
         <f>F29/D29</f>
         <v>100</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <f>H29/D29</f>
         <v>16</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <f>I29/D29</f>
         <v>34</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <f>J29/D29</f>
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2199,22 +2265,22 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <f>2*O12*D30</f>
+        <f>2*P12*D30</f>
         <v>480</v>
       </c>
       <c r="G30">
         <v>160</v>
       </c>
       <c r="H30">
-        <f>2*P12*D30</f>
+        <f>2*Q12*D30</f>
         <v>24</v>
       </c>
       <c r="I30">
-        <f>2*Q12*D30</f>
+        <f>2*R12*D30</f>
         <v>140</v>
       </c>
       <c r="J30">
-        <f>2*R12*D30</f>
+        <f>2*S12*D30</f>
         <v>24</v>
       </c>
       <c r="K30">
@@ -2224,26 +2290,30 @@
         <v>1</v>
       </c>
       <c r="M30">
+        <f>N30/0.3*0.25</f>
+        <v>0.375</v>
+      </c>
+      <c r="N30">
         <v>0.45</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <f>F30/D30</f>
         <v>120</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <f>H30/D30</f>
         <v>6</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <f>I30/D30</f>
         <v>35</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <f>J30/D30</f>
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +2348,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2313,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2348,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2383,7 +2453,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2418,10 +2488,13 @@
         <v>31</v>
       </c>
       <c r="M37" t="s">
+        <v>35</v>
+      </c>
+      <c r="N37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2438,22 +2511,22 @@
         <v>12</v>
       </c>
       <c r="F38">
-        <f>2.5*O20*D38</f>
+        <f>2.5*P20*D38</f>
         <v>100</v>
       </c>
       <c r="G38">
         <v>310</v>
       </c>
       <c r="H38">
-        <f>2.5*P20*D38</f>
+        <f>2.5*Q20*D38</f>
         <v>30</v>
       </c>
       <c r="I38">
-        <f>2.5*Q20*D38</f>
+        <f>2.5*R20*D38</f>
         <v>80</v>
       </c>
       <c r="J38">
-        <f>2.5*R20*D38</f>
+        <f>2.5*S20*D38</f>
         <v>20</v>
       </c>
       <c r="K38">
@@ -2463,26 +2536,29 @@
         <v>1</v>
       </c>
       <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
         <v>0.3</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <f>F38/D38</f>
         <v>100</v>
       </c>
-      <c r="P38">
+      <c r="Q38">
         <f>H38/D38</f>
         <v>30</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <f>I38/D38</f>
         <v>80</v>
       </c>
-      <c r="R38">
+      <c r="S38">
         <f>J38/D38</f>
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2499,22 +2575,22 @@
         <v>13</v>
       </c>
       <c r="F39">
-        <f>2.5*O21*D39</f>
+        <f>2.5*P21*D39</f>
         <v>150</v>
       </c>
       <c r="G39">
         <v>270</v>
       </c>
       <c r="H39">
-        <f>2.5*P21*D39</f>
+        <f>2.5*Q21*D39</f>
         <v>50</v>
       </c>
       <c r="I39">
-        <f>2.5*Q21*D39</f>
+        <f>2.5*R21*D39</f>
         <v>70</v>
       </c>
       <c r="J39">
-        <f>2.5*R21*D39</f>
+        <f>2.5*S21*D39</f>
         <v>30</v>
       </c>
       <c r="K39">
@@ -2524,26 +2600,29 @@
         <v>1</v>
       </c>
       <c r="M39">
+        <v>0</v>
+      </c>
+      <c r="N39">
         <v>0.3</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <f>F39/D39</f>
         <v>150</v>
       </c>
-      <c r="P39">
+      <c r="Q39">
         <f>H39/D39</f>
         <v>50</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <f>I39/D39</f>
         <v>70</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <f>J39/D39</f>
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2560,22 +2639,22 @@
         <v>14</v>
       </c>
       <c r="F40">
-        <f>2.5*O22*D40</f>
+        <f>2.5*P22*D40</f>
         <v>200</v>
       </c>
       <c r="G40">
         <v>180</v>
       </c>
       <c r="H40">
-        <f>2.5*P22*D40</f>
+        <f>2.5*Q22*D40</f>
         <v>30</v>
       </c>
       <c r="I40">
-        <f>2.5*Q22*D40</f>
+        <f>2.5*R22*D40</f>
         <v>80</v>
       </c>
       <c r="J40">
-        <f>2.5*R22*D40</f>
+        <f>2.5*S22*D40</f>
         <v>10</v>
       </c>
       <c r="K40">
@@ -2585,26 +2664,30 @@
         <v>1</v>
       </c>
       <c r="M40">
+        <f>N40/0.3*0.25</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="N40">
         <v>0.35</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <f>F40/D40</f>
         <v>200</v>
       </c>
-      <c r="P40">
+      <c r="Q40">
         <f>H40/D40</f>
         <v>30</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <f>I40/D40</f>
         <v>80</v>
       </c>
-      <c r="R40">
+      <c r="S40">
         <f>J40/D40</f>
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2621,22 +2704,22 @@
         <v>12</v>
       </c>
       <c r="F42">
-        <f>2.5*O24*D42</f>
+        <f>2.5*P24*D42</f>
         <v>1200</v>
       </c>
       <c r="G42">
         <v>1000</v>
       </c>
       <c r="H42">
-        <f>2.5*P24*D42</f>
+        <f>2.5*Q24*D42</f>
         <v>160</v>
       </c>
       <c r="I42">
-        <f>2.5*Q24*D42</f>
+        <f>2.5*R24*D42</f>
         <v>800</v>
       </c>
       <c r="J42">
-        <f>2.5*R24*D42</f>
+        <f>2.5*S24*D42</f>
         <v>160</v>
       </c>
       <c r="K42">
@@ -2646,26 +2729,29 @@
         <v>1</v>
       </c>
       <c r="M42">
+        <v>0</v>
+      </c>
+      <c r="N42">
         <v>0.4</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <f>F42/D42</f>
         <v>150</v>
       </c>
-      <c r="P42">
+      <c r="Q42">
         <f>H42/D42</f>
         <v>20</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <f>I42/D42</f>
         <v>100</v>
       </c>
-      <c r="R42">
+      <c r="S42">
         <f>J42/D42</f>
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2682,22 +2768,22 @@
         <v>13</v>
       </c>
       <c r="F43">
-        <f>2.5*O25*D43</f>
+        <f>2.5*P25*D43</f>
         <v>1600</v>
       </c>
       <c r="G43">
         <v>650</v>
       </c>
       <c r="H43">
-        <f>2.5*P25*D43</f>
+        <f>2.5*Q25*D43</f>
         <v>240</v>
       </c>
       <c r="I43">
-        <f>2.5*Q25*D43</f>
+        <f>2.5*R25*D43</f>
         <v>560</v>
       </c>
       <c r="J43">
-        <f>2.5*R25*D43</f>
+        <f>2.5*S25*D43</f>
         <v>200</v>
       </c>
       <c r="K43">
@@ -2707,26 +2793,29 @@
         <v>1</v>
       </c>
       <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
         <v>0.45</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <f>F43/D43</f>
         <v>200</v>
       </c>
-      <c r="P43">
+      <c r="Q43">
         <f>H43/D43</f>
         <v>30</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <f>I43/D43</f>
         <v>70</v>
       </c>
-      <c r="R43">
+      <c r="S43">
         <f>J43/D43</f>
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2743,22 +2832,22 @@
         <v>14</v>
       </c>
       <c r="F44">
-        <f>2.5*O26*D44</f>
+        <f>2.5*P26*D44</f>
         <v>1800</v>
       </c>
       <c r="G44">
         <v>180</v>
       </c>
       <c r="H44">
-        <f>2.5*P26*D44</f>
+        <f>2.5*Q26*D44</f>
         <v>120</v>
       </c>
       <c r="I44">
-        <f>2.5*Q26*D44</f>
+        <f>2.5*R26*D44</f>
         <v>600</v>
       </c>
       <c r="J44">
-        <f>2.5*R26*D44</f>
+        <f>2.5*S26*D44</f>
         <v>120</v>
       </c>
       <c r="K44">
@@ -2768,26 +2857,30 @@
         <v>1</v>
       </c>
       <c r="M44">
+        <f>N44/0.3*0.25</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N44">
         <v>0.5</v>
       </c>
-      <c r="O44">
+      <c r="P44">
         <f>F44/D44</f>
         <v>225</v>
       </c>
-      <c r="P44">
+      <c r="Q44">
         <f>H44/D44</f>
         <v>15</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <f>I44/D44</f>
         <v>75</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <f>J44/D44</f>
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2804,22 +2897,22 @@
         <v>12</v>
       </c>
       <c r="F46">
-        <f>2.5*O28*D46</f>
+        <f>2.5*P28*D46</f>
         <v>1000</v>
       </c>
       <c r="G46">
         <v>650</v>
       </c>
       <c r="H46">
-        <f>2.5*P28*D46</f>
+        <f>2.5*Q28*D46</f>
         <v>120</v>
       </c>
       <c r="I46">
-        <f>2.5*Q28*D46</f>
+        <f>2.5*R28*D46</f>
         <v>720</v>
       </c>
       <c r="J46">
-        <f>2.5*R28*D46</f>
+        <f>2.5*S28*D46</f>
         <v>120</v>
       </c>
       <c r="K46">
@@ -2829,26 +2922,29 @@
         <v>1</v>
       </c>
       <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
         <v>0.4</v>
       </c>
-      <c r="O46">
+      <c r="P46">
         <f>F46/D46</f>
         <v>125</v>
       </c>
-      <c r="P46">
+      <c r="Q46">
         <f>H46/D46</f>
         <v>15</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <f>I46/D46</f>
         <v>90</v>
       </c>
-      <c r="R46">
+      <c r="S46">
         <f>J46/D46</f>
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2865,22 +2961,22 @@
         <v>13</v>
       </c>
       <c r="F47">
-        <f>2.5*O29*D47</f>
+        <f>2.5*P29*D47</f>
         <v>2000</v>
       </c>
       <c r="G47">
         <v>680</v>
       </c>
       <c r="H47">
-        <f>2.5*P29*D47</f>
+        <f>2.5*Q29*D47</f>
         <v>320</v>
       </c>
       <c r="I47">
-        <f>2.5*Q29*D47</f>
+        <f>2.5*R29*D47</f>
         <v>680</v>
       </c>
       <c r="J47">
-        <f>2.5*R29*D47</f>
+        <f>2.5*S29*D47</f>
         <v>280</v>
       </c>
       <c r="K47">
@@ -2890,26 +2986,29 @@
         <v>1</v>
       </c>
       <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47">
         <v>0.5</v>
       </c>
-      <c r="O47">
-        <f t="shared" ref="O47:O48" si="0">F47/D47</f>
+      <c r="P47">
+        <f t="shared" ref="P47:P48" si="0">F47/D47</f>
         <v>250</v>
       </c>
-      <c r="P47">
-        <f t="shared" ref="P47:P48" si="1">H47/D47</f>
+      <c r="Q47">
+        <f t="shared" ref="Q47:Q48" si="1">H47/D47</f>
         <v>40</v>
       </c>
-      <c r="Q47">
-        <f t="shared" ref="Q47:Q48" si="2">I47/D47</f>
+      <c r="R47">
+        <f t="shared" ref="R47:R48" si="2">I47/D47</f>
         <v>85</v>
       </c>
-      <c r="R47">
-        <f t="shared" ref="R47:R48" si="3">J47/D47</f>
+      <c r="S47">
+        <f t="shared" ref="S47:S48" si="3">J47/D47</f>
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -2926,22 +3025,22 @@
         <v>14</v>
       </c>
       <c r="F48">
-        <f>2.5*O30*D48</f>
+        <f>2.5*P30*D48</f>
         <v>2400</v>
       </c>
       <c r="G48">
         <v>160</v>
       </c>
       <c r="H48">
-        <f>2.5*P30*D48</f>
+        <f>2.5*Q30*D48</f>
         <v>120</v>
       </c>
       <c r="I48">
-        <f>2.5*Q30*D48</f>
+        <f>2.5*R30*D48</f>
         <v>700</v>
       </c>
       <c r="J48">
-        <f>2.5*R30*D48</f>
+        <f>2.5*S30*D48</f>
         <v>120</v>
       </c>
       <c r="K48">
@@ -2951,21 +3050,25 @@
         <v>1</v>
       </c>
       <c r="M48">
+        <f>N48/0.3*0.25</f>
+        <v>0.45833333333333337</v>
+      </c>
+      <c r="N48">
         <v>0.55000000000000004</v>
       </c>
-      <c r="O48">
+      <c r="P48">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="P48">
+      <c r="Q48">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="Q48">
+      <c r="R48">
         <f t="shared" si="2"/>
         <v>87.5</v>
       </c>
-      <c r="R48">
+      <c r="S48">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
@@ -3168,7 +3271,7 @@
         <v>26</v>
       </c>
       <c r="F56">
-        <f>O28*D56*0.25</f>
+        <f>P28*D56*0.25</f>
         <v>250</v>
       </c>
       <c r="G56">
@@ -3176,15 +3279,15 @@
         <v>570</v>
       </c>
       <c r="H56">
-        <f>P29*D56*0.5</f>
+        <f>Q29*D56*0.5</f>
         <v>160</v>
       </c>
       <c r="I56">
-        <f>Q29*D56</f>
+        <f>R29*D56</f>
         <v>680</v>
       </c>
       <c r="J56">
-        <f>R29*D56*0.75</f>
+        <f>S29*D56*0.75</f>
         <v>210</v>
       </c>
       <c r="K56">
@@ -3217,7 +3320,7 @@
         <v>15</v>
       </c>
       <c r="F57">
-        <f>O38*D57*0.25</f>
+        <f>P38*D57*0.25</f>
         <v>500</v>
       </c>
       <c r="G57">
@@ -3225,15 +3328,15 @@
         <v>680</v>
       </c>
       <c r="H57">
-        <f>P47*D57*0.5</f>
+        <f>Q47*D57*0.5</f>
         <v>400</v>
       </c>
       <c r="I57">
-        <f>Q47*D57*0.55</f>
+        <f>R47*D57*0.55</f>
         <v>935.00000000000011</v>
       </c>
       <c r="J57">
-        <f>R47*D57*0.5</f>
+        <f>S47*D57*0.5</f>
         <v>350</v>
       </c>
       <c r="K57">
@@ -3266,7 +3369,7 @@
         <v>19</v>
       </c>
       <c r="F58">
-        <f>O28*D58*0.25</f>
+        <f>P28*D58*0.25</f>
         <v>250</v>
       </c>
       <c r="G58">
@@ -3274,15 +3377,15 @@
         <v>500</v>
       </c>
       <c r="H58">
-        <f>P29*D56*0.35</f>
+        <f>Q29*D56*0.35</f>
         <v>112</v>
       </c>
       <c r="I58">
-        <f>Q29*D56</f>
+        <f>R29*D56</f>
         <v>680</v>
       </c>
       <c r="J58">
-        <f>R29*D56*0.65</f>
+        <f>S29*D56*0.65</f>
         <v>182</v>
       </c>
       <c r="K58">

</xml_diff>

<commit_message>
Completely redesigned damage system
Now an armour penetration table is used to reach "reasonable" hit rates.
Also a damage mitigation system is introduced.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -935,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1030,7 @@
         <v>10</v>
       </c>
       <c r="G2">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="H2">
         <v>3</v>
@@ -1090,7 +1090,7 @@
         <v>15</v>
       </c>
       <c r="G3">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="H3">
         <v>5</v>
@@ -1150,7 +1150,7 @@
         <v>20</v>
       </c>
       <c r="G4">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -1211,7 +1211,7 @@
         <v>60</v>
       </c>
       <c r="G6">
-        <v>350</v>
+        <v>250</v>
       </c>
       <c r="H6">
         <v>8</v>
@@ -1271,7 +1271,7 @@
         <v>80</v>
       </c>
       <c r="G7">
-        <v>230</v>
+        <v>145</v>
       </c>
       <c r="H7">
         <v>12</v>
@@ -1331,7 +1331,7 @@
         <v>90</v>
       </c>
       <c r="G8">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="H8">
         <v>6</v>
@@ -1392,7 +1392,7 @@
         <v>50</v>
       </c>
       <c r="G10">
-        <v>280</v>
+        <v>180</v>
       </c>
       <c r="H10">
         <v>6</v>
@@ -1452,7 +1452,7 @@
         <v>100</v>
       </c>
       <c r="G11">
-        <v>260</v>
+        <v>175</v>
       </c>
       <c r="H11">
         <v>16</v>
@@ -1512,7 +1512,7 @@
         <v>120</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="H12">
         <v>6</v>
@@ -1602,7 +1602,7 @@
         <v>45</v>
       </c>
       <c r="F15">
-        <v>260</v>
+        <v>225</v>
       </c>
       <c r="G15">
         <v>10</v>
@@ -1637,7 +1637,7 @@
         <v>100</v>
       </c>
       <c r="F16">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="G16">
         <v>5</v>
@@ -1672,7 +1672,7 @@
         <v>75</v>
       </c>
       <c r="F17">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="G17">
         <v>7</v>
@@ -1755,7 +1755,7 @@
         <v>30</v>
       </c>
       <c r="G20">
-        <v>250</v>
+        <v>155</v>
       </c>
       <c r="H20">
         <f>2*Q2*D20</f>
@@ -1819,7 +1819,7 @@
         <v>45</v>
       </c>
       <c r="G21">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="H21">
         <f>2*Q3*D21</f>
@@ -1883,7 +1883,7 @@
         <v>60</v>
       </c>
       <c r="G22">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="H22">
         <f>2*Q4*D22</f>
@@ -1948,7 +1948,7 @@
         <v>240</v>
       </c>
       <c r="G24">
-        <v>750</v>
+        <v>500</v>
       </c>
       <c r="H24">
         <f>2*Q6*D24</f>
@@ -2012,7 +2012,7 @@
         <v>320</v>
       </c>
       <c r="G25">
-        <v>500</v>
+        <v>280</v>
       </c>
       <c r="H25">
         <f>2*Q7*D25</f>
@@ -2076,7 +2076,7 @@
         <v>360</v>
       </c>
       <c r="G26">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="H26">
         <f>2*Q8*D26</f>
@@ -2141,7 +2141,7 @@
         <v>200</v>
       </c>
       <c r="G28">
-        <v>580</v>
+        <v>380</v>
       </c>
       <c r="H28">
         <f>2*Q10*D28</f>
@@ -2205,7 +2205,7 @@
         <v>400</v>
       </c>
       <c r="G29">
-        <v>570</v>
+        <v>350</v>
       </c>
       <c r="H29">
         <f>2*Q11*D29</f>
@@ -2269,7 +2269,7 @@
         <v>480</v>
       </c>
       <c r="G30">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="H30">
         <f>2*Q12*D30</f>
@@ -2362,7 +2362,7 @@
         <v>100</v>
       </c>
       <c r="F33">
-        <v>525</v>
+        <v>450</v>
       </c>
       <c r="G33">
         <v>22</v>
@@ -2397,7 +2397,7 @@
         <v>250</v>
       </c>
       <c r="F34">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="G34">
         <v>12</v>
@@ -2432,7 +2432,7 @@
         <v>170</v>
       </c>
       <c r="F35">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="G35">
         <v>16</v>
@@ -2515,7 +2515,7 @@
         <v>100</v>
       </c>
       <c r="G38">
-        <v>310</v>
+        <v>270</v>
       </c>
       <c r="H38">
         <f>2.5*Q20*D38</f>
@@ -2579,7 +2579,7 @@
         <v>150</v>
       </c>
       <c r="G39">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="H39">
         <f>2.5*Q21*D39</f>
@@ -2643,7 +2643,7 @@
         <v>200</v>
       </c>
       <c r="G40">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="H40">
         <f>2.5*Q22*D40</f>
@@ -2772,7 +2772,7 @@
         <v>1600</v>
       </c>
       <c r="G43">
-        <v>650</v>
+        <v>600</v>
       </c>
       <c r="H43">
         <f>2.5*Q25*D43</f>
@@ -2836,7 +2836,7 @@
         <v>1800</v>
       </c>
       <c r="G44">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="H44">
         <f>2.5*Q26*D44</f>
@@ -2901,7 +2901,7 @@
         <v>1000</v>
       </c>
       <c r="G46">
-        <v>650</v>
+        <v>770</v>
       </c>
       <c r="H46">
         <f>2.5*Q28*D46</f>
@@ -2965,7 +2965,7 @@
         <v>2000</v>
       </c>
       <c r="G47">
-        <v>680</v>
+        <v>700</v>
       </c>
       <c r="H47">
         <f>2.5*Q29*D47</f>
@@ -2992,19 +2992,19 @@
         <v>0.5</v>
       </c>
       <c r="P47">
-        <f t="shared" ref="P47:P48" si="0">F47/D47</f>
+        <f>F47/D47</f>
         <v>250</v>
       </c>
       <c r="Q47">
-        <f t="shared" ref="Q47:Q48" si="1">H47/D47</f>
+        <f>H47/D47</f>
         <v>40</v>
       </c>
       <c r="R47">
-        <f t="shared" ref="R47:R48" si="2">I47/D47</f>
+        <f>I47/D47</f>
         <v>85</v>
       </c>
       <c r="S47">
-        <f t="shared" ref="S47:S48" si="3">J47/D47</f>
+        <f>J47/D47</f>
         <v>35</v>
       </c>
     </row>
@@ -3029,7 +3029,7 @@
         <v>2400</v>
       </c>
       <c r="G48">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="H48">
         <f>2.5*Q30*D48</f>
@@ -3057,19 +3057,19 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="P48">
-        <f t="shared" si="0"/>
+        <f>F48/D48</f>
         <v>300</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="1"/>
+        <f>H48/D48</f>
         <v>15</v>
       </c>
       <c r="R48">
-        <f t="shared" si="2"/>
+        <f>I48/D48</f>
         <v>87.5</v>
       </c>
       <c r="S48">
-        <f t="shared" si="3"/>
+        <f>J48/D48</f>
         <v>15</v>
       </c>
     </row>
@@ -3122,7 +3122,7 @@
         <v>210</v>
       </c>
       <c r="F51">
-        <v>625</v>
+        <v>800</v>
       </c>
       <c r="G51">
         <v>50</v>
@@ -3157,7 +3157,7 @@
         <v>560</v>
       </c>
       <c r="F52">
-        <v>270</v>
+        <v>450</v>
       </c>
       <c r="G52">
         <v>25</v>
@@ -3192,7 +3192,7 @@
         <v>370</v>
       </c>
       <c r="F53">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="G53">
         <v>35</v>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="G56">
         <f>G29</f>
-        <v>570</v>
+        <v>350</v>
       </c>
       <c r="H56">
         <f>Q29*D56*0.5</f>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="G57">
         <f>G47</f>
-        <v>680</v>
+        <v>700</v>
       </c>
       <c r="H57">
         <f>Q47*D57*0.5</f>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="G58">
         <f>G25</f>
-        <v>500</v>
+        <v>280</v>
       </c>
       <c r="H58">
         <f>Q29*D56*0.35</f>

</xml_diff>

<commit_message>
More work on strike craft
Implemented strike craft weapons that are configured from the main
configuration files.
Implemented a *very basic* strike craft AI. Also made some improvements
to ship AI.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="39">
   <si>
     <t>#</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Blast Radius</t>
+  </si>
+  <si>
+    <t>StrikeCraft</t>
+  </si>
+  <si>
+    <t>FighterCannon</t>
+  </si>
+  <si>
+    <t>FighterAutoannon</t>
   </si>
 </sst>
 </file>
@@ -933,16 +942,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="M56" sqref="M56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -3218,13 +3227,13 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F55" t="s">
         <v>4</v>
@@ -3248,156 +3257,289 @@
         <v>31</v>
       </c>
       <c r="M55" t="s">
+        <v>35</v>
+      </c>
+      <c r="N55" t="s">
         <v>27</v>
-      </c>
-      <c r="N55" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" t="s">
+        <v>37</v>
+      </c>
+      <c r="D56">
+        <v>0.75</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <f>1*D56*P20</f>
+        <v>30</v>
+      </c>
+      <c r="G56">
+        <v>175</v>
+      </c>
+      <c r="H56">
+        <f>1*D56*Q20</f>
+        <v>9</v>
+      </c>
+      <c r="I56">
+        <f>1*D56*R20</f>
+        <v>24</v>
+      </c>
+      <c r="J56">
+        <f>1*D56*S20</f>
+        <v>6</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57">
+        <v>0.5</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+      <c r="N57">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59" t="s">
         <v>4</v>
       </c>
-      <c r="B56" t="s">
+      <c r="G59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H59" t="s">
+        <v>6</v>
+      </c>
+      <c r="I59" t="s">
+        <v>7</v>
+      </c>
+      <c r="J59" t="s">
+        <v>8</v>
+      </c>
+      <c r="K59" t="s">
+        <v>9</v>
+      </c>
+      <c r="L59" t="s">
+        <v>31</v>
+      </c>
+      <c r="M59" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60" t="s">
         <v>34</v>
       </c>
-      <c r="C56">
+      <c r="C60">
         <v>4</v>
       </c>
-      <c r="D56">
+      <c r="D60">
         <v>20</v>
       </c>
-      <c r="E56">
+      <c r="E60">
         <v>26</v>
       </c>
-      <c r="F56">
-        <f>P28*D56*0.25</f>
+      <c r="F60">
+        <f>P28*D60*0.25</f>
         <v>250</v>
       </c>
-      <c r="G56">
+      <c r="G60">
         <f>G29</f>
         <v>350</v>
       </c>
-      <c r="H56">
-        <f>Q29*D56*0.5</f>
+      <c r="H60">
+        <f>Q29*D60*0.5</f>
         <v>160</v>
       </c>
-      <c r="I56">
-        <f>R29*D56</f>
+      <c r="I60">
+        <f>R29*D60</f>
         <v>680</v>
       </c>
-      <c r="J56">
-        <f>S29*D56*0.75</f>
+      <c r="J60">
+        <f>S29*D60*0.75</f>
         <v>210</v>
       </c>
-      <c r="K56">
-        <v>0</v>
-      </c>
-      <c r="L56">
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
         <v>2</v>
       </c>
-      <c r="M56">
+      <c r="M60">
         <v>0.45</v>
       </c>
-      <c r="N56">
+      <c r="N60">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61">
         <v>4</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B61" t="s">
         <v>21</v>
       </c>
-      <c r="C57">
-        <v>3</v>
-      </c>
-      <c r="D57">
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61">
         <v>20</v>
       </c>
-      <c r="E57">
+      <c r="E61">
         <v>15</v>
       </c>
-      <c r="F57">
-        <f>P38*D57*0.25</f>
+      <c r="F61">
+        <f>P38*D61*0.25</f>
         <v>500</v>
       </c>
-      <c r="G57">
+      <c r="G61">
         <f>G47</f>
         <v>700</v>
       </c>
-      <c r="H57">
-        <f>Q47*D57*0.5</f>
+      <c r="H61">
+        <f>Q47*D61*0.5</f>
         <v>400</v>
       </c>
-      <c r="I57">
-        <f>R47*D57*0.55</f>
+      <c r="I61">
+        <f>R47*D61*0.55</f>
         <v>935.00000000000011</v>
       </c>
-      <c r="J57">
-        <f>S47*D57*0.5</f>
+      <c r="J61">
+        <f>S47*D61*0.5</f>
         <v>350</v>
       </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <v>3</v>
-      </c>
-      <c r="M57">
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <v>3</v>
+      </c>
+      <c r="M61">
         <v>0.5</v>
       </c>
-      <c r="N57">
+      <c r="N61">
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
         <v>4</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B62" t="s">
         <v>29</v>
       </c>
-      <c r="C58">
+      <c r="C62">
         <v>2</v>
       </c>
-      <c r="D58">
+      <c r="D62">
         <v>20</v>
       </c>
-      <c r="E58">
+      <c r="E62">
         <v>19</v>
       </c>
-      <c r="F58">
-        <f>P28*D58*0.25</f>
+      <c r="F62">
+        <f>P28*D62*0.25</f>
         <v>250</v>
       </c>
-      <c r="G58">
+      <c r="G62">
         <f>G25</f>
         <v>280</v>
       </c>
-      <c r="H58">
-        <f>Q29*D56*0.35</f>
+      <c r="H62">
+        <f>Q29*D60*0.35</f>
         <v>112</v>
       </c>
-      <c r="I58">
-        <f>R29*D56</f>
+      <c r="I62">
+        <f>R29*D60</f>
         <v>680</v>
       </c>
-      <c r="J58">
-        <f>S29*D56*0.65</f>
+      <c r="J62">
+        <f>S29*D60*0.65</f>
         <v>182</v>
       </c>
-      <c r="K58">
-        <v>0</v>
-      </c>
-      <c r="L58">
+      <c r="K62">
+        <v>0</v>
+      </c>
+      <c r="L62">
         <v>2</v>
       </c>
-      <c r="M58">
+      <c r="M62">
         <v>0.45</v>
       </c>
-      <c r="N58">
+      <c r="N62">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rescaled the game by 0.5
All models, effects, AI ditance hints, etc. have been scaled by 0.5.
Also, all distance and size constants have been moved to a global class
(at least I hope it's all of them).
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -944,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection sqref="A1:N62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="P2">
         <f>F2/D2</f>
@@ -1120,7 +1120,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="P3">
         <f>F3/D3</f>
@@ -1178,10 +1178,10 @@
       </c>
       <c r="M4">
         <f>N4/0.3*0.25</f>
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="N4">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P4">
         <f>F4/D4</f>
@@ -1241,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P6">
         <f>F6/D6</f>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P7">
         <f>F7/D7</f>
@@ -1359,10 +1359,10 @@
       </c>
       <c r="M8">
         <f>N8/0.3*0.25</f>
-        <v>0.29166666666666669</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="N8">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P8">
         <f>F8/D8</f>
@@ -1422,7 +1422,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P10">
         <f>F10/D10</f>
@@ -1482,7 +1482,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P11">
         <f>F11/D11</f>
@@ -1540,10 +1540,10 @@
       </c>
       <c r="M12">
         <f>N12/0.3*0.25</f>
-        <v>0.29166666666666669</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="N12">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P12">
         <f>F12/D12</f>
@@ -1788,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P20">
         <f>F20/D20</f>
@@ -1852,7 +1852,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P21">
         <f>F21/D21</f>
@@ -1914,10 +1914,10 @@
       </c>
       <c r="M22">
         <f>N22/0.3*0.25</f>
-        <v>0.29166666666666669</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="N22">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P22">
         <f>F22/D22</f>
@@ -1981,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P24">
         <f>F24/D24</f>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P25">
         <f>F25/D25</f>
@@ -2107,10 +2107,10 @@
       </c>
       <c r="M26">
         <f>N26/0.3*0.25</f>
-        <v>0.33333333333333337</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="N26">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="P26">
         <f>F26/D26</f>
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P28">
         <f>F28/D28</f>
@@ -2238,7 +2238,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0.45</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="P29">
         <f>F29/D29</f>
@@ -2300,10 +2300,10 @@
       </c>
       <c r="M30">
         <f>N30/0.3*0.25</f>
-        <v>0.375</v>
+        <v>0.1875</v>
       </c>
       <c r="N30">
-        <v>0.45</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="P30">
         <f>F30/D30</f>
@@ -2548,7 +2548,7 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P38">
         <f>F38/D38</f>
@@ -2612,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="P39">
         <f>F39/D39</f>
@@ -2674,10 +2674,10 @@
       </c>
       <c r="M40">
         <f>N40/0.3*0.25</f>
-        <v>0.29166666666666669</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="N40">
-        <v>0.35</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="P40">
         <f>F40/D40</f>
@@ -2741,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="N42">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="P42">
         <f>F42/D42</f>
@@ -2805,7 +2805,7 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0.45</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="P43">
         <f>F43/D43</f>
@@ -2867,10 +2867,10 @@
       </c>
       <c r="M44">
         <f>N44/0.3*0.25</f>
-        <v>0.41666666666666669</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="N44">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P44">
         <f>F44/D44</f>
@@ -2934,7 +2934,7 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="P46">
         <f>F46/D46</f>
@@ -2998,7 +2998,7 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="P47">
         <f>F47/D47</f>
@@ -3060,10 +3060,10 @@
       </c>
       <c r="M48">
         <f>N48/0.3*0.25</f>
-        <v>0.45833333333333337</v>
+        <v>0.22916666666666669</v>
       </c>
       <c r="N48">
-        <v>0.55000000000000004</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="P48">
         <f>F48/D48</f>
@@ -3308,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="N56">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
@@ -3352,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="N57">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -3439,10 +3439,10 @@
         <v>2</v>
       </c>
       <c r="M60">
-        <v>0.45</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="N60">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -3488,10 +3488,10 @@
         <v>3</v>
       </c>
       <c r="M61">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="N61">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
@@ -3537,10 +3537,10 @@
         <v>2</v>
       </c>
       <c r="M62">
-        <v>0.45</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="N62">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented effectiveness vs. strike craft stat for warheads
Now weapons have a chance to completely miss strike craft, with heavier
weapons having a higher chance of missing.
Also slightly improved pathing algorithm. This will need more work.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="40">
   <si>
     <t>#</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>FighterAutoannon</t>
+  </si>
+  <si>
+    <t>Vs. strike craft</t>
   </si>
 </sst>
 </file>
@@ -942,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection sqref="A1:N62"/>
+    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,15 +958,16 @@
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1004,22 +1008,25 @@
         <v>35</v>
       </c>
       <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
         <v>27</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1060,26 +1067,29 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.1</v>
-      </c>
-      <c r="P2">
+        <v>0.65</v>
+      </c>
+      <c r="O2">
+        <v>0.2</v>
+      </c>
+      <c r="Q2">
         <f>F2/D2</f>
         <v>20</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <f>H2/D2</f>
         <v>6</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <f>I2/D2</f>
         <v>16</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <f>J2/D2</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1120,26 +1130,29 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.1</v>
-      </c>
-      <c r="P3">
+        <v>0.65</v>
+      </c>
+      <c r="O3">
+        <v>0.2</v>
+      </c>
+      <c r="Q3">
         <f>F3/D3</f>
         <v>30</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <f>H3/D3</f>
         <v>10</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <f>I3/D3</f>
         <v>14</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <f>J3/D3</f>
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1177,30 +1190,33 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <f>N4/0.3*0.25</f>
-        <v>0.125</v>
+        <f>O4/0.3*0.5</f>
+        <v>0.5</v>
       </c>
       <c r="N4">
-        <v>0.15</v>
-      </c>
-      <c r="P4">
+        <v>0.8</v>
+      </c>
+      <c r="O4">
+        <v>0.3</v>
+      </c>
+      <c r="Q4">
         <f>F4/D4</f>
         <v>40</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <f>H4/D4</f>
         <v>6</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <f>I4/D4</f>
         <v>16</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <f>J4/D4</f>
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1241,26 +1257,29 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.15</v>
-      </c>
-      <c r="P6">
+        <v>0.6</v>
+      </c>
+      <c r="O6">
+        <v>0.3</v>
+      </c>
+      <c r="Q6">
         <f>F6/D6</f>
         <v>30</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f>H6/D6</f>
         <v>4</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f>I6/D6</f>
         <v>20</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <f>J6/D6</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1301,26 +1320,29 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.15</v>
-      </c>
-      <c r="P7">
+        <v>0.6</v>
+      </c>
+      <c r="O7">
+        <v>0.3</v>
+      </c>
+      <c r="Q7">
         <f>F7/D7</f>
         <v>40</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f>H7/D7</f>
         <v>6</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f>I7/D7</f>
         <v>14</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <f>J7/D7</f>
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1358,30 +1380,33 @@
         <v>1</v>
       </c>
       <c r="M8">
-        <f>N8/0.3*0.25</f>
-        <v>0.14583333333333334</v>
+        <f>O8/0.3*0.5</f>
+        <v>0.58333333333333337</v>
       </c>
       <c r="N8">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P8">
+        <v>0.9</v>
+      </c>
+      <c r="O8">
+        <v>0.35</v>
+      </c>
+      <c r="Q8">
         <f>F8/D8</f>
         <v>45</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <f>H8/D8</f>
         <v>3</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <f>I8/D8</f>
         <v>15</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <f>J8/D8</f>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1422,26 +1447,29 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.15</v>
-      </c>
-      <c r="P10">
+        <v>0.6</v>
+      </c>
+      <c r="O10">
+        <v>0.3</v>
+      </c>
+      <c r="Q10">
         <f>F10/D10</f>
         <v>25</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <f>H10/D10</f>
         <v>3</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <f>I10/D10</f>
         <v>18</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <f>J10/D10</f>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1482,26 +1510,29 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P11">
+        <v>0.6</v>
+      </c>
+      <c r="O11">
+        <v>0.35</v>
+      </c>
+      <c r="Q11">
         <f>F11/D11</f>
         <v>50</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <f>H11/D11</f>
         <v>8</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f>I11/D11</f>
         <v>17</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <f>J11/D11</f>
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1539,30 +1570,33 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <f>N12/0.3*0.25</f>
-        <v>0.14583333333333334</v>
+        <f>O12/0.3*0.5</f>
+        <v>0.58333333333333337</v>
       </c>
       <c r="N12">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P12">
+        <v>0.9</v>
+      </c>
+      <c r="O12">
+        <v>0.35</v>
+      </c>
+      <c r="Q12">
         <f>F12/D12</f>
         <v>60</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <f>H12/D12</f>
         <v>3</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f>I12/D12</f>
         <v>17.5</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <f>J12/D12</f>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1597,7 +1631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1632,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1667,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1702,7 +1736,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1740,10 +1774,13 @@
         <v>35</v>
       </c>
       <c r="N19" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1760,22 +1797,22 @@
         <v>12</v>
       </c>
       <c r="F20">
-        <f>2*P2*D20</f>
+        <f>2*Q2*D20</f>
         <v>30</v>
       </c>
       <c r="G20">
         <v>155</v>
       </c>
       <c r="H20">
-        <f>2*Q2*D20</f>
+        <f>2*R2*D20</f>
         <v>9</v>
       </c>
       <c r="I20">
-        <f>2*R2*D20</f>
+        <f>2*S2*D20</f>
         <v>24</v>
       </c>
       <c r="J20">
-        <f>2*S2*D20</f>
+        <f>2*T2*D20</f>
         <v>6</v>
       </c>
       <c r="K20">
@@ -1788,26 +1825,29 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0.15</v>
-      </c>
-      <c r="P20">
+        <v>0.45</v>
+      </c>
+      <c r="O20">
+        <v>0.3</v>
+      </c>
+      <c r="Q20">
         <f>F20/D20</f>
         <v>40</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <f>H20/D20</f>
         <v>12</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <f>I20/D20</f>
         <v>32</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <f>J20/D20</f>
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1824,22 +1864,22 @@
         <v>13</v>
       </c>
       <c r="F21">
-        <f>2*P3*D21</f>
+        <f>2*Q3*D21</f>
         <v>45</v>
       </c>
       <c r="G21">
         <v>140</v>
       </c>
       <c r="H21">
-        <f>2*Q3*D21</f>
+        <f>2*R3*D21</f>
         <v>15</v>
       </c>
       <c r="I21">
-        <f>2*R3*D21</f>
+        <f>2*S3*D21</f>
         <v>21</v>
       </c>
       <c r="J21">
-        <f>2*S3*D21</f>
+        <f>2*T3*D21</f>
         <v>12</v>
       </c>
       <c r="K21">
@@ -1852,26 +1892,29 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.15</v>
-      </c>
-      <c r="P21">
+        <v>0.45</v>
+      </c>
+      <c r="O21">
+        <v>0.3</v>
+      </c>
+      <c r="Q21">
         <f>F21/D21</f>
         <v>60</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <f>H21/D21</f>
         <v>20</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <f>I21/D21</f>
         <v>28</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <f>J21/D21</f>
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1888,22 +1931,22 @@
         <v>14</v>
       </c>
       <c r="F22">
-        <f>2*P4*D22</f>
+        <f>2*Q4*D22</f>
         <v>60</v>
       </c>
       <c r="G22">
         <v>50</v>
       </c>
       <c r="H22">
-        <f>2*Q4*D22</f>
+        <f>2*R4*D22</f>
         <v>9</v>
       </c>
       <c r="I22">
-        <f>2*R4*D22</f>
+        <f>2*S4*D22</f>
         <v>24</v>
       </c>
       <c r="J22">
-        <f>2*S4*D22</f>
+        <f>2*T4*D22</f>
         <v>3</v>
       </c>
       <c r="K22">
@@ -1913,30 +1956,33 @@
         <v>1</v>
       </c>
       <c r="M22">
-        <f>N22/0.3*0.25</f>
-        <v>0.14583333333333334</v>
+        <f>O22/0.3*0.5</f>
+        <v>0.58333333333333337</v>
       </c>
       <c r="N22">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P22">
+        <v>0.9</v>
+      </c>
+      <c r="O22">
+        <v>0.35</v>
+      </c>
+      <c r="Q22">
         <f>F22/D22</f>
         <v>80</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <f>H22/D22</f>
         <v>12</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <f>I22/D22</f>
         <v>32</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <f>J22/D22</f>
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1953,22 +1999,22 @@
         <v>12</v>
       </c>
       <c r="F24">
-        <f>2*P6*D24</f>
+        <f>2*Q6*D24</f>
         <v>240</v>
       </c>
       <c r="G24">
         <v>500</v>
       </c>
       <c r="H24">
-        <f>2*Q6*D24</f>
+        <f>2*R6*D24</f>
         <v>32</v>
       </c>
       <c r="I24">
-        <f>2*R6*D24</f>
+        <f>2*S6*D24</f>
         <v>160</v>
       </c>
       <c r="J24">
-        <f>2*S6*D24</f>
+        <f>2*T6*D24</f>
         <v>32</v>
       </c>
       <c r="K24">
@@ -1981,26 +2027,29 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P24">
+        <v>0.35</v>
+      </c>
+      <c r="O24">
+        <v>0.35</v>
+      </c>
+      <c r="Q24">
         <f>F24/D24</f>
         <v>60</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <f>H24/D24</f>
         <v>8</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <f>I24/D24</f>
         <v>40</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <f>J24/D24</f>
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2017,22 +2066,22 @@
         <v>13</v>
       </c>
       <c r="F25">
-        <f>2*P7*D25</f>
+        <f>2*Q7*D25</f>
         <v>320</v>
       </c>
       <c r="G25">
         <v>280</v>
       </c>
       <c r="H25">
-        <f>2*Q7*D25</f>
+        <f>2*R7*D25</f>
         <v>48</v>
       </c>
       <c r="I25">
-        <f>2*R7*D25</f>
+        <f>2*S7*D25</f>
         <v>112</v>
       </c>
       <c r="J25">
-        <f>2*S7*D25</f>
+        <f>2*T7*D25</f>
         <v>64</v>
       </c>
       <c r="K25">
@@ -2045,26 +2094,29 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P25">
+        <v>0.35</v>
+      </c>
+      <c r="O25">
+        <v>0.35</v>
+      </c>
+      <c r="Q25">
         <f>F25/D25</f>
         <v>80</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <f>H25/D25</f>
         <v>12</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <f>I25/D25</f>
         <v>28</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <f>J25/D25</f>
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2081,22 +2133,22 @@
         <v>14</v>
       </c>
       <c r="F26">
-        <f>2*P8*D26</f>
+        <f>2*Q8*D26</f>
         <v>360</v>
       </c>
       <c r="G26">
         <v>100</v>
       </c>
       <c r="H26">
-        <f>2*Q8*D26</f>
+        <f>2*R8*D26</f>
         <v>24</v>
       </c>
       <c r="I26">
-        <f>2*R8*D26</f>
+        <f>2*S8*D26</f>
         <v>120</v>
       </c>
       <c r="J26">
-        <f>2*S8*D26</f>
+        <f>2*T8*D26</f>
         <v>24</v>
       </c>
       <c r="K26">
@@ -2106,30 +2158,33 @@
         <v>1</v>
       </c>
       <c r="M26">
-        <f>N26/0.3*0.25</f>
-        <v>0.16666666666666669</v>
+        <f>O26/0.3*0.5</f>
+        <v>0.66666666666666674</v>
       </c>
       <c r="N26">
-        <v>0.2</v>
-      </c>
-      <c r="P26">
+        <v>0.95</v>
+      </c>
+      <c r="O26">
+        <v>0.4</v>
+      </c>
+      <c r="Q26">
         <f>F26/D26</f>
         <v>90</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <f>H26/D26</f>
         <v>6</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <f>I26/D26</f>
         <v>30</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <f>J26/D26</f>
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2146,22 +2201,22 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <f>2*P10*D28</f>
+        <f>2*Q10*D28</f>
         <v>200</v>
       </c>
       <c r="G28">
         <v>380</v>
       </c>
       <c r="H28">
-        <f>2*Q10*D28</f>
+        <f>2*R10*D28</f>
         <v>24</v>
       </c>
       <c r="I28">
-        <f>2*R10*D28</f>
+        <f>2*S10*D28</f>
         <v>144</v>
       </c>
       <c r="J28">
-        <f>2*S10*D28</f>
+        <f>2*T10*D28</f>
         <v>24</v>
       </c>
       <c r="K28">
@@ -2174,26 +2229,29 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P28">
+        <v>0.35</v>
+      </c>
+      <c r="O28">
+        <v>0.35</v>
+      </c>
+      <c r="Q28">
         <f>F28/D28</f>
         <v>50</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <f>H28/D28</f>
         <v>6</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <f>I28/D28</f>
         <v>36</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <f>J28/D28</f>
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2210,22 +2268,22 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <f>2*P11*D29</f>
+        <f>2*Q11*D29</f>
         <v>400</v>
       </c>
       <c r="G29">
         <v>350</v>
       </c>
       <c r="H29">
-        <f>2*Q11*D29</f>
+        <f>2*R11*D29</f>
         <v>64</v>
       </c>
       <c r="I29">
-        <f>2*R11*D29</f>
+        <f>2*S11*D29</f>
         <v>136</v>
       </c>
       <c r="J29">
-        <f>2*S11*D29</f>
+        <f>2*T11*D29</f>
         <v>96</v>
       </c>
       <c r="K29">
@@ -2238,26 +2296,29 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="P29">
+        <v>0.35</v>
+      </c>
+      <c r="O29">
+        <v>0.45</v>
+      </c>
+      <c r="Q29">
         <f>F29/D29</f>
         <v>100</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <f>H29/D29</f>
         <v>16</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <f>I29/D29</f>
         <v>34</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <f>J29/D29</f>
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2274,22 +2335,22 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <f>2*P12*D30</f>
+        <f>2*Q12*D30</f>
         <v>480</v>
       </c>
       <c r="G30">
         <v>130</v>
       </c>
       <c r="H30">
-        <f>2*Q12*D30</f>
+        <f>2*R12*D30</f>
         <v>24</v>
       </c>
       <c r="I30">
-        <f>2*R12*D30</f>
+        <f>2*S12*D30</f>
         <v>140</v>
       </c>
       <c r="J30">
-        <f>2*S12*D30</f>
+        <f>2*T12*D30</f>
         <v>24</v>
       </c>
       <c r="K30">
@@ -2299,30 +2360,33 @@
         <v>1</v>
       </c>
       <c r="M30">
-        <f>N30/0.3*0.25</f>
-        <v>0.1875</v>
+        <f>O30/0.3*0.5</f>
+        <v>0.75</v>
       </c>
       <c r="N30">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="P30">
+        <v>0.95</v>
+      </c>
+      <c r="O30">
+        <v>0.45</v>
+      </c>
+      <c r="Q30">
         <f>F30/D30</f>
         <v>120</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <f>H30/D30</f>
         <v>6</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <f>I30/D30</f>
         <v>35</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <f>J30/D30</f>
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2357,7 +2421,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2392,7 +2456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2427,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2462,7 +2526,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2500,10 +2564,13 @@
         <v>35</v>
       </c>
       <c r="N37" t="s">
+        <v>39</v>
+      </c>
+      <c r="O37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2520,22 +2587,22 @@
         <v>12</v>
       </c>
       <c r="F38">
-        <f>2.5*P20*D38</f>
+        <f>2.5*Q20*D38</f>
         <v>100</v>
       </c>
       <c r="G38">
         <v>270</v>
       </c>
       <c r="H38">
-        <f>2.5*Q20*D38</f>
+        <f>2.5*R20*D38</f>
         <v>30</v>
       </c>
       <c r="I38">
-        <f>2.5*R20*D38</f>
+        <f>2.5*S20*D38</f>
         <v>80</v>
       </c>
       <c r="J38">
-        <f>2.5*S20*D38</f>
+        <f>2.5*T20*D38</f>
         <v>20</v>
       </c>
       <c r="K38">
@@ -2548,26 +2615,29 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0.15</v>
-      </c>
-      <c r="P38">
+        <v>0.3</v>
+      </c>
+      <c r="O38">
+        <v>0.3</v>
+      </c>
+      <c r="Q38">
         <f>F38/D38</f>
         <v>100</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <f>H38/D38</f>
         <v>30</v>
       </c>
-      <c r="R38">
+      <c r="S38">
         <f>I38/D38</f>
         <v>80</v>
       </c>
-      <c r="S38">
+      <c r="T38">
         <f>J38/D38</f>
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2584,22 +2654,22 @@
         <v>13</v>
       </c>
       <c r="F39">
-        <f>2.5*P21*D39</f>
+        <f>2.5*Q21*D39</f>
         <v>150</v>
       </c>
       <c r="G39">
         <v>250</v>
       </c>
       <c r="H39">
-        <f>2.5*Q21*D39</f>
+        <f>2.5*R21*D39</f>
         <v>50</v>
       </c>
       <c r="I39">
-        <f>2.5*R21*D39</f>
+        <f>2.5*S21*D39</f>
         <v>70</v>
       </c>
       <c r="J39">
-        <f>2.5*S21*D39</f>
+        <f>2.5*T21*D39</f>
         <v>40</v>
       </c>
       <c r="K39">
@@ -2612,26 +2682,29 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0.15</v>
-      </c>
-      <c r="P39">
+        <v>0.3</v>
+      </c>
+      <c r="O39">
+        <v>0.3</v>
+      </c>
+      <c r="Q39">
         <f>F39/D39</f>
         <v>150</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <f>H39/D39</f>
         <v>50</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <f>I39/D39</f>
         <v>70</v>
       </c>
-      <c r="S39">
+      <c r="T39">
         <f>J39/D39</f>
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2648,22 +2721,22 @@
         <v>14</v>
       </c>
       <c r="F40">
-        <f>2.5*P22*D40</f>
+        <f>2.5*Q22*D40</f>
         <v>200</v>
       </c>
       <c r="G40">
         <v>100</v>
       </c>
       <c r="H40">
-        <f>2.5*Q22*D40</f>
+        <f>2.5*R22*D40</f>
         <v>30</v>
       </c>
       <c r="I40">
-        <f>2.5*R22*D40</f>
+        <f>2.5*S22*D40</f>
         <v>80</v>
       </c>
       <c r="J40">
-        <f>2.5*S22*D40</f>
+        <f>2.5*T22*D40</f>
         <v>10</v>
       </c>
       <c r="K40">
@@ -2673,30 +2746,33 @@
         <v>1</v>
       </c>
       <c r="M40">
-        <f>N40/0.3*0.25</f>
-        <v>0.14583333333333334</v>
+        <f>O40/0.3*0.25</f>
+        <v>0.29166666666666669</v>
       </c>
       <c r="N40">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="P40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>0.35</v>
+      </c>
+      <c r="Q40">
         <f>F40/D40</f>
         <v>200</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <f>H40/D40</f>
         <v>30</v>
       </c>
-      <c r="R40">
+      <c r="S40">
         <f>I40/D40</f>
         <v>80</v>
       </c>
-      <c r="S40">
+      <c r="T40">
         <f>J40/D40</f>
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2713,22 +2789,22 @@
         <v>12</v>
       </c>
       <c r="F42">
-        <f>2.5*P24*D42</f>
+        <f>2.5*Q24*D42</f>
         <v>1200</v>
       </c>
       <c r="G42">
         <v>1000</v>
       </c>
       <c r="H42">
-        <f>2.5*Q24*D42</f>
+        <f>2.5*R24*D42</f>
         <v>160</v>
       </c>
       <c r="I42">
-        <f>2.5*R24*D42</f>
+        <f>2.5*S24*D42</f>
         <v>800</v>
       </c>
       <c r="J42">
-        <f>2.5*S24*D42</f>
+        <f>2.5*T24*D42</f>
         <v>160</v>
       </c>
       <c r="K42">
@@ -2743,24 +2819,27 @@
       <c r="N42">
         <v>0.2</v>
       </c>
-      <c r="P42">
+      <c r="O42">
+        <v>0.4</v>
+      </c>
+      <c r="Q42">
         <f>F42/D42</f>
         <v>150</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <f>H42/D42</f>
         <v>20</v>
       </c>
-      <c r="R42">
+      <c r="S42">
         <f>I42/D42</f>
         <v>100</v>
       </c>
-      <c r="S42">
+      <c r="T42">
         <f>J42/D42</f>
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2777,22 +2856,22 @@
         <v>13</v>
       </c>
       <c r="F43">
-        <f>2.5*P25*D43</f>
+        <f>2.5*Q25*D43</f>
         <v>1600</v>
       </c>
       <c r="G43">
         <v>600</v>
       </c>
       <c r="H43">
-        <f>2.5*Q25*D43</f>
+        <f>2.5*R25*D43</f>
         <v>240</v>
       </c>
       <c r="I43">
-        <f>2.5*R25*D43</f>
+        <f>2.5*S25*D43</f>
         <v>560</v>
       </c>
       <c r="J43">
-        <f>2.5*S25*D43</f>
+        <f>2.5*T25*D43</f>
         <v>320</v>
       </c>
       <c r="K43">
@@ -2805,26 +2884,29 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="P43">
+        <v>0.2</v>
+      </c>
+      <c r="O43">
+        <v>0.45</v>
+      </c>
+      <c r="Q43">
         <f>F43/D43</f>
         <v>200</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <f>H43/D43</f>
         <v>30</v>
       </c>
-      <c r="R43">
+      <c r="S43">
         <f>I43/D43</f>
         <v>70</v>
       </c>
-      <c r="S43">
+      <c r="T43">
         <f>J43/D43</f>
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2841,22 +2923,22 @@
         <v>14</v>
       </c>
       <c r="F44">
-        <f>2.5*P26*D44</f>
+        <f>2.5*Q26*D44</f>
         <v>1800</v>
       </c>
       <c r="G44">
         <v>160</v>
       </c>
       <c r="H44">
-        <f>2.5*Q26*D44</f>
+        <f>2.5*R26*D44</f>
         <v>120</v>
       </c>
       <c r="I44">
-        <f>2.5*R26*D44</f>
+        <f>2.5*S26*D44</f>
         <v>600</v>
       </c>
       <c r="J44">
-        <f>2.5*S26*D44</f>
+        <f>2.5*T26*D44</f>
         <v>120</v>
       </c>
       <c r="K44">
@@ -2866,30 +2948,33 @@
         <v>1</v>
       </c>
       <c r="M44">
-        <f>N44/0.3*0.25</f>
-        <v>0.20833333333333334</v>
+        <f>O44/0.3*0.25</f>
+        <v>0.41666666666666669</v>
       </c>
       <c r="N44">
-        <v>0.25</v>
-      </c>
-      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <v>0.5</v>
+      </c>
+      <c r="Q44">
         <f>F44/D44</f>
         <v>225</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <f>H44/D44</f>
         <v>15</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <f>I44/D44</f>
         <v>75</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <f>J44/D44</f>
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2906,22 +2991,22 @@
         <v>12</v>
       </c>
       <c r="F46">
-        <f>2.5*P28*D46</f>
+        <f>2.5*Q28*D46</f>
         <v>1000</v>
       </c>
       <c r="G46">
         <v>770</v>
       </c>
       <c r="H46">
-        <f>2.5*Q28*D46</f>
+        <f>2.5*R28*D46</f>
         <v>120</v>
       </c>
       <c r="I46">
-        <f>2.5*R28*D46</f>
+        <f>2.5*S28*D46</f>
         <v>720</v>
       </c>
       <c r="J46">
-        <f>2.5*S28*D46</f>
+        <f>2.5*T28*D46</f>
         <v>120</v>
       </c>
       <c r="K46">
@@ -2936,24 +3021,27 @@
       <c r="N46">
         <v>0.2</v>
       </c>
-      <c r="P46">
+      <c r="O46">
+        <v>0.4</v>
+      </c>
+      <c r="Q46">
         <f>F46/D46</f>
         <v>125</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <f>H46/D46</f>
         <v>15</v>
       </c>
-      <c r="R46">
+      <c r="S46">
         <f>I46/D46</f>
         <v>90</v>
       </c>
-      <c r="S46">
+      <c r="T46">
         <f>J46/D46</f>
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -2970,22 +3058,22 @@
         <v>13</v>
       </c>
       <c r="F47">
-        <f>2.5*P29*D47</f>
+        <f>2.5*Q29*D47</f>
         <v>2000</v>
       </c>
       <c r="G47">
         <v>700</v>
       </c>
       <c r="H47">
-        <f>2.5*Q29*D47</f>
+        <f>2.5*R29*D47</f>
         <v>320</v>
       </c>
       <c r="I47">
-        <f>2.5*R29*D47</f>
+        <f>2.5*S29*D47</f>
         <v>680</v>
       </c>
       <c r="J47">
-        <f>2.5*S29*D47</f>
+        <f>2.5*T29*D47</f>
         <v>480</v>
       </c>
       <c r="K47">
@@ -2998,26 +3086,29 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0.25</v>
-      </c>
-      <c r="P47">
+        <v>0.2</v>
+      </c>
+      <c r="O47">
+        <v>0.5</v>
+      </c>
+      <c r="Q47">
         <f>F47/D47</f>
         <v>250</v>
       </c>
-      <c r="Q47">
+      <c r="R47">
         <f>H47/D47</f>
         <v>40</v>
       </c>
-      <c r="R47">
+      <c r="S47">
         <f>I47/D47</f>
         <v>85</v>
       </c>
-      <c r="S47">
+      <c r="T47">
         <f>J47/D47</f>
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -3034,22 +3125,22 @@
         <v>14</v>
       </c>
       <c r="F48">
-        <f>2.5*P30*D48</f>
+        <f>2.5*Q30*D48</f>
         <v>2400</v>
       </c>
       <c r="G48">
         <v>180</v>
       </c>
       <c r="H48">
-        <f>2.5*Q30*D48</f>
+        <f>2.5*R30*D48</f>
         <v>120</v>
       </c>
       <c r="I48">
-        <f>2.5*R30*D48</f>
+        <f>2.5*S30*D48</f>
         <v>700</v>
       </c>
       <c r="J48">
-        <f>2.5*S30*D48</f>
+        <f>2.5*T30*D48</f>
         <v>120</v>
       </c>
       <c r="K48">
@@ -3059,30 +3150,33 @@
         <v>1</v>
       </c>
       <c r="M48">
-        <f>N48/0.3*0.25</f>
-        <v>0.22916666666666669</v>
+        <f>O48/0.3*0.25</f>
+        <v>0.45833333333333337</v>
       </c>
       <c r="N48">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="O48">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Q48">
         <f>F48/D48</f>
         <v>300</v>
       </c>
-      <c r="Q48">
+      <c r="R48">
         <f>H48/D48</f>
         <v>15</v>
       </c>
-      <c r="R48">
+      <c r="S48">
         <f>I48/D48</f>
         <v>87.5</v>
       </c>
-      <c r="S48">
+      <c r="T48">
         <f>J48/D48</f>
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -3117,7 +3211,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3152,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3187,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3222,7 +3316,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -3260,10 +3354,13 @@
         <v>35</v>
       </c>
       <c r="N55" t="s">
+        <v>39</v>
+      </c>
+      <c r="O55" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3280,22 +3377,22 @@
         <v>12</v>
       </c>
       <c r="F56">
-        <f>1*D56*P20</f>
+        <f>1*D56*Q20</f>
         <v>30</v>
       </c>
       <c r="G56">
         <v>175</v>
       </c>
       <c r="H56">
-        <f>1*D56*Q20</f>
+        <f>1*D56*R20</f>
         <v>9</v>
       </c>
       <c r="I56">
-        <f>1*D56*R20</f>
+        <f>1*D56*S20</f>
         <v>24</v>
       </c>
       <c r="J56">
-        <f>1*D56*S20</f>
+        <f>1*D56*T20</f>
         <v>6</v>
       </c>
       <c r="K56">
@@ -3308,10 +3405,13 @@
         <v>0</v>
       </c>
       <c r="N56">
+        <v>1</v>
+      </c>
+      <c r="O56">
         <v>0.15</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -3352,10 +3452,13 @@
         <v>0</v>
       </c>
       <c r="N57">
+        <v>0.65</v>
+      </c>
+      <c r="O57">
         <v>0.1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -3396,7 +3499,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -3413,7 +3516,7 @@
         <v>26</v>
       </c>
       <c r="F60">
-        <f>P28*D60*0.25</f>
+        <f>Q28*D60*0.25</f>
         <v>250</v>
       </c>
       <c r="G60">
@@ -3421,15 +3524,15 @@
         <v>350</v>
       </c>
       <c r="H60">
-        <f>Q29*D60*0.5</f>
+        <f>R29*D60*0.5</f>
         <v>160</v>
       </c>
       <c r="I60">
-        <f>R29*D60</f>
+        <f>S29*D60</f>
         <v>680</v>
       </c>
       <c r="J60">
-        <f>S29*D60*0.75</f>
+        <f>T29*D60*0.75</f>
         <v>360</v>
       </c>
       <c r="K60">
@@ -3445,7 +3548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -3462,7 +3565,7 @@
         <v>15</v>
       </c>
       <c r="F61">
-        <f>P38*D61*0.25</f>
+        <f>Q38*D61*0.25</f>
         <v>500</v>
       </c>
       <c r="G61">
@@ -3470,15 +3573,15 @@
         <v>700</v>
       </c>
       <c r="H61">
-        <f>Q47*D61*0.5</f>
+        <f>R47*D61*0.5</f>
         <v>400</v>
       </c>
       <c r="I61">
-        <f>R47*D61*0.55</f>
+        <f>S47*D61*0.55</f>
         <v>935.00000000000011</v>
       </c>
       <c r="J61">
-        <f>S47*D61*0.5</f>
+        <f>T47*D61*0.5</f>
         <v>600</v>
       </c>
       <c r="K61">
@@ -3494,7 +3597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -3511,7 +3614,7 @@
         <v>19</v>
       </c>
       <c r="F62">
-        <f>P28*D62*0.25</f>
+        <f>Q28*D62*0.25</f>
         <v>250</v>
       </c>
       <c r="G62">
@@ -3519,15 +3622,15 @@
         <v>280</v>
       </c>
       <c r="H62">
-        <f>Q29*D60*0.35</f>
+        <f>R29*D60*0.35</f>
         <v>112</v>
       </c>
       <c r="I62">
-        <f>R29*D60</f>
+        <f>S29*D60</f>
         <v>680</v>
       </c>
       <c r="J62">
-        <f>S29*D60*0.65</f>
+        <f>T29*D60*0.65</f>
         <v>312</v>
       </c>
       <c r="K62">

</xml_diff>

<commit_message>
Added NavBoxes for all ships
NavBoxes are box colliders that are all assigned to a special
NavColliders layer. They will be used in the Bug0 navigation algorithm
(not yet committed), and possibly other collider tests that do not
require high precision.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="O2">
         <v>0.2</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="O3">
         <v>0.2</v>
@@ -1194,7 +1194,7 @@
         <v>0.5</v>
       </c>
       <c r="N4">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="O4">
         <v>0.3</v>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O6">
         <v>0.3</v>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O7">
         <v>0.3</v>
@@ -1384,7 +1384,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N8">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="O8">
         <v>0.35</v>
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O10">
         <v>0.3</v>
@@ -1510,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.6</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O11">
         <v>0.35</v>
@@ -1574,7 +1574,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N12">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="O12">
         <v>0.35</v>
@@ -1825,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="O20">
         <v>0.3</v>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.45</v>
+        <v>0.35</v>
       </c>
       <c r="O21">
         <v>0.3</v>
@@ -1960,7 +1960,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N22">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="O22">
         <v>0.35</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="O24">
         <v>0.35</v>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="O25">
         <v>0.35</v>
@@ -2162,7 +2162,7 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="N26">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="O26">
         <v>0.4</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="O28">
         <v>0.35</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="O29">
         <v>0.45</v>
@@ -2364,7 +2364,7 @@
         <v>0.75</v>
       </c>
       <c r="N30">
-        <v>0.95</v>
+        <v>0.9</v>
       </c>
       <c r="O30">
         <v>0.45</v>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O38">
         <v>0.3</v>
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O39">
         <v>0.3</v>
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="N42">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O42">
         <v>0.4</v>
@@ -2884,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O43">
         <v>0.45</v>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O46">
         <v>0.4</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O47">
         <v>0.5</v>

</xml_diff>

<commit_message>
Minor re-balancing of weapons
Made strike craft even harder to hit.
Also changed the scale of projectile trails so that they it would be
easier to tell smaller weapons from larger ones when zoomed out.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="O2">
         <v>0.2</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="O3">
         <v>0.2</v>
@@ -1194,7 +1194,7 @@
         <v>0.5</v>
       </c>
       <c r="N4">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="O4">
         <v>0.3</v>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="O6">
         <v>0.3</v>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="O7">
         <v>0.3</v>
@@ -1384,7 +1384,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N8">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="O8">
         <v>0.35</v>
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="O10">
         <v>0.3</v>
@@ -1510,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.55000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="O11">
         <v>0.35</v>
@@ -1574,7 +1574,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N12">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="O12">
         <v>0.35</v>
@@ -1825,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="O20">
         <v>0.3</v>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.35</v>
+        <v>0.2</v>
       </c>
       <c r="O21">
         <v>0.3</v>
@@ -1960,7 +1960,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N22">
-        <v>0.85</v>
+        <v>0.4</v>
       </c>
       <c r="O22">
         <v>0.35</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="O24">
         <v>0.35</v>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="O25">
         <v>0.35</v>
@@ -2162,7 +2162,7 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="N26">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="O26">
         <v>0.4</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="O28">
         <v>0.35</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="O29">
         <v>0.45</v>
@@ -2364,7 +2364,7 @@
         <v>0.75</v>
       </c>
       <c r="N30">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="O30">
         <v>0.45</v>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="O38">
         <v>0.3</v>
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="O39">
         <v>0.3</v>
@@ -2750,7 +2750,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="N40">
-        <v>1</v>
+        <v>0.65</v>
       </c>
       <c r="O40">
         <v>0.35</v>
@@ -2952,7 +2952,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="N44">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="O44">
         <v>0.5</v>
@@ -3154,7 +3154,7 @@
         <v>0.45833333333333337</v>
       </c>
       <c r="N48">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="O48">
         <v>0.55000000000000004</v>

</xml_diff>

<commit_message>
Several changes to buff/debuff system and damage
1. Implemented hitpoint buffs/debuffs for the ship hull, components, and
turrets.
2. Implemented hit multiplicity. Now weapons with a multiplicity on n
roll armour penetration n times cause damage for each success.
3. Unified scale of ship hitpoints with strike craft hitpoints. Strike
craft no longer have "fractions of hitpoints".
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="J58" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1055,7 @@
         <v>8</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="T2">
         <f>J2/D2</f>
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1118,7 +1118,7 @@
         <v>7</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="T3">
         <f>J3/D3</f>
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1181,7 +1181,7 @@
         <v>8</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="T4">
         <f>J4/D4</f>
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -1245,7 +1245,7 @@
         <v>40</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="T6">
         <f>J6/D6</f>
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1308,7 +1308,7 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="T7">
         <f>J7/D7</f>
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -1371,7 +1371,7 @@
         <v>30</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="T8">
         <f>J8/D8</f>
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1435,7 +1435,7 @@
         <v>36</v>
       </c>
       <c r="J10">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="T10">
         <f>J10/D10</f>
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1498,7 +1498,7 @@
         <v>34</v>
       </c>
       <c r="J11">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="T11">
         <f>J11/D11</f>
-        <v>12</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1561,7 +1561,7 @@
         <v>35</v>
       </c>
       <c r="J12">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="T12">
         <f>J12/D12</f>
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1657,7 +1657,7 @@
         <v>8</v>
       </c>
       <c r="J15">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1692,7 +1692,7 @@
         <v>7</v>
       </c>
       <c r="J16">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1727,7 +1727,7 @@
         <v>7</v>
       </c>
       <c r="J17">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="J20">
         <f>2*T2*D20</f>
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="T20">
         <f>J20/D20</f>
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
@@ -1879,8 +1879,8 @@
         <v>21</v>
       </c>
       <c r="J21">
-        <f>2*T3*D21</f>
-        <v>12</v>
+        <f>2.5*T3*D21</f>
+        <v>150</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="T21">
         <f>J21/D21</f>
-        <v>16</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
       </c>
       <c r="J22">
         <f>2*T4*D22</f>
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="T22">
         <f>J22/D22</f>
-        <v>4</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -2010,12 +2010,12 @@
         <v>32</v>
       </c>
       <c r="I24">
-        <f>2*S6*D24</f>
-        <v>160</v>
+        <f>3*S6*D24</f>
+        <v>240</v>
       </c>
       <c r="J24">
         <f>2*T6*D24</f>
-        <v>32</v>
+        <v>320</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -2042,11 +2042,11 @@
       </c>
       <c r="S24">
         <f>I24/D24</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="T24">
         <f>J24/D24</f>
-        <v>8</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
@@ -2081,8 +2081,8 @@
         <v>112</v>
       </c>
       <c r="J25">
-        <f>2*T7*D25</f>
-        <v>64</v>
+        <f>2.5*T7*D25</f>
+        <v>800</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="T25">
         <f>J25/D25</f>
-        <v>16</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
@@ -2149,7 +2149,7 @@
       </c>
       <c r="J26">
         <f>2*T8*D26</f>
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="T26">
         <f>J26/D26</f>
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
       </c>
       <c r="J28">
         <f>2*T10*D28</f>
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -2248,7 +2248,7 @@
       </c>
       <c r="T28">
         <f>J28/D28</f>
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
@@ -2283,8 +2283,8 @@
         <v>136</v>
       </c>
       <c r="J29">
-        <f>2*T11*D29</f>
-        <v>96</v>
+        <f>2.5*T11*D29</f>
+        <v>1200</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="T29">
         <f>J29/D29</f>
-        <v>24</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="J30">
         <f>2*T12*D30</f>
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -2383,7 +2383,7 @@
       </c>
       <c r="T30">
         <f>J30/D30</f>
-        <v>6</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
@@ -2598,12 +2598,12 @@
         <v>30</v>
       </c>
       <c r="I38">
-        <f>2.5*S20*D38</f>
-        <v>80</v>
+        <f>3*S20*D38</f>
+        <v>96</v>
       </c>
       <c r="J38">
         <f>2.5*T20*D38</f>
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -2630,11 +2630,11 @@
       </c>
       <c r="S38">
         <f>I38/D38</f>
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="T38">
         <f>J38/D38</f>
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
@@ -2669,8 +2669,8 @@
         <v>70</v>
       </c>
       <c r="J39">
-        <f>2.5*T21*D39</f>
-        <v>40</v>
+        <f>3*T21*D39</f>
+        <v>600</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="T39">
         <f>J39/D39</f>
-        <v>40</v>
+        <v>600</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
@@ -2737,7 +2737,7 @@
       </c>
       <c r="J40">
         <f>2.5*T22*D40</f>
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="T40">
         <f>J40/D40</f>
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
@@ -2800,12 +2800,12 @@
         <v>160</v>
       </c>
       <c r="I42">
-        <f>2.5*S24*D42</f>
-        <v>800</v>
+        <f>3.5*S24*D42</f>
+        <v>1680</v>
       </c>
       <c r="J42">
         <f>2.5*T24*D42</f>
-        <v>160</v>
+        <v>1600</v>
       </c>
       <c r="K42">
         <v>0</v>
@@ -2832,11 +2832,11 @@
       </c>
       <c r="S42">
         <f>I42/D42</f>
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="T42">
         <f>J42/D42</f>
-        <v>20</v>
+        <v>200</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
@@ -2871,8 +2871,8 @@
         <v>560</v>
       </c>
       <c r="J43">
-        <f>2.5*T25*D43</f>
-        <v>320</v>
+        <f>3*T25*D43</f>
+        <v>4800</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="T43">
         <f>J43/D43</f>
-        <v>40</v>
+        <v>600</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="J44">
         <f>2.5*T26*D44</f>
-        <v>120</v>
+        <v>1200</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -2971,7 +2971,7 @@
       </c>
       <c r="T44">
         <f>J44/D44</f>
-        <v>15</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
@@ -3002,12 +3002,12 @@
         <v>120</v>
       </c>
       <c r="I46">
-        <f>2.5*S28*D46</f>
-        <v>720</v>
+        <f>3*S28*D46</f>
+        <v>864</v>
       </c>
       <c r="J46">
         <f>2.5*T28*D46</f>
-        <v>120</v>
+        <v>1200</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -3034,11 +3034,11 @@
       </c>
       <c r="S46">
         <f>I46/D46</f>
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="T46">
         <f>J46/D46</f>
-        <v>15</v>
+        <v>150</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
@@ -3073,8 +3073,8 @@
         <v>680</v>
       </c>
       <c r="J47">
-        <f>2.5*T29*D47</f>
-        <v>480</v>
+        <f>3.5*T29*D47</f>
+        <v>8400</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -3105,7 +3105,7 @@
       </c>
       <c r="T47">
         <f>J47/D47</f>
-        <v>60</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
@@ -3141,7 +3141,7 @@
       </c>
       <c r="J48">
         <f>2.5*T30*D48</f>
-        <v>120</v>
+        <v>1200</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="T48">
         <f>J48/D48</f>
-        <v>15</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -3392,8 +3392,7 @@
         <v>24</v>
       </c>
       <c r="J56">
-        <f>1*D56*T20</f>
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="K56">
         <v>0</v>
@@ -3440,7 +3439,7 @@
         <v>0</v>
       </c>
       <c r="J57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K57">
         <v>0</v>
@@ -3524,16 +3523,16 @@
         <v>350</v>
       </c>
       <c r="H60">
-        <f>R29*D60*0.5</f>
-        <v>160</v>
+        <f>R29*D60*0.25</f>
+        <v>80</v>
       </c>
       <c r="I60">
-        <f>S29*D60</f>
-        <v>680</v>
+        <f>S29*D60*0.65</f>
+        <v>442</v>
       </c>
       <c r="J60">
-        <f>T29*D60*0.75</f>
-        <v>360</v>
+        <f>T29*D60*0.5</f>
+        <v>3000</v>
       </c>
       <c r="K60">
         <v>0</v>
@@ -3573,16 +3572,16 @@
         <v>700</v>
       </c>
       <c r="H61">
-        <f>R47*D61*0.5</f>
-        <v>400</v>
+        <f>R47*D61*0.25</f>
+        <v>200</v>
       </c>
       <c r="I61">
-        <f>S47*D61*0.55</f>
-        <v>935.00000000000011</v>
+        <f>S47*D61*0.3</f>
+        <v>510</v>
       </c>
       <c r="J61">
-        <f>T47*D61*0.5</f>
-        <v>600</v>
+        <f>T47*D61*0.25</f>
+        <v>5250</v>
       </c>
       <c r="K61">
         <v>0</v>
@@ -3622,16 +3621,16 @@
         <v>280</v>
       </c>
       <c r="H62">
-        <f>R29*D60*0.35</f>
-        <v>112</v>
+        <f>R29*D60*0.25</f>
+        <v>80</v>
       </c>
       <c r="I62">
-        <f>S29*D60</f>
-        <v>680</v>
+        <f>S29*D60*0.65</f>
+        <v>442</v>
       </c>
       <c r="J62">
-        <f>T29*D60*0.65</f>
-        <v>312</v>
+        <f>T29*D60*0.45</f>
+        <v>2700</v>
       </c>
       <c r="K62">
         <v>0</v>

</xml_diff>

<commit_message>
Minor tweak in weapons and reimported model
Imported a new Devastation class model in which the superheavy cannon is not ridiculously thin.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="O2">
         <v>0.2</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="O3">
         <v>0.2</v>
@@ -1194,7 +1194,7 @@
         <v>0.5</v>
       </c>
       <c r="N4">
-        <v>0.3</v>
+        <v>0.125</v>
       </c>
       <c r="O4">
         <v>0.3</v>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O6">
         <v>0.3</v>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O7">
         <v>0.3</v>
@@ -1384,7 +1384,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N8">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="O8">
         <v>0.35</v>
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O10">
         <v>0.3</v>
@@ -1510,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O11">
         <v>0.35</v>
@@ -1574,7 +1574,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N12">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="O12">
         <v>0.35</v>
@@ -1825,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O20">
         <v>0.3</v>
@@ -1892,7 +1892,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O21">
         <v>0.3</v>
@@ -1960,7 +1960,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N22">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="O22">
         <v>0.35</v>
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="O24">
         <v>0.35</v>
@@ -2162,7 +2162,7 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="N26">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O26">
         <v>0.4</v>
@@ -2229,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="O28">
         <v>0.35</v>
@@ -2296,7 +2296,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="O29">
         <v>0.45</v>
@@ -2364,7 +2364,7 @@
         <v>0.75</v>
       </c>
       <c r="N30">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O30">
         <v>0.45</v>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="O38">
         <v>0.3</v>
@@ -2682,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
       <c r="O39">
         <v>0.3</v>
@@ -2750,7 +2750,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="N40">
-        <v>0.65</v>
+        <v>0.6</v>
       </c>
       <c r="O40">
         <v>0.35</v>
@@ -2817,7 +2817,7 @@
         <v>0</v>
       </c>
       <c r="N42">
-        <v>0.1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="O42">
         <v>0.4</v>
@@ -2884,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="N43">
-        <v>0.1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="O43">
         <v>0.45</v>
@@ -3019,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="N46">
-        <v>0.1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="O46">
         <v>0.4</v>
@@ -3086,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="N47">
-        <v>0.1</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="O47">
         <v>0.5</v>

</xml_diff>

<commit_message>
Redesigned crew damage system
More or less on a whim.
Now each warhead type has an anti-personnel property, which indicates the probability to incapacitate a crew member. For each successful hit on a ship, the number of crew members hit follows a binomial distrubution over 5 (a global setting) crew members.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="41">
   <si>
     <t>#</t>
   </si>
@@ -138,7 +138,10 @@
     <t>FighterAutoannon</t>
   </si>
   <si>
-    <t>Vs. strike craft</t>
+    <t>Anti personnel</t>
+  </si>
+  <si>
+    <t>Anti strike craft</t>
   </si>
 </sst>
 </file>
@@ -945,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T62"/>
+  <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59:O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,15 +962,16 @@
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1008,25 +1012,28 @@
         <v>35</v>
       </c>
       <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1070,26 +1077,29 @@
         <v>0.1</v>
       </c>
       <c r="O2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P2">
         <v>0.2</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <f>F2/D2</f>
         <v>20</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <f>H2/D2</f>
         <v>6</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <f>I2/D2</f>
         <v>16</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <f>J2/D2</f>
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1133,26 +1143,29 @@
         <v>0.1</v>
       </c>
       <c r="O3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="P3">
         <v>0.2</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <f>F3/D3</f>
         <v>30</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <f>H3/D3</f>
         <v>10</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <f>I3/D3</f>
         <v>14</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <f>J3/D3</f>
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1190,33 +1203,36 @@
         <v>1</v>
       </c>
       <c r="M4">
-        <f>O4/0.3*0.5</f>
+        <f>P4/0.3*0.5</f>
         <v>0.5</v>
       </c>
       <c r="N4">
         <v>0.125</v>
       </c>
       <c r="O4">
+        <v>0.1</v>
+      </c>
+      <c r="P4">
         <v>0.3</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <f>F4/D4</f>
         <v>40</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <f>H4/D4</f>
         <v>6</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <f>I4/D4</f>
         <v>16</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <f>J4/D4</f>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1260,26 +1276,29 @@
         <v>0.1</v>
       </c>
       <c r="O6">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P6">
         <v>0.3</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f>F6/D6</f>
         <v>30</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f>H6/D6</f>
         <v>4</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <f>I6/D6</f>
         <v>20</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <f>J6/D6</f>
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1323,26 +1342,29 @@
         <v>0.1</v>
       </c>
       <c r="O7">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P7">
         <v>0.3</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f>F7/D7</f>
         <v>40</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f>H7/D7</f>
         <v>6</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <f>I7/D7</f>
         <v>14</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <f>J7/D7</f>
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1380,33 +1402,36 @@
         <v>1</v>
       </c>
       <c r="M8">
-        <f>O8/0.3*0.5</f>
+        <f>P8/0.3*0.5</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="N8">
         <v>0.2</v>
       </c>
       <c r="O8">
+        <v>0.18</v>
+      </c>
+      <c r="P8">
         <v>0.35</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <f>F8/D8</f>
         <v>45</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <f>H8/D8</f>
         <v>3</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <f>I8/D8</f>
         <v>15</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <f>J8/D8</f>
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1450,26 +1475,29 @@
         <v>0.1</v>
       </c>
       <c r="O10">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P10">
         <v>0.3</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <f>F10/D10</f>
         <v>25</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <f>H10/D10</f>
         <v>3</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <f>I10/D10</f>
         <v>18</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <f>J10/D10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1513,26 +1541,29 @@
         <v>0.1</v>
       </c>
       <c r="O11">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P11">
         <v>0.35</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <f>F11/D11</f>
         <v>50</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f>H11/D11</f>
         <v>8</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <f>I11/D11</f>
         <v>17</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <f>J11/D11</f>
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1570,33 +1601,36 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <f>O12/0.3*0.5</f>
+        <f>P12/0.3*0.5</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="N12">
         <v>0.2</v>
       </c>
       <c r="O12">
+        <v>0.22</v>
+      </c>
+      <c r="P12">
         <v>0.35</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <f>F12/D12</f>
         <v>60</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f>H12/D12</f>
         <v>3</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <f>I12/D12</f>
         <v>17.5</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <f>J12/D12</f>
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1630,8 +1664,11 @@
       <c r="L14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1665,8 +1702,11 @@
       <c r="L15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1700,8 +1740,11 @@
       <c r="L16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1735,8 +1778,11 @@
       <c r="L17">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1774,13 +1820,16 @@
         <v>35</v>
       </c>
       <c r="N19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" t="s">
         <v>39</v>
       </c>
-      <c r="O19" t="s">
+      <c r="P19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1797,22 +1846,22 @@
         <v>12</v>
       </c>
       <c r="F20">
-        <f>2*Q2*D20</f>
+        <f>2*R2*D20</f>
         <v>30</v>
       </c>
       <c r="G20">
         <v>155</v>
       </c>
       <c r="H20">
-        <f>2*R2*D20</f>
+        <f>2*S2*D20</f>
         <v>9</v>
       </c>
       <c r="I20">
-        <f>2*S2*D20</f>
+        <f>2*T2*D20</f>
         <v>24</v>
       </c>
       <c r="J20">
-        <f>2*T2*D20</f>
+        <f>2*U2*D20</f>
         <v>60</v>
       </c>
       <c r="K20">
@@ -1828,26 +1877,29 @@
         <v>0.1</v>
       </c>
       <c r="O20">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P20">
         <v>0.3</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <f>F20/D20</f>
         <v>40</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <f>H20/D20</f>
         <v>12</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <f>I20/D20</f>
         <v>32</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <f>J20/D20</f>
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1864,22 +1916,22 @@
         <v>13</v>
       </c>
       <c r="F21">
-        <f>2*Q3*D21</f>
+        <f>2*R3*D21</f>
         <v>45</v>
       </c>
       <c r="G21">
         <v>140</v>
       </c>
       <c r="H21">
-        <f>2*R3*D21</f>
+        <f>2*S3*D21</f>
         <v>15</v>
       </c>
       <c r="I21">
-        <f>2*S3*D21</f>
+        <f>2*T3*D21</f>
         <v>21</v>
       </c>
       <c r="J21">
-        <f>2.5*T3*D21</f>
+        <f>2.5*U3*D21</f>
         <v>150</v>
       </c>
       <c r="K21">
@@ -1895,26 +1947,29 @@
         <v>0.1</v>
       </c>
       <c r="O21">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="P21">
         <v>0.3</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <f>F21/D21</f>
         <v>60</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <f>H21/D21</f>
         <v>20</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <f>I21/D21</f>
         <v>28</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <f>J21/D21</f>
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1931,22 +1986,22 @@
         <v>14</v>
       </c>
       <c r="F22">
-        <f>2*Q4*D22</f>
+        <f>2*R4*D22</f>
         <v>60</v>
       </c>
       <c r="G22">
         <v>50</v>
       </c>
       <c r="H22">
-        <f>2*R4*D22</f>
+        <f>2*S4*D22</f>
         <v>9</v>
       </c>
       <c r="I22">
-        <f>2*S4*D22</f>
+        <f>2*T4*D22</f>
         <v>24</v>
       </c>
       <c r="J22">
-        <f>2*T4*D22</f>
+        <f>2*U4*D22</f>
         <v>30</v>
       </c>
       <c r="K22">
@@ -1956,33 +2011,36 @@
         <v>1</v>
       </c>
       <c r="M22">
-        <f>O22/0.3*0.5</f>
+        <f>P22/0.3*0.5</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="N22">
         <v>0.3</v>
       </c>
       <c r="O22">
+        <v>0.25</v>
+      </c>
+      <c r="P22">
         <v>0.35</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <f>F22/D22</f>
         <v>80</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <f>H22/D22</f>
         <v>12</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <f>I22/D22</f>
         <v>32</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <f>J22/D22</f>
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1999,22 +2057,22 @@
         <v>12</v>
       </c>
       <c r="F24">
-        <f>2*Q6*D24</f>
+        <f>2*R6*D24</f>
         <v>240</v>
       </c>
       <c r="G24">
         <v>500</v>
       </c>
       <c r="H24">
-        <f>2*R6*D24</f>
+        <f>2*S6*D24</f>
         <v>32</v>
       </c>
       <c r="I24">
-        <f>3*S6*D24</f>
+        <f>3*T6*D24</f>
         <v>240</v>
       </c>
       <c r="J24">
-        <f>2*T6*D24</f>
+        <f>2*U6*D24</f>
         <v>320</v>
       </c>
       <c r="K24">
@@ -2030,26 +2088,29 @@
         <v>0.1</v>
       </c>
       <c r="O24">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="P24">
         <v>0.35</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <f>F24/D24</f>
         <v>60</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <f>H24/D24</f>
         <v>8</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <f>I24/D24</f>
         <v>60</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <f>J24/D24</f>
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2066,22 +2127,22 @@
         <v>13</v>
       </c>
       <c r="F25">
-        <f>2*Q7*D25</f>
+        <f>2*R7*D25</f>
         <v>320</v>
       </c>
       <c r="G25">
         <v>280</v>
       </c>
       <c r="H25">
-        <f>2*R7*D25</f>
+        <f>2*S7*D25</f>
         <v>48</v>
       </c>
       <c r="I25">
-        <f>2*S7*D25</f>
+        <f>2*T7*D25</f>
         <v>112</v>
       </c>
       <c r="J25">
-        <f>2.5*T7*D25</f>
+        <f>2.5*U7*D25</f>
         <v>800</v>
       </c>
       <c r="K25">
@@ -2097,26 +2158,29 @@
         <v>0.15</v>
       </c>
       <c r="O25">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P25">
         <v>0.35</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <f>F25/D25</f>
         <v>80</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <f>H25/D25</f>
         <v>12</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <f>I25/D25</f>
         <v>28</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <f>J25/D25</f>
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2133,22 +2197,22 @@
         <v>14</v>
       </c>
       <c r="F26">
-        <f>2*Q8*D26</f>
+        <f>2*R8*D26</f>
         <v>360</v>
       </c>
       <c r="G26">
         <v>100</v>
       </c>
       <c r="H26">
-        <f>2*R8*D26</f>
+        <f>2*S8*D26</f>
         <v>24</v>
       </c>
       <c r="I26">
-        <f>2*S8*D26</f>
+        <f>2*T8*D26</f>
         <v>120</v>
       </c>
       <c r="J26">
-        <f>2*T8*D26</f>
+        <f>2*U8*D26</f>
         <v>240</v>
       </c>
       <c r="K26">
@@ -2158,33 +2222,36 @@
         <v>1</v>
       </c>
       <c r="M26">
-        <f>O26/0.3*0.5</f>
+        <f>P26/0.3*0.5</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="N26">
         <v>0.4</v>
       </c>
       <c r="O26">
+        <v>0.3</v>
+      </c>
+      <c r="P26">
         <v>0.4</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <f>F26/D26</f>
         <v>90</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <f>H26/D26</f>
         <v>6</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <f>I26/D26</f>
         <v>30</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <f>J26/D26</f>
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2201,22 +2268,22 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <f>2*Q10*D28</f>
+        <f>2*R10*D28</f>
         <v>200</v>
       </c>
       <c r="G28">
         <v>380</v>
       </c>
       <c r="H28">
-        <f>2*R10*D28</f>
+        <f>2*S10*D28</f>
         <v>24</v>
       </c>
       <c r="I28">
-        <f>2*S10*D28</f>
+        <f>2*T10*D28</f>
         <v>144</v>
       </c>
       <c r="J28">
-        <f>2*T10*D28</f>
+        <f>2*U10*D28</f>
         <v>240</v>
       </c>
       <c r="K28">
@@ -2232,26 +2299,29 @@
         <v>0.1</v>
       </c>
       <c r="O28">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P28">
         <v>0.35</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <f>F28/D28</f>
         <v>50</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <f>H28/D28</f>
         <v>6</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <f>I28/D28</f>
         <v>36</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <f>J28/D28</f>
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2268,22 +2338,22 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <f>2*Q11*D29</f>
+        <f>2*R11*D29</f>
         <v>400</v>
       </c>
       <c r="G29">
         <v>350</v>
       </c>
       <c r="H29">
-        <f>2*R11*D29</f>
+        <f>2*S11*D29</f>
         <v>64</v>
       </c>
       <c r="I29">
-        <f>2*S11*D29</f>
+        <f>2*T11*D29</f>
         <v>136</v>
       </c>
       <c r="J29">
-        <f>2.5*T11*D29</f>
+        <f>2.5*U11*D29</f>
         <v>1200</v>
       </c>
       <c r="K29">
@@ -2299,26 +2369,29 @@
         <v>0.1</v>
       </c>
       <c r="O29">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="P29">
         <v>0.45</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <f>F29/D29</f>
         <v>100</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <f>H29/D29</f>
         <v>16</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <f>I29/D29</f>
         <v>34</v>
       </c>
-      <c r="T29">
+      <c r="U29">
         <f>J29/D29</f>
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2335,22 +2408,22 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <f>2*Q12*D30</f>
+        <f>2*R12*D30</f>
         <v>480</v>
       </c>
       <c r="G30">
         <v>130</v>
       </c>
       <c r="H30">
-        <f>2*R12*D30</f>
+        <f>2*S12*D30</f>
         <v>24</v>
       </c>
       <c r="I30">
-        <f>2*S12*D30</f>
+        <f>2*T12*D30</f>
         <v>140</v>
       </c>
       <c r="J30">
-        <f>2*T12*D30</f>
+        <f>2*U12*D30</f>
         <v>240</v>
       </c>
       <c r="K30">
@@ -2360,33 +2433,36 @@
         <v>1</v>
       </c>
       <c r="M30">
-        <f>O30/0.3*0.5</f>
+        <f>P30/0.3*0.5</f>
         <v>0.75</v>
       </c>
       <c r="N30">
         <v>0.4</v>
       </c>
       <c r="O30">
+        <v>0.4</v>
+      </c>
+      <c r="P30">
         <v>0.45</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <f>F30/D30</f>
         <v>120</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <f>H30/D30</f>
         <v>6</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <f>I30/D30</f>
         <v>35</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <f>J30/D30</f>
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2420,8 +2496,11 @@
       <c r="L32" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2455,8 +2534,11 @@
       <c r="L33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2490,8 +2572,11 @@
       <c r="L34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2525,8 +2610,11 @@
       <c r="L35">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2564,13 +2652,16 @@
         <v>35</v>
       </c>
       <c r="N37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O37" t="s">
         <v>39</v>
       </c>
-      <c r="O37" t="s">
+      <c r="P37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2587,22 +2678,22 @@
         <v>12</v>
       </c>
       <c r="F38">
-        <f>2.5*Q20*D38</f>
+        <f>2.5*R20*D38</f>
         <v>100</v>
       </c>
       <c r="G38">
         <v>270</v>
       </c>
       <c r="H38">
-        <f>2.5*R20*D38</f>
+        <f>2.5*S20*D38</f>
         <v>30</v>
       </c>
       <c r="I38">
-        <f>3*S20*D38</f>
+        <f>3*T20*D38</f>
         <v>96</v>
       </c>
       <c r="J38">
-        <f>2.5*T20*D38</f>
+        <f>2.5*U20*D38</f>
         <v>200</v>
       </c>
       <c r="K38">
@@ -2618,26 +2709,29 @@
         <v>0.05</v>
       </c>
       <c r="O38">
+        <v>0.03</v>
+      </c>
+      <c r="P38">
         <v>0.3</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <f>F38/D38</f>
         <v>100</v>
       </c>
-      <c r="R38">
+      <c r="S38">
         <f>H38/D38</f>
         <v>30</v>
       </c>
-      <c r="S38">
+      <c r="T38">
         <f>I38/D38</f>
         <v>96</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <f>J38/D38</f>
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2654,22 +2748,22 @@
         <v>13</v>
       </c>
       <c r="F39">
-        <f>2.5*Q21*D39</f>
+        <f>2.5*R21*D39</f>
         <v>150</v>
       </c>
       <c r="G39">
         <v>250</v>
       </c>
       <c r="H39">
-        <f>2.5*R21*D39</f>
+        <f>2.5*S21*D39</f>
         <v>50</v>
       </c>
       <c r="I39">
-        <f>2.5*S21*D39</f>
+        <f>2.5*T21*D39</f>
         <v>70</v>
       </c>
       <c r="J39">
-        <f>3*T21*D39</f>
+        <f>3*U21*D39</f>
         <v>600</v>
       </c>
       <c r="K39">
@@ -2685,26 +2779,29 @@
         <v>0.05</v>
       </c>
       <c r="O39">
+        <v>0.03</v>
+      </c>
+      <c r="P39">
         <v>0.3</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <f>F39/D39</f>
         <v>150</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <f>H39/D39</f>
         <v>50</v>
       </c>
-      <c r="S39">
+      <c r="T39">
         <f>I39/D39</f>
         <v>70</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <f>J39/D39</f>
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2721,22 +2818,22 @@
         <v>14</v>
       </c>
       <c r="F40">
-        <f>2.5*Q22*D40</f>
+        <f>2.5*R22*D40</f>
         <v>200</v>
       </c>
       <c r="G40">
         <v>100</v>
       </c>
       <c r="H40">
-        <f>2.5*R22*D40</f>
+        <f>2.5*S22*D40</f>
         <v>30</v>
       </c>
       <c r="I40">
-        <f>2.5*S22*D40</f>
+        <f>2.5*T22*D40</f>
         <v>80</v>
       </c>
       <c r="J40">
-        <f>2.5*T22*D40</f>
+        <f>2.5*U22*D40</f>
         <v>100</v>
       </c>
       <c r="K40">
@@ -2746,33 +2843,36 @@
         <v>1</v>
       </c>
       <c r="M40">
-        <f>O40/0.3*0.25</f>
+        <f>P40/0.3*0.25</f>
         <v>0.29166666666666669</v>
       </c>
       <c r="N40">
         <v>0.6</v>
       </c>
       <c r="O40">
+        <v>0.4</v>
+      </c>
+      <c r="P40">
         <v>0.35</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <f>F40/D40</f>
         <v>200</v>
       </c>
-      <c r="R40">
+      <c r="S40">
         <f>H40/D40</f>
         <v>30</v>
       </c>
-      <c r="S40">
+      <c r="T40">
         <f>I40/D40</f>
         <v>80</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <f>J40/D40</f>
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2789,22 +2889,22 @@
         <v>12</v>
       </c>
       <c r="F42">
-        <f>2.5*Q24*D42</f>
+        <f>2.5*R24*D42</f>
         <v>1200</v>
       </c>
       <c r="G42">
         <v>1000</v>
       </c>
       <c r="H42">
-        <f>2.5*R24*D42</f>
+        <f>2.5*S24*D42</f>
         <v>160</v>
       </c>
       <c r="I42">
-        <f>3.5*S24*D42</f>
+        <f>3.5*T24*D42</f>
         <v>1680</v>
       </c>
       <c r="J42">
-        <f>2.5*T24*D42</f>
+        <f>2.5*U24*D42</f>
         <v>1600</v>
       </c>
       <c r="K42">
@@ -2820,26 +2920,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="O42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P42">
         <v>0.4</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <f>F42/D42</f>
         <v>150</v>
       </c>
-      <c r="R42">
+      <c r="S42">
         <f>H42/D42</f>
         <v>20</v>
       </c>
-      <c r="S42">
+      <c r="T42">
         <f>I42/D42</f>
         <v>210</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <f>J42/D42</f>
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2856,22 +2959,22 @@
         <v>13</v>
       </c>
       <c r="F43">
-        <f>2.5*Q25*D43</f>
+        <f>2.5*R25*D43</f>
         <v>1600</v>
       </c>
       <c r="G43">
         <v>600</v>
       </c>
       <c r="H43">
-        <f>2.5*R25*D43</f>
+        <f>2.5*S25*D43</f>
         <v>240</v>
       </c>
       <c r="I43">
-        <f>2.5*S25*D43</f>
+        <f>2.5*T25*D43</f>
         <v>560</v>
       </c>
       <c r="J43">
-        <f>3*T25*D43</f>
+        <f>3*U25*D43</f>
         <v>4800</v>
       </c>
       <c r="K43">
@@ -2887,26 +2990,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="O43">
+        <v>0.05</v>
+      </c>
+      <c r="P43">
         <v>0.45</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <f>F43/D43</f>
         <v>200</v>
       </c>
-      <c r="R43">
+      <c r="S43">
         <f>H43/D43</f>
         <v>30</v>
       </c>
-      <c r="S43">
+      <c r="T43">
         <f>I43/D43</f>
         <v>70</v>
       </c>
-      <c r="T43">
+      <c r="U43">
         <f>J43/D43</f>
         <v>600</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -2923,22 +3029,22 @@
         <v>14</v>
       </c>
       <c r="F44">
-        <f>2.5*Q26*D44</f>
+        <f>2.5*R26*D44</f>
         <v>1800</v>
       </c>
       <c r="G44">
         <v>160</v>
       </c>
       <c r="H44">
-        <f>2.5*R26*D44</f>
+        <f>2.5*S26*D44</f>
         <v>120</v>
       </c>
       <c r="I44">
-        <f>2.5*S26*D44</f>
+        <f>2.5*T26*D44</f>
         <v>600</v>
       </c>
       <c r="J44">
-        <f>2.5*T26*D44</f>
+        <f>2.5*U26*D44</f>
         <v>1200</v>
       </c>
       <c r="K44">
@@ -2948,33 +3054,36 @@
         <v>1</v>
       </c>
       <c r="M44">
-        <f>O44/0.3*0.25</f>
+        <f>P44/0.3*0.25</f>
         <v>0.41666666666666669</v>
       </c>
       <c r="N44">
         <v>0.75</v>
       </c>
       <c r="O44">
+        <v>0.6</v>
+      </c>
+      <c r="P44">
         <v>0.5</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <f>F44/D44</f>
         <v>225</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <f>H44/D44</f>
         <v>15</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <f>I44/D44</f>
         <v>75</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <f>J44/D44</f>
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -2991,22 +3100,22 @@
         <v>12</v>
       </c>
       <c r="F46">
-        <f>2.5*Q28*D46</f>
+        <f>2.5*R28*D46</f>
         <v>1000</v>
       </c>
       <c r="G46">
         <v>770</v>
       </c>
       <c r="H46">
-        <f>2.5*R28*D46</f>
+        <f>2.5*S28*D46</f>
         <v>120</v>
       </c>
       <c r="I46">
-        <f>3*S28*D46</f>
+        <f>3*T28*D46</f>
         <v>864</v>
       </c>
       <c r="J46">
-        <f>2.5*T28*D46</f>
+        <f>2.5*U28*D46</f>
         <v>1200</v>
       </c>
       <c r="K46">
@@ -3022,26 +3131,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="O46">
+        <v>0.05</v>
+      </c>
+      <c r="P46">
         <v>0.4</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
         <f>F46/D46</f>
         <v>125</v>
       </c>
-      <c r="R46">
+      <c r="S46">
         <f>H46/D46</f>
         <v>15</v>
       </c>
-      <c r="S46">
+      <c r="T46">
         <f>I46/D46</f>
         <v>108</v>
       </c>
-      <c r="T46">
+      <c r="U46">
         <f>J46/D46</f>
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -3058,22 +3170,22 @@
         <v>13</v>
       </c>
       <c r="F47">
-        <f>2.5*Q29*D47</f>
+        <f>2.5*R29*D47</f>
         <v>2000</v>
       </c>
       <c r="G47">
         <v>700</v>
       </c>
       <c r="H47">
-        <f>2.5*R29*D47</f>
+        <f>2.5*S29*D47</f>
         <v>320</v>
       </c>
       <c r="I47">
-        <f>2.5*S29*D47</f>
+        <f>2.5*T29*D47</f>
         <v>680</v>
       </c>
       <c r="J47">
-        <f>3.5*T29*D47</f>
+        <f>3.5*U29*D47</f>
         <v>8400</v>
       </c>
       <c r="K47">
@@ -3089,26 +3201,29 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="O47">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P47">
         <v>0.5</v>
       </c>
-      <c r="Q47">
+      <c r="R47">
         <f>F47/D47</f>
         <v>250</v>
       </c>
-      <c r="R47">
+      <c r="S47">
         <f>H47/D47</f>
         <v>40</v>
       </c>
-      <c r="S47">
+      <c r="T47">
         <f>I47/D47</f>
         <v>85</v>
       </c>
-      <c r="T47">
+      <c r="U47">
         <f>J47/D47</f>
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -3125,22 +3240,22 @@
         <v>14</v>
       </c>
       <c r="F48">
-        <f>2.5*Q30*D48</f>
+        <f>2.5*R30*D48</f>
         <v>2400</v>
       </c>
       <c r="G48">
         <v>180</v>
       </c>
       <c r="H48">
-        <f>2.5*R30*D48</f>
+        <f>2.5*S30*D48</f>
         <v>120</v>
       </c>
       <c r="I48">
-        <f>2.5*S30*D48</f>
+        <f>2.5*T30*D48</f>
         <v>700</v>
       </c>
       <c r="J48">
-        <f>2.5*T30*D48</f>
+        <f>2.5*U30*D48</f>
         <v>1200</v>
       </c>
       <c r="K48">
@@ -3150,33 +3265,36 @@
         <v>1</v>
       </c>
       <c r="M48">
-        <f>O48/0.3*0.25</f>
+        <f>P48/0.3*0.25</f>
         <v>0.45833333333333337</v>
       </c>
       <c r="N48">
         <v>0.75</v>
       </c>
       <c r="O48">
+        <v>0.8</v>
+      </c>
+      <c r="P48">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q48">
+      <c r="R48">
         <f>F48/D48</f>
         <v>300</v>
       </c>
-      <c r="R48">
+      <c r="S48">
         <f>H48/D48</f>
         <v>15</v>
       </c>
-      <c r="S48">
+      <c r="T48">
         <f>I48/D48</f>
         <v>87.5</v>
       </c>
-      <c r="T48">
+      <c r="U48">
         <f>J48/D48</f>
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -3210,8 +3328,11 @@
       <c r="L50" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3245,8 +3366,11 @@
       <c r="L51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M51">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3280,8 +3404,11 @@
       <c r="L52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3315,8 +3442,11 @@
       <c r="L53">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M53">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -3354,13 +3484,16 @@
         <v>35</v>
       </c>
       <c r="N55" t="s">
+        <v>40</v>
+      </c>
+      <c r="O55" t="s">
         <v>39</v>
       </c>
-      <c r="O55" t="s">
+      <c r="P55" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3377,18 +3510,18 @@
         <v>12</v>
       </c>
       <c r="F56">
-        <f>1*D56*Q20</f>
+        <f>1*D56*R20</f>
         <v>30</v>
       </c>
       <c r="G56">
         <v>175</v>
       </c>
       <c r="H56">
-        <f>1*D56*R20</f>
+        <f>1*D56*S20</f>
         <v>9</v>
       </c>
       <c r="I56">
-        <f>1*D56*S20</f>
+        <f>1*D56*T20</f>
         <v>24</v>
       </c>
       <c r="J56">
@@ -3407,10 +3540,13 @@
         <v>1</v>
       </c>
       <c r="O56">
+        <v>0.03</v>
+      </c>
+      <c r="P56">
         <v>0.15</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -3454,10 +3590,13 @@
         <v>0.65</v>
       </c>
       <c r="O57">
+        <v>0</v>
+      </c>
+      <c r="P57">
         <v>0.1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -3492,13 +3631,16 @@
         <v>31</v>
       </c>
       <c r="M59" t="s">
+        <v>39</v>
+      </c>
+      <c r="N59" t="s">
         <v>27</v>
       </c>
-      <c r="N59" t="s">
+      <c r="O59" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -3515,7 +3657,7 @@
         <v>26</v>
       </c>
       <c r="F60">
-        <f>Q28*D60*0.25</f>
+        <f>R28*D60*0.25</f>
         <v>250</v>
       </c>
       <c r="G60">
@@ -3523,15 +3665,15 @@
         <v>350</v>
       </c>
       <c r="H60">
-        <f>R29*D60*0.25</f>
+        <f>S29*D60*0.25</f>
         <v>80</v>
       </c>
       <c r="I60">
-        <f>S29*D60*0.65</f>
+        <f>T29*D60*0.65</f>
         <v>442</v>
       </c>
       <c r="J60">
-        <f>T29*D60*0.5</f>
+        <f>U29*D60*0.5</f>
         <v>3000</v>
       </c>
       <c r="K60">
@@ -3541,13 +3683,16 @@
         <v>2</v>
       </c>
       <c r="M60">
+        <v>0.5</v>
+      </c>
+      <c r="N60">
         <v>0.22500000000000001</v>
       </c>
-      <c r="N60">
+      <c r="O60">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -3564,7 +3709,7 @@
         <v>15</v>
       </c>
       <c r="F61">
-        <f>Q38*D61*0.25</f>
+        <f>R38*D61*0.25</f>
         <v>500</v>
       </c>
       <c r="G61">
@@ -3572,15 +3717,15 @@
         <v>700</v>
       </c>
       <c r="H61">
-        <f>R47*D61*0.25</f>
+        <f>S47*D61*0.25</f>
         <v>200</v>
       </c>
       <c r="I61">
-        <f>S47*D61*0.3</f>
+        <f>T47*D61*0.3</f>
         <v>510</v>
       </c>
       <c r="J61">
-        <f>T47*D61*0.25</f>
+        <f>U47*D61*0.25</f>
         <v>5250</v>
       </c>
       <c r="K61">
@@ -3590,13 +3735,16 @@
         <v>3</v>
       </c>
       <c r="M61">
+        <v>0.6</v>
+      </c>
+      <c r="N61">
         <v>0.25</v>
       </c>
-      <c r="N61">
+      <c r="O61">
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -3613,7 +3761,7 @@
         <v>19</v>
       </c>
       <c r="F62">
-        <f>Q28*D62*0.25</f>
+        <f>R28*D62*0.25</f>
         <v>250</v>
       </c>
       <c r="G62">
@@ -3621,15 +3769,15 @@
         <v>280</v>
       </c>
       <c r="H62">
-        <f>R29*D60*0.25</f>
+        <f>S29*D60*0.25</f>
         <v>80</v>
       </c>
       <c r="I62">
-        <f>S29*D60*0.65</f>
+        <f>T29*D60*0.65</f>
         <v>442</v>
       </c>
       <c r="J62">
-        <f>T29*D60*0.45</f>
+        <f>U29*D60*0.45</f>
         <v>2700</v>
       </c>
       <c r="K62">
@@ -3639,9 +3787,12 @@
         <v>2</v>
       </c>
       <c r="M62">
+        <v>0.4</v>
+      </c>
+      <c r="N62">
         <v>0.22500000000000001</v>
       </c>
-      <c r="N62">
+      <c r="O62">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Converted key lookup system for turrets and weapons from enums to strings
This will allow greater flexibility for adding new turrets and weapons only via the YAML loading system, without changing the code. The disadvantage of this is losing the "error-proofing" that enums give.
Gun turrets are set up correctly, as well as the Monitor, Richmond, and Cochrane classes. Torpedo tubes and strike craft still need testing. Other ships classes need configuring.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -142,6 +142,27 @@
   </si>
   <si>
     <t>Anti strike craft</t>
+  </si>
+  <si>
+    <t>WeaponEffectAssetBundle</t>
+  </si>
+  <si>
+    <t>AssetBundles\StandaloneWindows\effects</t>
+  </si>
+  <si>
+    <t>WeaponEffectObj</t>
+  </si>
+  <si>
+    <t>BulletImpactMetalEffect no Decal</t>
+  </si>
+  <si>
+    <t>SmallExplosionEffect</t>
+  </si>
+  <si>
+    <t>FlakSmallExplosionEffect</t>
+  </si>
+  <si>
+    <t>PlasmaExplosionEffect</t>
   </si>
 </sst>
 </file>
@@ -948,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U62"/>
+  <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F49" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59:O62"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,15 +984,16 @@
     <col min="12" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1020,20 +1042,26 @@
       <c r="P1" t="s">
         <v>27</v>
       </c>
+      <c r="Q1" t="s">
+        <v>41</v>
+      </c>
       <c r="R1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1082,24 +1110,30 @@
       <c r="P2">
         <v>0.2</v>
       </c>
-      <c r="R2">
+      <c r="Q2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2">
         <f>F2/D2</f>
         <v>20</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <f>H2/D2</f>
         <v>6</v>
       </c>
-      <c r="T2">
+      <c r="V2">
         <f>I2/D2</f>
         <v>16</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <f>J2/D2</f>
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1148,24 +1182,30 @@
       <c r="P3">
         <v>0.2</v>
       </c>
-      <c r="R3">
+      <c r="Q3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3">
         <f>F3/D3</f>
         <v>30</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <f>H3/D3</f>
         <v>10</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <f>I3/D3</f>
         <v>14</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <f>J3/D3</f>
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1215,24 +1255,30 @@
       <c r="P4">
         <v>0.3</v>
       </c>
-      <c r="R4">
+      <c r="Q4" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4">
         <f>F4/D4</f>
         <v>40</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <f>H4/D4</f>
         <v>6</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <f>I4/D4</f>
         <v>16</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <f>J4/D4</f>
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1281,24 +1327,30 @@
       <c r="P6">
         <v>0.3</v>
       </c>
-      <c r="R6">
+      <c r="Q6" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6">
         <f>F6/D6</f>
         <v>30</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <f>H6/D6</f>
         <v>4</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <f>I6/D6</f>
         <v>20</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <f>J6/D6</f>
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1347,24 +1399,30 @@
       <c r="P7">
         <v>0.3</v>
       </c>
-      <c r="R7">
+      <c r="Q7" t="s">
+        <v>42</v>
+      </c>
+      <c r="R7" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7">
         <f>F7/D7</f>
         <v>40</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <f>H7/D7</f>
         <v>6</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <f>I7/D7</f>
         <v>14</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <f>J7/D7</f>
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1414,24 +1472,30 @@
       <c r="P8">
         <v>0.35</v>
       </c>
-      <c r="R8">
+      <c r="Q8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" t="s">
+        <v>46</v>
+      </c>
+      <c r="T8">
         <f>F8/D8</f>
         <v>45</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <f>H8/D8</f>
         <v>3</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <f>I8/D8</f>
         <v>15</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <f>J8/D8</f>
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1480,24 +1544,30 @@
       <c r="P10">
         <v>0.3</v>
       </c>
-      <c r="R10">
+      <c r="Q10" t="s">
+        <v>42</v>
+      </c>
+      <c r="R10" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10">
         <f>F10/D10</f>
         <v>25</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <f>H10/D10</f>
         <v>3</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <f>I10/D10</f>
         <v>18</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <f>J10/D10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1546,24 +1616,30 @@
       <c r="P11">
         <v>0.35</v>
       </c>
-      <c r="R11">
+      <c r="Q11" t="s">
+        <v>42</v>
+      </c>
+      <c r="R11" t="s">
+        <v>45</v>
+      </c>
+      <c r="T11">
         <f>F11/D11</f>
         <v>50</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <f>H11/D11</f>
         <v>8</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <f>I11/D11</f>
         <v>17</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <f>J11/D11</f>
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1613,24 +1689,30 @@
       <c r="P12">
         <v>0.35</v>
       </c>
-      <c r="R12">
+      <c r="Q12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R12" t="s">
+        <v>46</v>
+      </c>
+      <c r="T12">
         <f>F12/D12</f>
         <v>60</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <f>H12/D12</f>
         <v>3</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <f>I12/D12</f>
         <v>17.5</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <f>J12/D12</f>
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1667,8 +1749,11 @@
       <c r="M14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1706,7 +1791,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1744,7 +1829,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1781,8 +1866,14 @@
       <c r="M17">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N17" t="s">
+        <v>42</v>
+      </c>
+      <c r="P17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1828,8 +1919,14 @@
       <c r="P19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>41</v>
+      </c>
+      <c r="R19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -1846,22 +1943,22 @@
         <v>12</v>
       </c>
       <c r="F20">
-        <f>2*R2*D20</f>
+        <f>2*T2*D20</f>
         <v>30</v>
       </c>
       <c r="G20">
         <v>155</v>
       </c>
       <c r="H20">
-        <f>2*S2*D20</f>
+        <f>2*U2*D20</f>
         <v>9</v>
       </c>
       <c r="I20">
-        <f>2*T2*D20</f>
+        <f>2*V2*D20</f>
         <v>24</v>
       </c>
       <c r="J20">
-        <f>2*U2*D20</f>
+        <f>2*W2*D20</f>
         <v>60</v>
       </c>
       <c r="K20">
@@ -1882,24 +1979,30 @@
       <c r="P20">
         <v>0.3</v>
       </c>
-      <c r="R20">
+      <c r="Q20" t="s">
+        <v>42</v>
+      </c>
+      <c r="R20" t="s">
+        <v>44</v>
+      </c>
+      <c r="T20">
         <f>F20/D20</f>
         <v>40</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <f>H20/D20</f>
         <v>12</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <f>I20/D20</f>
         <v>32</v>
       </c>
-      <c r="U20">
+      <c r="W20">
         <f>J20/D20</f>
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -1916,22 +2019,22 @@
         <v>13</v>
       </c>
       <c r="F21">
-        <f>2*R3*D21</f>
+        <f>2*T3*D21</f>
         <v>45</v>
       </c>
       <c r="G21">
         <v>140</v>
       </c>
       <c r="H21">
-        <f>2*S3*D21</f>
+        <f>2*U3*D21</f>
         <v>15</v>
       </c>
       <c r="I21">
-        <f>2*T3*D21</f>
+        <f>2*V3*D21</f>
         <v>21</v>
       </c>
       <c r="J21">
-        <f>2.5*U3*D21</f>
+        <f>2.5*W3*D21</f>
         <v>150</v>
       </c>
       <c r="K21">
@@ -1952,24 +2055,30 @@
       <c r="P21">
         <v>0.3</v>
       </c>
-      <c r="R21">
+      <c r="Q21" t="s">
+        <v>42</v>
+      </c>
+      <c r="R21" t="s">
+        <v>45</v>
+      </c>
+      <c r="T21">
         <f>F21/D21</f>
         <v>60</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <f>H21/D21</f>
         <v>20</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <f>I21/D21</f>
         <v>28</v>
       </c>
-      <c r="U21">
+      <c r="W21">
         <f>J21/D21</f>
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -1986,22 +2095,22 @@
         <v>14</v>
       </c>
       <c r="F22">
-        <f>2*R4*D22</f>
+        <f>2*T4*D22</f>
         <v>60</v>
       </c>
       <c r="G22">
         <v>50</v>
       </c>
       <c r="H22">
-        <f>2*S4*D22</f>
+        <f>2*U4*D22</f>
         <v>9</v>
       </c>
       <c r="I22">
-        <f>2*T4*D22</f>
+        <f>2*V4*D22</f>
         <v>24</v>
       </c>
       <c r="J22">
-        <f>2*U4*D22</f>
+        <f>2*W4*D22</f>
         <v>30</v>
       </c>
       <c r="K22">
@@ -2023,24 +2132,30 @@
       <c r="P22">
         <v>0.35</v>
       </c>
-      <c r="R22">
+      <c r="Q22" t="s">
+        <v>42</v>
+      </c>
+      <c r="R22" t="s">
+        <v>46</v>
+      </c>
+      <c r="T22">
         <f>F22/D22</f>
         <v>80</v>
       </c>
-      <c r="S22">
+      <c r="U22">
         <f>H22/D22</f>
         <v>12</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <f>I22/D22</f>
         <v>32</v>
       </c>
-      <c r="U22">
+      <c r="W22">
         <f>J22/D22</f>
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2057,22 +2172,22 @@
         <v>12</v>
       </c>
       <c r="F24">
-        <f>2*R6*D24</f>
+        <f>2*T6*D24</f>
         <v>240</v>
       </c>
       <c r="G24">
         <v>500</v>
       </c>
       <c r="H24">
-        <f>2*S6*D24</f>
+        <f>2*U6*D24</f>
         <v>32</v>
       </c>
       <c r="I24">
-        <f>3*T6*D24</f>
+        <f>3*V6*D24</f>
         <v>240</v>
       </c>
       <c r="J24">
-        <f>2*U6*D24</f>
+        <f>2*W6*D24</f>
         <v>320</v>
       </c>
       <c r="K24">
@@ -2093,24 +2208,30 @@
       <c r="P24">
         <v>0.35</v>
       </c>
-      <c r="R24">
+      <c r="Q24" t="s">
+        <v>42</v>
+      </c>
+      <c r="R24" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24">
         <f>F24/D24</f>
         <v>60</v>
       </c>
-      <c r="S24">
+      <c r="U24">
         <f>H24/D24</f>
         <v>8</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <f>I24/D24</f>
         <v>60</v>
       </c>
-      <c r="U24">
+      <c r="W24">
         <f>J24/D24</f>
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2127,22 +2248,22 @@
         <v>13</v>
       </c>
       <c r="F25">
-        <f>2*R7*D25</f>
+        <f>2*T7*D25</f>
         <v>320</v>
       </c>
       <c r="G25">
         <v>280</v>
       </c>
       <c r="H25">
-        <f>2*S7*D25</f>
+        <f>2*U7*D25</f>
         <v>48</v>
       </c>
       <c r="I25">
-        <f>2*T7*D25</f>
+        <f>2*V7*D25</f>
         <v>112</v>
       </c>
       <c r="J25">
-        <f>2.5*U7*D25</f>
+        <f>2.5*W7*D25</f>
         <v>800</v>
       </c>
       <c r="K25">
@@ -2163,24 +2284,30 @@
       <c r="P25">
         <v>0.35</v>
       </c>
-      <c r="R25">
+      <c r="Q25" t="s">
+        <v>42</v>
+      </c>
+      <c r="R25" t="s">
+        <v>45</v>
+      </c>
+      <c r="T25">
         <f>F25/D25</f>
         <v>80</v>
       </c>
-      <c r="S25">
+      <c r="U25">
         <f>H25/D25</f>
         <v>12</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <f>I25/D25</f>
         <v>28</v>
       </c>
-      <c r="U25">
+      <c r="W25">
         <f>J25/D25</f>
         <v>200</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2197,22 +2324,22 @@
         <v>14</v>
       </c>
       <c r="F26">
-        <f>2*R8*D26</f>
+        <f>2*T8*D26</f>
         <v>360</v>
       </c>
       <c r="G26">
         <v>100</v>
       </c>
       <c r="H26">
-        <f>2*S8*D26</f>
+        <f>2*U8*D26</f>
         <v>24</v>
       </c>
       <c r="I26">
-        <f>2*T8*D26</f>
+        <f>2*V8*D26</f>
         <v>120</v>
       </c>
       <c r="J26">
-        <f>2*U8*D26</f>
+        <f>2*W8*D26</f>
         <v>240</v>
       </c>
       <c r="K26">
@@ -2234,24 +2361,30 @@
       <c r="P26">
         <v>0.4</v>
       </c>
-      <c r="R26">
+      <c r="Q26" t="s">
+        <v>42</v>
+      </c>
+      <c r="R26" t="s">
+        <v>46</v>
+      </c>
+      <c r="T26">
         <f>F26/D26</f>
         <v>90</v>
       </c>
-      <c r="S26">
+      <c r="U26">
         <f>H26/D26</f>
         <v>6</v>
       </c>
-      <c r="T26">
+      <c r="V26">
         <f>I26/D26</f>
         <v>30</v>
       </c>
-      <c r="U26">
+      <c r="W26">
         <f>J26/D26</f>
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2268,22 +2401,22 @@
         <v>12</v>
       </c>
       <c r="F28">
-        <f>2*R10*D28</f>
+        <f>2*T10*D28</f>
         <v>200</v>
       </c>
       <c r="G28">
         <v>380</v>
       </c>
       <c r="H28">
-        <f>2*S10*D28</f>
+        <f>2*U10*D28</f>
         <v>24</v>
       </c>
       <c r="I28">
-        <f>2*T10*D28</f>
+        <f>2*V10*D28</f>
         <v>144</v>
       </c>
       <c r="J28">
-        <f>2*U10*D28</f>
+        <f>2*W10*D28</f>
         <v>240</v>
       </c>
       <c r="K28">
@@ -2304,24 +2437,30 @@
       <c r="P28">
         <v>0.35</v>
       </c>
-      <c r="R28">
+      <c r="Q28" t="s">
+        <v>42</v>
+      </c>
+      <c r="R28" t="s">
+        <v>44</v>
+      </c>
+      <c r="T28">
         <f>F28/D28</f>
         <v>50</v>
       </c>
-      <c r="S28">
+      <c r="U28">
         <f>H28/D28</f>
         <v>6</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <f>I28/D28</f>
         <v>36</v>
       </c>
-      <c r="U28">
+      <c r="W28">
         <f>J28/D28</f>
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2338,22 +2477,22 @@
         <v>13</v>
       </c>
       <c r="F29">
-        <f>2*R11*D29</f>
+        <f>2*T11*D29</f>
         <v>400</v>
       </c>
       <c r="G29">
         <v>350</v>
       </c>
       <c r="H29">
-        <f>2*S11*D29</f>
+        <f>2*U11*D29</f>
         <v>64</v>
       </c>
       <c r="I29">
-        <f>2*T11*D29</f>
+        <f>2*V11*D29</f>
         <v>136</v>
       </c>
       <c r="J29">
-        <f>2.5*U11*D29</f>
+        <f>2.5*W11*D29</f>
         <v>1200</v>
       </c>
       <c r="K29">
@@ -2374,24 +2513,30 @@
       <c r="P29">
         <v>0.45</v>
       </c>
-      <c r="R29">
+      <c r="Q29" t="s">
+        <v>42</v>
+      </c>
+      <c r="R29" t="s">
+        <v>45</v>
+      </c>
+      <c r="T29">
         <f>F29/D29</f>
         <v>100</v>
       </c>
-      <c r="S29">
+      <c r="U29">
         <f>H29/D29</f>
         <v>16</v>
       </c>
-      <c r="T29">
+      <c r="V29">
         <f>I29/D29</f>
         <v>34</v>
       </c>
-      <c r="U29">
+      <c r="W29">
         <f>J29/D29</f>
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2408,22 +2553,22 @@
         <v>14</v>
       </c>
       <c r="F30">
-        <f>2*R12*D30</f>
+        <f>2*T12*D30</f>
         <v>480</v>
       </c>
       <c r="G30">
         <v>130</v>
       </c>
       <c r="H30">
-        <f>2*S12*D30</f>
+        <f>2*U12*D30</f>
         <v>24</v>
       </c>
       <c r="I30">
-        <f>2*T12*D30</f>
+        <f>2*V12*D30</f>
         <v>140</v>
       </c>
       <c r="J30">
-        <f>2*U12*D30</f>
+        <f>2*W12*D30</f>
         <v>240</v>
       </c>
       <c r="K30">
@@ -2445,24 +2590,30 @@
       <c r="P30">
         <v>0.45</v>
       </c>
-      <c r="R30">
+      <c r="Q30" t="s">
+        <v>42</v>
+      </c>
+      <c r="R30" t="s">
+        <v>46</v>
+      </c>
+      <c r="T30">
         <f>F30/D30</f>
         <v>120</v>
       </c>
-      <c r="S30">
+      <c r="U30">
         <f>H30/D30</f>
         <v>6</v>
       </c>
-      <c r="T30">
+      <c r="V30">
         <f>I30/D30</f>
         <v>35</v>
       </c>
-      <c r="U30">
+      <c r="W30">
         <f>J30/D30</f>
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2499,8 +2650,14 @@
       <c r="M32" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N32" t="s">
+        <v>41</v>
+      </c>
+      <c r="P32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2538,7 +2695,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2576,7 +2733,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -2613,8 +2770,14 @@
       <c r="M35">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>42</v>
+      </c>
+      <c r="P35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2660,8 +2823,14 @@
       <c r="P37" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q37" t="s">
+        <v>41</v>
+      </c>
+      <c r="R37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -2678,22 +2847,22 @@
         <v>12</v>
       </c>
       <c r="F38">
-        <f>2.5*R20*D38</f>
+        <f>2.5*T20*D38</f>
         <v>100</v>
       </c>
       <c r="G38">
         <v>270</v>
       </c>
       <c r="H38">
-        <f>2.5*S20*D38</f>
+        <f>2.5*U20*D38</f>
         <v>30</v>
       </c>
       <c r="I38">
-        <f>3*T20*D38</f>
+        <f>3*V20*D38</f>
         <v>96</v>
       </c>
       <c r="J38">
-        <f>2.5*U20*D38</f>
+        <f>2.5*W20*D38</f>
         <v>200</v>
       </c>
       <c r="K38">
@@ -2714,24 +2883,30 @@
       <c r="P38">
         <v>0.3</v>
       </c>
-      <c r="R38">
+      <c r="Q38" t="s">
+        <v>42</v>
+      </c>
+      <c r="R38" t="s">
+        <v>44</v>
+      </c>
+      <c r="T38">
         <f>F38/D38</f>
         <v>100</v>
       </c>
-      <c r="S38">
+      <c r="U38">
         <f>H38/D38</f>
         <v>30</v>
       </c>
-      <c r="T38">
+      <c r="V38">
         <f>I38/D38</f>
         <v>96</v>
       </c>
-      <c r="U38">
+      <c r="W38">
         <f>J38/D38</f>
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -2748,22 +2923,22 @@
         <v>13</v>
       </c>
       <c r="F39">
-        <f>2.5*R21*D39</f>
+        <f>2.5*T21*D39</f>
         <v>150</v>
       </c>
       <c r="G39">
         <v>250</v>
       </c>
       <c r="H39">
-        <f>2.5*S21*D39</f>
+        <f>2.5*U21*D39</f>
         <v>50</v>
       </c>
       <c r="I39">
-        <f>2.5*T21*D39</f>
+        <f>2.5*V21*D39</f>
         <v>70</v>
       </c>
       <c r="J39">
-        <f>3*U21*D39</f>
+        <f>3*W21*D39</f>
         <v>600</v>
       </c>
       <c r="K39">
@@ -2784,24 +2959,30 @@
       <c r="P39">
         <v>0.3</v>
       </c>
-      <c r="R39">
+      <c r="Q39" t="s">
+        <v>42</v>
+      </c>
+      <c r="R39" t="s">
+        <v>45</v>
+      </c>
+      <c r="T39">
         <f>F39/D39</f>
         <v>150</v>
       </c>
-      <c r="S39">
+      <c r="U39">
         <f>H39/D39</f>
         <v>50</v>
       </c>
-      <c r="T39">
+      <c r="V39">
         <f>I39/D39</f>
         <v>70</v>
       </c>
-      <c r="U39">
+      <c r="W39">
         <f>J39/D39</f>
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2818,22 +2999,22 @@
         <v>14</v>
       </c>
       <c r="F40">
-        <f>2.5*R22*D40</f>
+        <f>2.5*T22*D40</f>
         <v>200</v>
       </c>
       <c r="G40">
         <v>100</v>
       </c>
       <c r="H40">
-        <f>2.5*S22*D40</f>
+        <f>2.5*U22*D40</f>
         <v>30</v>
       </c>
       <c r="I40">
-        <f>2.5*T22*D40</f>
+        <f>2.5*V22*D40</f>
         <v>80</v>
       </c>
       <c r="J40">
-        <f>2.5*U22*D40</f>
+        <f>2.5*W22*D40</f>
         <v>100</v>
       </c>
       <c r="K40">
@@ -2855,24 +3036,30 @@
       <c r="P40">
         <v>0.35</v>
       </c>
-      <c r="R40">
+      <c r="Q40" t="s">
+        <v>42</v>
+      </c>
+      <c r="R40" t="s">
+        <v>46</v>
+      </c>
+      <c r="T40">
         <f>F40/D40</f>
         <v>200</v>
       </c>
-      <c r="S40">
+      <c r="U40">
         <f>H40/D40</f>
         <v>30</v>
       </c>
-      <c r="T40">
+      <c r="V40">
         <f>I40/D40</f>
         <v>80</v>
       </c>
-      <c r="U40">
+      <c r="W40">
         <f>J40/D40</f>
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2889,22 +3076,22 @@
         <v>12</v>
       </c>
       <c r="F42">
-        <f>2.5*R24*D42</f>
+        <f>2.5*T24*D42</f>
         <v>1200</v>
       </c>
       <c r="G42">
         <v>1000</v>
       </c>
       <c r="H42">
-        <f>2.5*S24*D42</f>
+        <f>2.5*U24*D42</f>
         <v>160</v>
       </c>
       <c r="I42">
-        <f>3.5*T24*D42</f>
+        <f>3.5*V24*D42</f>
         <v>1680</v>
       </c>
       <c r="J42">
-        <f>2.5*U24*D42</f>
+        <f>2.5*W24*D42</f>
         <v>1600</v>
       </c>
       <c r="K42">
@@ -2925,24 +3112,30 @@
       <c r="P42">
         <v>0.4</v>
       </c>
-      <c r="R42">
+      <c r="Q42" t="s">
+        <v>42</v>
+      </c>
+      <c r="R42" t="s">
+        <v>44</v>
+      </c>
+      <c r="T42">
         <f>F42/D42</f>
         <v>150</v>
       </c>
-      <c r="S42">
+      <c r="U42">
         <f>H42/D42</f>
         <v>20</v>
       </c>
-      <c r="T42">
+      <c r="V42">
         <f>I42/D42</f>
         <v>210</v>
       </c>
-      <c r="U42">
+      <c r="W42">
         <f>J42/D42</f>
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -2959,22 +3152,22 @@
         <v>13</v>
       </c>
       <c r="F43">
-        <f>2.5*R25*D43</f>
+        <f>2.5*T25*D43</f>
         <v>1600</v>
       </c>
       <c r="G43">
         <v>600</v>
       </c>
       <c r="H43">
-        <f>2.5*S25*D43</f>
+        <f>2.5*U25*D43</f>
         <v>240</v>
       </c>
       <c r="I43">
-        <f>2.5*T25*D43</f>
+        <f>2.5*V25*D43</f>
         <v>560</v>
       </c>
       <c r="J43">
-        <f>3*U25*D43</f>
+        <f>3*W25*D43</f>
         <v>4800</v>
       </c>
       <c r="K43">
@@ -2995,24 +3188,30 @@
       <c r="P43">
         <v>0.45</v>
       </c>
-      <c r="R43">
+      <c r="Q43" t="s">
+        <v>42</v>
+      </c>
+      <c r="R43" t="s">
+        <v>45</v>
+      </c>
+      <c r="T43">
         <f>F43/D43</f>
         <v>200</v>
       </c>
-      <c r="S43">
+      <c r="U43">
         <f>H43/D43</f>
         <v>30</v>
       </c>
-      <c r="T43">
+      <c r="V43">
         <f>I43/D43</f>
         <v>70</v>
       </c>
-      <c r="U43">
+      <c r="W43">
         <f>J43/D43</f>
         <v>600</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -3029,22 +3228,22 @@
         <v>14</v>
       </c>
       <c r="F44">
-        <f>2.5*R26*D44</f>
+        <f>2.5*T26*D44</f>
         <v>1800</v>
       </c>
       <c r="G44">
         <v>160</v>
       </c>
       <c r="H44">
-        <f>2.5*S26*D44</f>
+        <f>2.5*U26*D44</f>
         <v>120</v>
       </c>
       <c r="I44">
-        <f>2.5*T26*D44</f>
+        <f>2.5*V26*D44</f>
         <v>600</v>
       </c>
       <c r="J44">
-        <f>2.5*U26*D44</f>
+        <f>2.5*W26*D44</f>
         <v>1200</v>
       </c>
       <c r="K44">
@@ -3066,24 +3265,30 @@
       <c r="P44">
         <v>0.5</v>
       </c>
-      <c r="R44">
+      <c r="Q44" t="s">
+        <v>42</v>
+      </c>
+      <c r="R44" t="s">
+        <v>46</v>
+      </c>
+      <c r="T44">
         <f>F44/D44</f>
         <v>225</v>
       </c>
-      <c r="S44">
+      <c r="U44">
         <f>H44/D44</f>
         <v>15</v>
       </c>
-      <c r="T44">
+      <c r="V44">
         <f>I44/D44</f>
         <v>75</v>
       </c>
-      <c r="U44">
+      <c r="W44">
         <f>J44/D44</f>
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -3100,22 +3305,22 @@
         <v>12</v>
       </c>
       <c r="F46">
-        <f>2.5*R28*D46</f>
+        <f>2.5*T28*D46</f>
         <v>1000</v>
       </c>
       <c r="G46">
         <v>770</v>
       </c>
       <c r="H46">
-        <f>2.5*S28*D46</f>
+        <f>2.5*U28*D46</f>
         <v>120</v>
       </c>
       <c r="I46">
-        <f>3*T28*D46</f>
+        <f>3*V28*D46</f>
         <v>864</v>
       </c>
       <c r="J46">
-        <f>2.5*U28*D46</f>
+        <f>2.5*W28*D46</f>
         <v>1200</v>
       </c>
       <c r="K46">
@@ -3136,24 +3341,30 @@
       <c r="P46">
         <v>0.4</v>
       </c>
-      <c r="R46">
+      <c r="Q46" t="s">
+        <v>42</v>
+      </c>
+      <c r="R46" t="s">
+        <v>44</v>
+      </c>
+      <c r="T46">
         <f>F46/D46</f>
         <v>125</v>
       </c>
-      <c r="S46">
+      <c r="U46">
         <f>H46/D46</f>
         <v>15</v>
       </c>
-      <c r="T46">
+      <c r="V46">
         <f>I46/D46</f>
         <v>108</v>
       </c>
-      <c r="U46">
+      <c r="W46">
         <f>J46/D46</f>
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -3170,22 +3381,22 @@
         <v>13</v>
       </c>
       <c r="F47">
-        <f>2.5*R29*D47</f>
+        <f>2.5*T29*D47</f>
         <v>2000</v>
       </c>
       <c r="G47">
         <v>700</v>
       </c>
       <c r="H47">
-        <f>2.5*S29*D47</f>
+        <f>2.5*U29*D47</f>
         <v>320</v>
       </c>
       <c r="I47">
-        <f>2.5*T29*D47</f>
+        <f>2.5*V29*D47</f>
         <v>680</v>
       </c>
       <c r="J47">
-        <f>3.5*U29*D47</f>
+        <f>3.5*W29*D47</f>
         <v>8400</v>
       </c>
       <c r="K47">
@@ -3206,24 +3417,30 @@
       <c r="P47">
         <v>0.5</v>
       </c>
-      <c r="R47">
+      <c r="Q47" t="s">
+        <v>42</v>
+      </c>
+      <c r="R47" t="s">
+        <v>45</v>
+      </c>
+      <c r="T47">
         <f>F47/D47</f>
         <v>250</v>
       </c>
-      <c r="S47">
+      <c r="U47">
         <f>H47/D47</f>
         <v>40</v>
       </c>
-      <c r="T47">
+      <c r="V47">
         <f>I47/D47</f>
         <v>85</v>
       </c>
-      <c r="U47">
+      <c r="W47">
         <f>J47/D47</f>
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -3240,22 +3457,22 @@
         <v>14</v>
       </c>
       <c r="F48">
-        <f>2.5*R30*D48</f>
+        <f>2.5*T30*D48</f>
         <v>2400</v>
       </c>
       <c r="G48">
         <v>180</v>
       </c>
       <c r="H48">
-        <f>2.5*S30*D48</f>
+        <f>2.5*U30*D48</f>
         <v>120</v>
       </c>
       <c r="I48">
-        <f>2.5*T30*D48</f>
+        <f>2.5*V30*D48</f>
         <v>700</v>
       </c>
       <c r="J48">
-        <f>2.5*U30*D48</f>
+        <f>2.5*W30*D48</f>
         <v>1200</v>
       </c>
       <c r="K48">
@@ -3277,24 +3494,30 @@
       <c r="P48">
         <v>0.55000000000000004</v>
       </c>
-      <c r="R48">
+      <c r="Q48" t="s">
+        <v>42</v>
+      </c>
+      <c r="R48" t="s">
+        <v>46</v>
+      </c>
+      <c r="T48">
         <f>F48/D48</f>
         <v>300</v>
       </c>
-      <c r="S48">
+      <c r="U48">
         <f>H48/D48</f>
         <v>15</v>
       </c>
-      <c r="T48">
+      <c r="V48">
         <f>I48/D48</f>
         <v>87.5</v>
       </c>
-      <c r="U48">
+      <c r="W48">
         <f>J48/D48</f>
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -3331,8 +3554,14 @@
       <c r="M50" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>41</v>
+      </c>
+      <c r="P50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3370,7 +3599,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -3408,7 +3637,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -3445,8 +3674,14 @@
       <c r="M53">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N53" t="s">
+        <v>42</v>
+      </c>
+      <c r="P53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -3492,8 +3727,14 @@
       <c r="P55" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q55" t="s">
+        <v>41</v>
+      </c>
+      <c r="R55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3510,18 +3751,18 @@
         <v>12</v>
       </c>
       <c r="F56">
-        <f>1*D56*R20</f>
+        <f>1*D56*T20</f>
         <v>30</v>
       </c>
       <c r="G56">
         <v>175</v>
       </c>
       <c r="H56">
-        <f>1*D56*S20</f>
+        <f>1*D56*U20</f>
         <v>9</v>
       </c>
       <c r="I56">
-        <f>1*D56*T20</f>
+        <f>1*D56*V20</f>
         <v>24</v>
       </c>
       <c r="J56">
@@ -3545,8 +3786,14 @@
       <c r="P56">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q56" t="s">
+        <v>42</v>
+      </c>
+      <c r="R56" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>3</v>
       </c>
@@ -3595,8 +3842,14 @@
       <c r="P57">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q57" t="s">
+        <v>42</v>
+      </c>
+      <c r="R57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -3639,8 +3892,14 @@
       <c r="O59" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P59" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -3657,7 +3916,7 @@
         <v>26</v>
       </c>
       <c r="F60">
-        <f>R28*D60*0.25</f>
+        <f>T28*D60*0.25</f>
         <v>250</v>
       </c>
       <c r="G60">
@@ -3665,15 +3924,15 @@
         <v>350</v>
       </c>
       <c r="H60">
-        <f>S29*D60*0.25</f>
+        <f>U29*D60*0.25</f>
         <v>80</v>
       </c>
       <c r="I60">
-        <f>T29*D60*0.65</f>
+        <f>V29*D60*0.65</f>
         <v>442</v>
       </c>
       <c r="J60">
-        <f>U29*D60*0.5</f>
+        <f>W29*D60*0.5</f>
         <v>3000</v>
       </c>
       <c r="K60">
@@ -3691,8 +3950,14 @@
       <c r="O60">
         <v>5</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P60" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -3709,7 +3974,7 @@
         <v>15</v>
       </c>
       <c r="F61">
-        <f>R38*D61*0.25</f>
+        <f>T38*D61*0.25</f>
         <v>500</v>
       </c>
       <c r="G61">
@@ -3717,15 +3982,15 @@
         <v>700</v>
       </c>
       <c r="H61">
-        <f>S47*D61*0.25</f>
+        <f>U47*D61*0.25</f>
         <v>200</v>
       </c>
       <c r="I61">
-        <f>T47*D61*0.3</f>
+        <f>V47*D61*0.3</f>
         <v>510</v>
       </c>
       <c r="J61">
-        <f>U47*D61*0.25</f>
+        <f>W47*D61*0.25</f>
         <v>5250</v>
       </c>
       <c r="K61">
@@ -3743,8 +4008,14 @@
       <c r="O61">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P61" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -3761,7 +4032,7 @@
         <v>19</v>
       </c>
       <c r="F62">
-        <f>R28*D62*0.25</f>
+        <f>T28*D62*0.25</f>
         <v>250</v>
       </c>
       <c r="G62">
@@ -3769,15 +4040,15 @@
         <v>280</v>
       </c>
       <c r="H62">
-        <f>S29*D60*0.25</f>
+        <f>U29*D60*0.25</f>
         <v>80</v>
       </c>
       <c r="I62">
-        <f>T29*D60*0.65</f>
+        <f>V29*D60*0.65</f>
         <v>442</v>
       </c>
       <c r="J62">
-        <f>U29*D60*0.45</f>
+        <f>W29*D60*0.45</f>
         <v>2700</v>
       </c>
       <c r="K62">
@@ -3794,6 +4065,12 @@
       </c>
       <c r="O62">
         <v>6</v>
+      </c>
+      <c r="P62" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjustments to strike craft and torpedo-type weapons for using strings as keys
1. Ship torpedo tubes are loaded from a YAML file
2. All strike craft weapons are loaded from YAML files. These include the fighter autocannons the fighter main cannon, the bomber autocannon, and the bomber torpedoes.
3. Adjusted default priorities file to new torpedo lookup.
4. Exported strike craft to an asset bundle. This was necessary because the torpedo bomber turret model is part of the strike craft fbx file, not the guns file.
5. Updated Chickasaw, Sachsen, Aurora, and Arminius classes to have string slot lists.
6. Fixed numerous typos that caused stuff to fail.
7. Discovered bug in torpedo bomber formations: if one torpedo bomber runs out of ammo before the others spawn, it will try to return to host. Will need to address this.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -135,9 +135,6 @@
     <t>FighterCannon</t>
   </si>
   <si>
-    <t>FighterAutoannon</t>
-  </si>
-  <si>
     <t>Anti personnel</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
   </si>
   <si>
     <t>PlasmaExplosionEffect</t>
+  </si>
+  <si>
+    <t>FighterAutocannon</t>
   </si>
 </sst>
 </file>
@@ -971,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,19 +1034,19 @@
         <v>35</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P1" t="s">
         <v>27</v>
       </c>
       <c r="Q1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T1" t="s">
         <v>22</v>
@@ -1111,10 +1111,10 @@
         <v>0.2</v>
       </c>
       <c r="Q2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T2">
         <f>F2/D2</f>
@@ -1183,10 +1183,10 @@
         <v>0.2</v>
       </c>
       <c r="Q3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T3">
         <f>F3/D3</f>
@@ -1256,10 +1256,10 @@
         <v>0.3</v>
       </c>
       <c r="Q4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T4">
         <f>F4/D4</f>
@@ -1328,10 +1328,10 @@
         <v>0.3</v>
       </c>
       <c r="Q6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T6">
         <f>F6/D6</f>
@@ -1400,10 +1400,10 @@
         <v>0.3</v>
       </c>
       <c r="Q7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T7">
         <f>F7/D7</f>
@@ -1473,10 +1473,10 @@
         <v>0.35</v>
       </c>
       <c r="Q8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T8">
         <f>F8/D8</f>
@@ -1545,10 +1545,10 @@
         <v>0.3</v>
       </c>
       <c r="Q10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T10">
         <f>F10/D10</f>
@@ -1617,10 +1617,10 @@
         <v>0.35</v>
       </c>
       <c r="Q11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T11">
         <f>F11/D11</f>
@@ -1690,10 +1690,10 @@
         <v>0.35</v>
       </c>
       <c r="Q12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T12">
         <f>F12/D12</f>
@@ -1747,10 +1747,10 @@
         <v>27</v>
       </c>
       <c r="M14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1867,10 +1867,10 @@
         <v>0.2</v>
       </c>
       <c r="N17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -1911,19 +1911,19 @@
         <v>35</v>
       </c>
       <c r="N19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P19" t="s">
         <v>27</v>
       </c>
       <c r="Q19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -1980,10 +1980,10 @@
         <v>0.3</v>
       </c>
       <c r="Q20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T20">
         <f>F20/D20</f>
@@ -2056,10 +2056,10 @@
         <v>0.3</v>
       </c>
       <c r="Q21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T21">
         <f>F21/D21</f>
@@ -2133,10 +2133,10 @@
         <v>0.35</v>
       </c>
       <c r="Q22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T22">
         <f>F22/D22</f>
@@ -2209,10 +2209,10 @@
         <v>0.35</v>
       </c>
       <c r="Q24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T24">
         <f>F24/D24</f>
@@ -2285,10 +2285,10 @@
         <v>0.35</v>
       </c>
       <c r="Q25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T25">
         <f>F25/D25</f>
@@ -2362,10 +2362,10 @@
         <v>0.4</v>
       </c>
       <c r="Q26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T26">
         <f>F26/D26</f>
@@ -2438,10 +2438,10 @@
         <v>0.35</v>
       </c>
       <c r="Q28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T28">
         <f>F28/D28</f>
@@ -2514,10 +2514,10 @@
         <v>0.45</v>
       </c>
       <c r="Q29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T29">
         <f>F29/D29</f>
@@ -2591,10 +2591,10 @@
         <v>0.45</v>
       </c>
       <c r="Q30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T30">
         <f>F30/D30</f>
@@ -2648,13 +2648,13 @@
         <v>27</v>
       </c>
       <c r="M32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -2771,10 +2771,10 @@
         <v>0.35</v>
       </c>
       <c r="N35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -2815,19 +2815,19 @@
         <v>35</v>
       </c>
       <c r="N37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P37" t="s">
         <v>27</v>
       </c>
       <c r="Q37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -2884,10 +2884,10 @@
         <v>0.3</v>
       </c>
       <c r="Q38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T38">
         <f>F38/D38</f>
@@ -2960,10 +2960,10 @@
         <v>0.3</v>
       </c>
       <c r="Q39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T39">
         <f>F39/D39</f>
@@ -3037,10 +3037,10 @@
         <v>0.35</v>
       </c>
       <c r="Q40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T40">
         <f>F40/D40</f>
@@ -3113,10 +3113,10 @@
         <v>0.4</v>
       </c>
       <c r="Q42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T42">
         <f>F42/D42</f>
@@ -3189,10 +3189,10 @@
         <v>0.45</v>
       </c>
       <c r="Q43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T43">
         <f>F43/D43</f>
@@ -3266,10 +3266,10 @@
         <v>0.5</v>
       </c>
       <c r="Q44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T44">
         <f>F44/D44</f>
@@ -3342,10 +3342,10 @@
         <v>0.4</v>
       </c>
       <c r="Q46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T46">
         <f>F46/D46</f>
@@ -3418,10 +3418,10 @@
         <v>0.5</v>
       </c>
       <c r="Q47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T47">
         <f>F47/D47</f>
@@ -3495,10 +3495,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="Q48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T48">
         <f>F48/D48</f>
@@ -3552,13 +3552,13 @@
         <v>27</v>
       </c>
       <c r="M50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
@@ -3675,10 +3675,10 @@
         <v>0.75</v>
       </c>
       <c r="N53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -3719,19 +3719,19 @@
         <v>35</v>
       </c>
       <c r="N55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P55" t="s">
         <v>27</v>
       </c>
       <c r="Q55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -3787,10 +3787,10 @@
         <v>0.15</v>
       </c>
       <c r="Q56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -3801,7 +3801,7 @@
         <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D57">
         <v>0.5</v>
@@ -3843,10 +3843,10 @@
         <v>0.1</v>
       </c>
       <c r="Q57" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -3884,7 +3884,7 @@
         <v>31</v>
       </c>
       <c r="M59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N59" t="s">
         <v>27</v>
@@ -3893,10 +3893,10 @@
         <v>28</v>
       </c>
       <c r="P59" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
@@ -3951,10 +3951,10 @@
         <v>5</v>
       </c>
       <c r="P60" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -4009,10 +4009,10 @@
         <v>9</v>
       </c>
       <c r="P61" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
@@ -4067,10 +4067,10 @@
         <v>6</v>
       </c>
       <c r="P62" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q62" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started implementing dragging items in ship editor
Ship editor now adds markers on the weapon hardpoints of each ship.
Weapons can be dragged, but since weapons do not have a size yet, they can't be assigned to valid hardpoints.
Fixed scrollbars in ship editor.
Also created an awesome looking lightning particle system that isn't used anywhere.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -1,20 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sosin\Documents\Privateer\TextData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\Privateer\TextData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD88E0-B534-42EA-91F0-FC5994A1E0F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Warheads" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -168,7 +179,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -968,11 +979,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O2">
         <v>1.4999999999999999E-2</v>
@@ -1175,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O3">
         <v>1.4999999999999999E-2</v>
@@ -1248,7 +1259,7 @@
         <v>0.5</v>
       </c>
       <c r="N4">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="O4">
         <v>0.1</v>
@@ -1320,7 +1331,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O6">
         <v>1.7000000000000001E-2</v>
@@ -1392,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O7">
         <v>1.7000000000000001E-2</v>
@@ -1465,7 +1476,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N8">
-        <v>0.2</v>
+        <v>0.125</v>
       </c>
       <c r="O8">
         <v>0.18</v>
@@ -1537,7 +1548,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O10">
         <v>1.7000000000000001E-2</v>
@@ -1609,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O11">
         <v>1.7000000000000001E-2</v>
@@ -1682,7 +1693,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N12">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="O12">
         <v>0.22</v>
@@ -1972,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O20">
         <v>1.7000000000000001E-2</v>
@@ -2048,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="O21">
         <v>1.7000000000000001E-2</v>
@@ -2125,7 +2136,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N22">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="O22">
         <v>0.25</v>
@@ -2354,7 +2365,7 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="N26">
-        <v>0.4</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="O26">
         <v>0.3</v>
@@ -3029,7 +3040,7 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="N40">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="O40">
         <v>0.4</v>
@@ -3258,7 +3269,7 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="N44">
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="O44">
         <v>0.6</v>

</xml_diff>

<commit_message>
Modified battle test scene to load ship designs from YAML
This replaces the old hard-coded designs.
Also:
1. Gave the project a name and a company name. This is needed to store user data (for now, the ship classes).
2. Modified the periodic component behavior in ships to do heat exchange first, power generation second, and the other components last. This is to maximize the available power / heat budget, making it more predictable for the player.
3. Finished implementing the conversion between the component templates and actual components (which I previosuly forgot), and ship shadow to actual ship.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\Privateer\TextData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BD88E0-B534-42EA-91F0-FC5994A1E0F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A084DCC3-94A9-4054-B0E6-8EC917DCB37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3977,7 +3977,7 @@
         <v>21</v>
       </c>
       <c r="C61">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D61">
         <v>20</v>

</xml_diff>

<commit_message>
Added weapon info panel to ship editor
With icons and all.
The order of the ammo types is now changed from this panel, rather than the main weapons panel.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\Privateer\TextData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A084DCC3-94A9-4054-B0E6-8EC917DCB37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF5195A-E2FC-4868-A416-7FD8A4BE996C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,8 +1472,8 @@
         <v>1</v>
       </c>
       <c r="M8">
-        <f>P8/0.3*0.5</f>
-        <v>0.58333333333333337</v>
+        <f>P8/0.3*0.25</f>
+        <v>0.29166666666666669</v>
       </c>
       <c r="N8">
         <v>0.125</v>
@@ -1689,8 +1689,8 @@
         <v>1</v>
       </c>
       <c r="M12">
-        <f>P12/0.3*0.5</f>
-        <v>0.58333333333333337</v>
+        <f>P12/0.3*0.25</f>
+        <v>0.29166666666666669</v>
       </c>
       <c r="N12">
         <v>0.15</v>
@@ -2132,8 +2132,8 @@
         <v>1</v>
       </c>
       <c r="M22">
-        <f>P22/0.3*0.5</f>
-        <v>0.58333333333333337</v>
+        <f>P22/0.3*0.25</f>
+        <v>0.29166666666666669</v>
       </c>
       <c r="N22">
         <v>0.25</v>
@@ -2361,8 +2361,8 @@
         <v>1</v>
       </c>
       <c r="M26">
-        <f>P26/0.3*0.5</f>
-        <v>0.66666666666666674</v>
+        <f>P26/0.3*0.25</f>
+        <v>0.33333333333333337</v>
       </c>
       <c r="N26">
         <v>0.32500000000000001</v>
@@ -2590,8 +2590,8 @@
         <v>1</v>
       </c>
       <c r="M30">
-        <f>P30/0.3*0.5</f>
-        <v>0.75</v>
+        <f>P30/0.3*0.25</f>
+        <v>0.375</v>
       </c>
       <c r="N30">
         <v>0.4</v>

</xml_diff>

<commit_message>
Minor redesign of the buff system
1. Deleted "static buffs". When they are reimplemented, they will be applied when the ships are created from the shadow objects, rather than on ship intializtion.
2. Turret mods can have special buffs associated with them. They are defined in YAML files. Turret mods can now be applied only on turret creation, and cannot be modified. The effects of the turret mods are applied when the turrets are initialized, and many of the values are pre-computed, to reduce the amount of computations that need to be done during combat.
3. Implemented acceleration booster, fast autoloader, and (partially) advanced targeting mods.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\Privateer\TextData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF5195A-E2FC-4868-A416-7FD8A4BE996C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F93F905-7D7A-4CD8-9663-5B2471FF41B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -983,7 +983,7 @@
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3092,7 +3092,7 @@
         <v>360</v>
       </c>
       <c r="G42">
-        <v>1000</v>
+        <v>850</v>
       </c>
       <c r="H42">
         <f>2.5*U24*D42</f>

</xml_diff>

<commit_message>
Renaming, rebalancing and bug fixes
1. Renamed ammo types
2. Nerfed HV gun damage
3. Added Hermes class fast carrier
4. Fixed bug in carrier modules that support multiple strike craft formations AND have multiple launch points.
5. Fixed bug in ship component repair.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\Privateer\TextData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F93F905-7D7A-4CD8-9663-5B2471FF41B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11874C14-6B83-41A5-9A4A-6DEA447390EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,15 +68,6 @@
     <t>Autocannon</t>
   </si>
   <si>
-    <t>KineticPenetrator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShapedCharge     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ShrapnelRound    </t>
-  </si>
-  <si>
     <t>HVGun</t>
   </si>
   <si>
@@ -174,6 +165,15 @@
   </si>
   <si>
     <t>FighterAutocannon</t>
+  </si>
+  <si>
+    <t>AP round</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HE round     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frag round    </t>
   </si>
 </sst>
 </file>
@@ -983,7 +983,7 @@
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1040,37 +1040,37 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
         <v>35</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>40</v>
-      </c>
-      <c r="R1" t="s">
-        <v>42</v>
-      </c>
       <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
         <v>22</v>
-      </c>
-      <c r="U1" t="s">
-        <v>23</v>
-      </c>
-      <c r="V1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
         <v>0.5</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -1123,10 +1123,10 @@
         <v>0.2</v>
       </c>
       <c r="Q2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T2">
         <f>F2/D2</f>
@@ -1159,7 +1159,7 @@
         <v>0.5</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F3">
         <v>8</v>
@@ -1195,10 +1195,10 @@
         <v>0.2</v>
       </c>
       <c r="Q3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R3" t="s">
         <v>41</v>
-      </c>
-      <c r="R3" t="s">
-        <v>44</v>
       </c>
       <c r="T3">
         <f>F3/D3</f>
@@ -1231,7 +1231,7 @@
         <v>0.5</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -1268,10 +1268,10 @@
         <v>0.3</v>
       </c>
       <c r="Q4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T4">
         <f>F4/D4</f>
@@ -1298,13 +1298,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F6">
         <v>30</v>
@@ -1340,10 +1340,10 @@
         <v>0.3</v>
       </c>
       <c r="Q6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T6">
         <f>F6/D6</f>
@@ -1370,13 +1370,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F7">
         <v>40</v>
@@ -1412,10 +1412,10 @@
         <v>0.3</v>
       </c>
       <c r="Q7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R7" t="s">
         <v>41</v>
-      </c>
-      <c r="R7" t="s">
-        <v>44</v>
       </c>
       <c r="T7">
         <f>F7/D7</f>
@@ -1442,13 +1442,13 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F8">
         <v>45</v>
@@ -1485,10 +1485,10 @@
         <v>0.35</v>
       </c>
       <c r="Q8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T8">
         <f>F8/D8</f>
@@ -1515,13 +1515,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F10">
         <v>25</v>
@@ -1557,10 +1557,10 @@
         <v>0.3</v>
       </c>
       <c r="Q10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T10">
         <f>F10/D10</f>
@@ -1587,13 +1587,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F11">
         <v>45</v>
@@ -1629,10 +1629,10 @@
         <v>0.35</v>
       </c>
       <c r="Q11" t="s">
+        <v>38</v>
+      </c>
+      <c r="R11" t="s">
         <v>41</v>
-      </c>
-      <c r="R11" t="s">
-        <v>44</v>
       </c>
       <c r="T11">
         <f>F11/D11</f>
@@ -1659,13 +1659,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F12">
         <v>50</v>
@@ -1702,10 +1702,10 @@
         <v>0.35</v>
       </c>
       <c r="Q12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T12">
         <f>F12/D12</f>
@@ -1753,16 +1753,16 @@
         <v>9</v>
       </c>
       <c r="K14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -1773,7 +1773,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15">
         <v>25</v>
@@ -1811,7 +1811,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <v>45</v>
@@ -1849,7 +1849,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E17">
         <v>35</v>
@@ -1879,10 +1879,10 @@
         <v>0.2</v>
       </c>
       <c r="N17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
@@ -1917,25 +1917,25 @@
         <v>9</v>
       </c>
       <c r="L19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N19" t="s">
+        <v>36</v>
+      </c>
+      <c r="O19" t="s">
         <v>35</v>
       </c>
-      <c r="N19" t="s">
+      <c r="P19" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>37</v>
+      </c>
+      <c r="R19" t="s">
         <v>39</v>
-      </c>
-      <c r="O19" t="s">
-        <v>38</v>
-      </c>
-      <c r="P19" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>40</v>
-      </c>
-      <c r="R19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
         <v>11</v>
@@ -1952,7 +1952,7 @@
         <v>0.75</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F20">
         <f>1.5*T2*D20</f>
@@ -1992,10 +1992,10 @@
         <v>0.3</v>
       </c>
       <c r="Q20" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T20">
         <f>F20/D20</f>
@@ -2019,7 +2019,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -2028,7 +2028,7 @@
         <v>0.75</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F21">
         <f>1.5*T3*D21</f>
@@ -2046,8 +2046,8 @@
         <v>21</v>
       </c>
       <c r="J21">
-        <f>2.5*W3*D21</f>
-        <v>150</v>
+        <f>2*W3*D21</f>
+        <v>120</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -2068,10 +2068,10 @@
         <v>0.3</v>
       </c>
       <c r="Q21" t="s">
+        <v>38</v>
+      </c>
+      <c r="R21" t="s">
         <v>41</v>
-      </c>
-      <c r="R21" t="s">
-        <v>44</v>
       </c>
       <c r="T21">
         <f>F21/D21</f>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="W21">
         <f>J21/D21</f>
-        <v>200</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -2095,7 +2095,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
         <v>11</v>
@@ -2104,7 +2104,7 @@
         <v>0.75</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F22">
         <f>1.5*T4*D22</f>
@@ -2145,10 +2145,10 @@
         <v>0.35</v>
       </c>
       <c r="Q22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T22">
         <f>F22/D22</f>
@@ -2172,16 +2172,16 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D24">
         <v>4</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F24">
         <f>1.5*T6*D24</f>
@@ -2195,8 +2195,8 @@
         <v>32</v>
       </c>
       <c r="I24">
-        <f>3*V6*D24</f>
-        <v>240</v>
+        <f>1.5*V6*D24</f>
+        <v>120</v>
       </c>
       <c r="J24">
         <f>2*W6*D24</f>
@@ -2221,10 +2221,10 @@
         <v>0.35</v>
       </c>
       <c r="Q24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R24" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T24">
         <f>F24/D24</f>
@@ -2236,7 +2236,7 @@
       </c>
       <c r="V24">
         <f>I24/D24</f>
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="W24">
         <f>J24/D24</f>
@@ -2248,16 +2248,16 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F25">
         <f>1.5*T7*D25</f>
@@ -2275,8 +2275,8 @@
         <v>112</v>
       </c>
       <c r="J25">
-        <f>2.5*W7*D25</f>
-        <v>800</v>
+        <f>2*W7*D25</f>
+        <v>640</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -2297,10 +2297,10 @@
         <v>0.35</v>
       </c>
       <c r="Q25" t="s">
+        <v>38</v>
+      </c>
+      <c r="R25" t="s">
         <v>41</v>
-      </c>
-      <c r="R25" t="s">
-        <v>44</v>
       </c>
       <c r="T25">
         <f>F25/D25</f>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="W25">
         <f>J25/D25</f>
-        <v>200</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -2324,16 +2324,16 @@
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F26">
         <f>1.5*T8*D26</f>
@@ -2374,10 +2374,10 @@
         <v>0.4</v>
       </c>
       <c r="Q26" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T26">
         <f>F26/D26</f>
@@ -2401,16 +2401,16 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D28">
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F28">
         <f>1.5*T10*D28</f>
@@ -2450,10 +2450,10 @@
         <v>0.35</v>
       </c>
       <c r="Q28" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T28">
         <f>F28/D28</f>
@@ -2477,16 +2477,16 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D29">
         <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F29">
         <f>1.5*T11*D29</f>
@@ -2526,10 +2526,10 @@
         <v>0.45</v>
       </c>
       <c r="Q29" t="s">
+        <v>38</v>
+      </c>
+      <c r="R29" t="s">
         <v>41</v>
-      </c>
-      <c r="R29" t="s">
-        <v>44</v>
       </c>
       <c r="T29">
         <f>F29/D29</f>
@@ -2553,16 +2553,16 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D30">
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F30">
         <f>1.5*T12*D30</f>
@@ -2603,10 +2603,10 @@
         <v>0.45</v>
       </c>
       <c r="Q30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T30">
         <f>F30/D30</f>
@@ -2654,19 +2654,19 @@
         <v>9</v>
       </c>
       <c r="K32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L32" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -2674,10 +2674,10 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E33">
         <v>80</v>
@@ -2712,10 +2712,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E34">
         <v>135</v>
@@ -2750,10 +2750,10 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C35" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E35">
         <v>115</v>
@@ -2783,10 +2783,10 @@
         <v>0.35</v>
       </c>
       <c r="N35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P35" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -2821,25 +2821,25 @@
         <v>9</v>
       </c>
       <c r="L37" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M37" t="s">
+        <v>32</v>
+      </c>
+      <c r="N37" t="s">
+        <v>36</v>
+      </c>
+      <c r="O37" t="s">
         <v>35</v>
       </c>
-      <c r="N37" t="s">
+      <c r="P37" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>37</v>
+      </c>
+      <c r="R37" t="s">
         <v>39</v>
-      </c>
-      <c r="O37" t="s">
-        <v>38</v>
-      </c>
-      <c r="P37" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>40</v>
-      </c>
-      <c r="R37" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -2847,7 +2847,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C38" t="s">
         <v>11</v>
@@ -2856,7 +2856,7 @@
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F38">
         <f>2*T20*D38</f>
@@ -2870,8 +2870,8 @@
         <v>30</v>
       </c>
       <c r="I38">
-        <f>3*V20*D38</f>
-        <v>96</v>
+        <f>2.5*V20*D38</f>
+        <v>80</v>
       </c>
       <c r="J38">
         <f>2.5*W20*D38</f>
@@ -2896,10 +2896,10 @@
         <v>0.3</v>
       </c>
       <c r="Q38" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R38" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T38">
         <f>F38/D38</f>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="V38">
         <f>I38/D38</f>
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="W38">
         <f>J38/D38</f>
@@ -2923,7 +2923,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C39" t="s">
         <v>11</v>
@@ -2932,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F39">
         <f>2*T21*D39</f>
@@ -2950,8 +2950,8 @@
         <v>70</v>
       </c>
       <c r="J39">
-        <f>3*W21*D39</f>
-        <v>600</v>
+        <f>2.5*W21*D39</f>
+        <v>400</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2972,10 +2972,10 @@
         <v>0.3</v>
       </c>
       <c r="Q39" t="s">
+        <v>38</v>
+      </c>
+      <c r="R39" t="s">
         <v>41</v>
-      </c>
-      <c r="R39" t="s">
-        <v>44</v>
       </c>
       <c r="T39">
         <f>F39/D39</f>
@@ -2991,7 +2991,7 @@
       </c>
       <c r="W39">
         <f>J39/D39</f>
-        <v>600</v>
+        <v>400</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -2999,7 +2999,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
         <v>11</v>
@@ -3008,7 +3008,7 @@
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F40">
         <f>2*T22*D40</f>
@@ -3049,10 +3049,10 @@
         <v>0.35</v>
       </c>
       <c r="Q40" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R40" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T40">
         <f>F40/D40</f>
@@ -3076,16 +3076,16 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D42">
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F42">
         <f>2*T24*D42</f>
@@ -3099,8 +3099,8 @@
         <v>160</v>
       </c>
       <c r="I42">
-        <f>3.5*V24*D42</f>
-        <v>1680</v>
+        <f>2.5*V24*D42</f>
+        <v>600</v>
       </c>
       <c r="J42">
         <f>2.5*W24*D42</f>
@@ -3125,10 +3125,10 @@
         <v>0.4</v>
       </c>
       <c r="Q42" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R42" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T42">
         <f>F42/D42</f>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="V42">
         <f>I42/D42</f>
-        <v>210</v>
+        <v>75</v>
       </c>
       <c r="W42">
         <f>J42/D42</f>
@@ -3152,16 +3152,16 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D43">
         <v>8</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F43">
         <f>2*T25*D43</f>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="J43">
         <f>3*W25*D43</f>
-        <v>4800</v>
+        <v>3840</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -3201,10 +3201,10 @@
         <v>0.45</v>
       </c>
       <c r="Q43" t="s">
+        <v>38</v>
+      </c>
+      <c r="R43" t="s">
         <v>41</v>
-      </c>
-      <c r="R43" t="s">
-        <v>44</v>
       </c>
       <c r="T43">
         <f>F43/D43</f>
@@ -3220,7 +3220,7 @@
       </c>
       <c r="W43">
         <f>J43/D43</f>
-        <v>600</v>
+        <v>480</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -3228,16 +3228,16 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D44">
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F44">
         <f>2*T26*D44</f>
@@ -3278,10 +3278,10 @@
         <v>0.5</v>
       </c>
       <c r="Q44" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T44">
         <f>F44/D44</f>
@@ -3305,16 +3305,16 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D46">
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F46">
         <f>2.5*T28*D46</f>
@@ -3328,8 +3328,8 @@
         <v>120</v>
       </c>
       <c r="I46">
-        <f>3*V28*D46</f>
-        <v>864</v>
+        <f>2.5*V28*D46</f>
+        <v>720</v>
       </c>
       <c r="J46">
         <f>2.5*W28*D46</f>
@@ -3354,10 +3354,10 @@
         <v>0.4</v>
       </c>
       <c r="Q46" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="T46">
         <f>F46/D46</f>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="V46">
         <f>I46/D46</f>
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="W46">
         <f>J46/D46</f>
@@ -3381,16 +3381,16 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D47">
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="F47">
         <f>2*T29*D47</f>
@@ -3408,8 +3408,8 @@
         <v>680</v>
       </c>
       <c r="J47">
-        <f>3.5*W29*D47</f>
-        <v>8400</v>
+        <f>3*W29*D47</f>
+        <v>7200</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -3430,10 +3430,10 @@
         <v>0.5</v>
       </c>
       <c r="Q47" t="s">
+        <v>38</v>
+      </c>
+      <c r="R47" t="s">
         <v>41</v>
-      </c>
-      <c r="R47" t="s">
-        <v>44</v>
       </c>
       <c r="T47">
         <f>F47/D47</f>
@@ -3449,7 +3449,7 @@
       </c>
       <c r="W47">
         <f>J47/D47</f>
-        <v>1050</v>
+        <v>900</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -3457,16 +3457,16 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D48">
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F48">
         <f>2*T30*D48</f>
@@ -3507,10 +3507,10 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="Q48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R48" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="T48">
         <f>F48/D48</f>
@@ -3558,19 +3558,19 @@
         <v>9</v>
       </c>
       <c r="K50" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L50" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M50" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N50" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="P50" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
@@ -3578,10 +3578,10 @@
         <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C51" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E51">
         <v>350</v>
@@ -3616,10 +3616,10 @@
         <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E52">
         <v>540</v>
@@ -3654,10 +3654,10 @@
         <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E53">
         <v>410</v>
@@ -3687,10 +3687,10 @@
         <v>0.75</v>
       </c>
       <c r="N53" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="P53" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -3725,25 +3725,25 @@
         <v>9</v>
       </c>
       <c r="L55" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M55" t="s">
+        <v>32</v>
+      </c>
+      <c r="N55" t="s">
+        <v>36</v>
+      </c>
+      <c r="O55" t="s">
         <v>35</v>
       </c>
-      <c r="N55" t="s">
+      <c r="P55" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>37</v>
+      </c>
+      <c r="R55" t="s">
         <v>39</v>
-      </c>
-      <c r="O55" t="s">
-        <v>38</v>
-      </c>
-      <c r="P55" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>40</v>
-      </c>
-      <c r="R55" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -3751,16 +3751,16 @@
         <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D56">
         <v>0.75</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F56">
         <f>1*D56*T20</f>
@@ -3799,10 +3799,10 @@
         <v>0.15</v>
       </c>
       <c r="Q56" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R56" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -3810,16 +3810,16 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C57" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D57">
         <v>0.5</v>
       </c>
       <c r="E57" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -3855,10 +3855,10 @@
         <v>0.1</v>
       </c>
       <c r="Q57" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R57" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -3866,13 +3866,13 @@
         <v>0</v>
       </c>
       <c r="B59" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E59" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F59" t="s">
         <v>4</v>
@@ -3893,22 +3893,22 @@
         <v>9</v>
       </c>
       <c r="L59" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M59" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="N59" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O59" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P59" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q59" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C60">
         <v>4</v>
@@ -3963,10 +3963,10 @@
         <v>5</v>
       </c>
       <c r="P60" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q60" t="s">
         <v>41</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3974,7 +3974,7 @@
         <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -4003,7 +4003,7 @@
       </c>
       <c r="J61">
         <f>W47*D61*0.25</f>
-        <v>5250</v>
+        <v>4500</v>
       </c>
       <c r="K61">
         <v>0</v>
@@ -4021,10 +4021,10 @@
         <v>9</v>
       </c>
       <c r="P61" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q61" t="s">
         <v>41</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
@@ -4032,7 +4032,7 @@
         <v>4</v>
       </c>
       <c r="B62" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C62">
         <v>2</v>
@@ -4079,10 +4079,10 @@
         <v>6</v>
       </c>
       <c r="P62" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q62" t="s">
         <v>41</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes to strike craft behavior
1. Fighters now chase enemy strike craft. It looks chaotic but cool.
2. Strike craft had a tendency to get stuck with their target inside their own turning circle, and not be able to get a good angle to shoot it. Started working on a hit-and-run behavior to fix this issue. Still needs work.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\Privateer\TextData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11874C14-6B83-41A5-9A4A-6DEA447390EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E7C91A-C81C-4B8C-A34F-482D6FB0BA8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -982,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3763,8 +3763,8 @@
         <v>45</v>
       </c>
       <c r="F56">
-        <f>1*D56*T20</f>
-        <v>11.25</v>
+        <f>2*D56*T20</f>
+        <v>22.5</v>
       </c>
       <c r="G56">
         <v>175</v>

</xml_diff>

<commit_message>
Started work on correcting the coordinate system of all models
For now, finished much of the code, the Charleston model, small fixed weapon mounts, small barbette weapon mounts, and torpedo tube.
</commit_message>
<xml_diff>
--- a/TextData/Warheads.xlsx
+++ b/TextData/Warheads.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boris\Documents\Privateer\TextData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E7C91A-C81C-4B8C-A34F-482D6FB0BA8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAE6826-F79B-4AB7-9F35-F7CA4B9F5B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Warheads" sheetId="1" r:id="rId1"/>
@@ -983,7 +983,7 @@
   <dimension ref="A1:W62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+      <selection activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3960,7 +3960,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="O60">
-        <v>5</v>
+        <v>0.6</v>
       </c>
       <c r="P60" t="s">
         <v>38</v>
@@ -4018,7 +4018,7 @@
         <v>0.25</v>
       </c>
       <c r="O61">
-        <v>9</v>
+        <v>0.9</v>
       </c>
       <c r="P61" t="s">
         <v>38</v>
@@ -4076,7 +4076,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="O62">
-        <v>6</v>
+        <v>0.7</v>
       </c>
       <c r="P62" t="s">
         <v>38</v>

</xml_diff>